<commit_message>
GBP std curve like murex
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
@@ -667,7 +667,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="ddd\,\ d\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
@@ -681,6 +681,7 @@
     <numFmt numFmtId="174" formatCode="General_)"/>
     <numFmt numFmtId="175" formatCode="#,##0.0;#,##0.0"/>
     <numFmt numFmtId="176" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="179" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -1309,7 +1310,7 @@
     <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1690,6 +1691,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1706,19 +1720,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2061,19 +2064,19 @@
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
-      <c r="E2" s="179"/>
-      <c r="F2" s="180"/>
-      <c r="K2" s="178" t="s">
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="185"/>
+      <c r="K2" s="183" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="181"/>
+      <c r="L2" s="184"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="186"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="43"/>
@@ -2210,12 +2213,12 @@
       </c>
       <c r="E9" s="41"/>
       <c r="F9" s="40"/>
-      <c r="K9" s="178" t="s">
+      <c r="K9" s="183" t="s">
         <v>105</v>
       </c>
-      <c r="L9" s="179"/>
-      <c r="M9" s="179"/>
-      <c r="N9" s="181"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="186"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="43"/>
@@ -2290,7 +2293,7 @@
       </c>
       <c r="D14" s="59" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_GBPYCSTD#0044</v>
+        <v>_GBPYCSTD#0007</v>
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="40"/>
@@ -2419,7 +2422,7 @@
       </c>
       <c r="D23" s="120">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>2.9360550614404159E-2</v>
+        <v>2.9405344144962379E-2</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="40"/>
@@ -2576,7 +2579,7 @@
     <row r="2" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="149" t="str">
         <f>Deposits!J3</f>
-        <v>obj_00337#0031</v>
+        <v>obj_00357#0006</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B2)</f>
@@ -2615,7 +2618,7 @@
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="149" t="str">
         <f>Deposits!J4</f>
-        <v>obj_0033a#0008</v>
+        <v>obj_0035b#0006</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B3)</f>
@@ -2654,7 +2657,7 @@
     <row r="4" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="149" t="str">
         <f>Deposits!J5</f>
-        <v>obj_0064e#0007</v>
+        <v>obj_00348#0006</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B4)</f>
@@ -2686,7 +2689,7 @@
     <row r="5" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="149" t="str">
         <f>Deposits!J6</f>
-        <v>obj_0033c#0005</v>
+        <v>obj_0035f#0006</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B5)</f>
@@ -2718,7 +2721,7 @@
     <row r="6" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="149" t="str">
         <f>Deposits!J7</f>
-        <v>obj_00338#0005</v>
+        <v>obj_00361#0006</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B6)</f>
@@ -2750,7 +2753,7 @@
     <row r="7" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="149" t="str">
         <f>Deposits!J8</f>
-        <v>obj_0033d#0019</v>
+        <v>obj_00355#0006</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B7)</f>
@@ -2782,7 +2785,7 @@
     <row r="8" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="149" t="str">
         <f>Deposits!J9</f>
-        <v>obj_0062a#0017</v>
+        <v>obj_00351#0006</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B8)</f>
@@ -2814,7 +2817,7 @@
     <row r="9" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="149" t="str">
         <f>Deposits!J10</f>
-        <v>obj_0062b#0017</v>
+        <v>obj_00353#0006</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B9)</f>
@@ -2846,7 +2849,7 @@
     <row r="10" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="149" t="str">
         <f>Deposits!J11</f>
-        <v>obj_0064c#0003</v>
+        <v>obj_0035e#0006</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B10)</f>
@@ -2878,7 +2881,7 @@
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="149" t="str">
         <f>Deposits!J12</f>
-        <v>obj_00339#0005</v>
+        <v>obj_0035d#0006</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B11)</f>
@@ -2917,7 +2920,7 @@
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="149" t="str">
         <f>Deposits!J13</f>
-        <v>obj_0062d#0017</v>
+        <v>obj_0034f#0006</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B12)</f>
@@ -2956,7 +2959,7 @@
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="149" t="str">
         <f>Deposits!J14</f>
-        <v>obj_00647#0003</v>
+        <v>obj_00360#0006</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B13)</f>
@@ -2995,7 +2998,7 @@
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="149" t="str">
         <f>Deposits!J15</f>
-        <v>obj_00648#0003</v>
+        <v>obj_00362#0006</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B14)</f>
@@ -3034,7 +3037,7 @@
     <row r="15" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="149" t="str">
         <f>Deposits!J16</f>
-        <v>obj_00649#0003</v>
+        <v>obj_00359#0006</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B15)</f>
@@ -3066,7 +3069,7 @@
     <row r="16" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="149" t="str">
         <f>Deposits!J17</f>
-        <v>obj_0064a#0003</v>
+        <v>obj_0035a#0006</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B16)</f>
@@ -3098,7 +3101,7 @@
     <row r="17" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="149" t="str">
         <f>Deposits!J18</f>
-        <v>obj_0064b#0003</v>
+        <v>obj_0035c#0006</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B17)</f>
@@ -3130,7 +3133,7 @@
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="149" t="str">
         <f>Deposits!J19</f>
-        <v>obj_0062c#0017</v>
+        <v>obj_0034d#0006</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B18)</f>
@@ -3172,7 +3175,7 @@
       </c>
       <c r="B19" s="150" t="str">
         <f>Futures!H3</f>
-        <v>obj_00340#0001</v>
+        <v>obj_00377#0006</v>
       </c>
       <c r="C19" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B19)</f>
@@ -3210,7 +3213,7 @@
       </c>
       <c r="B20" s="149" t="str">
         <f>Futures!H4</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00391#0006</v>
       </c>
       <c r="C20" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B20)</f>
@@ -3248,7 +3251,7 @@
       </c>
       <c r="B21" s="149" t="str">
         <f>Futures!H5</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0036e#0006</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B21)</f>
@@ -3260,7 +3263,7 @@
       </c>
       <c r="E21" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B21,Trigger)</f>
-        <v>0</v>
+        <v>4.7335137414518424E-6</v>
       </c>
       <c r="F21" s="74" t="b">
         <v>0</v>
@@ -3286,7 +3289,7 @@
       </c>
       <c r="B22" s="149" t="str">
         <f>Futures!H6</f>
-        <v>obj_00344#0001</v>
+        <v>obj_003ae#0006</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B22)</f>
@@ -3324,7 +3327,7 @@
       </c>
       <c r="B23" s="149" t="str">
         <f>Futures!H7</f>
-        <v>obj_0035a#0001</v>
+        <v>obj_003ac#0006</v>
       </c>
       <c r="C23" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B23)</f>
@@ -3362,7 +3365,7 @@
       </c>
       <c r="B24" s="149" t="str">
         <f>Futures!H8</f>
-        <v>obj_0034c#0001</v>
+        <v>obj_00389#0006</v>
       </c>
       <c r="C24" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B24)</f>
@@ -3370,11 +3373,11 @@
       </c>
       <c r="D24" s="16">
         <f>_xll.qlRateHelperQuoteValue($B24,Trigger)</f>
-        <v>99.155000000000001</v>
+        <v>99.164999999999992</v>
       </c>
       <c r="E24" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B24,Trigger)</f>
-        <v>0</v>
+        <v>1.3420654014619364E-5</v>
       </c>
       <c r="F24" s="74" t="b">
         <v>0</v>
@@ -3400,7 +3403,7 @@
       </c>
       <c r="B25" s="149" t="str">
         <f>Futures!H9</f>
-        <v>obj_00360#0001</v>
+        <v>obj_00394#0006</v>
       </c>
       <c r="C25" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B25)</f>
@@ -3438,7 +3441,7 @@
       </c>
       <c r="B26" s="149" t="str">
         <f>Futures!H10</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00383#0006</v>
       </c>
       <c r="C26" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B26)</f>
@@ -3476,7 +3479,7 @@
       </c>
       <c r="B27" s="149" t="str">
         <f>Futures!H11</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00393#0006</v>
       </c>
       <c r="C27" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B27)</f>
@@ -3484,11 +3487,11 @@
       </c>
       <c r="D27" s="16">
         <f>_xll.qlRateHelperQuoteValue($B27,Trigger)</f>
-        <v>98.954999999999998</v>
+        <v>98.965000000000003</v>
       </c>
       <c r="E27" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B27,Trigger)</f>
-        <v>0</v>
+        <v>2.5467539818158627E-5</v>
       </c>
       <c r="F27" s="74" t="b">
         <v>1</v>
@@ -3515,7 +3518,7 @@
       </c>
       <c r="B28" s="149" t="str">
         <f>Futures!H12</f>
-        <v>obj_00373#0001</v>
+        <v>obj_0036b#0006</v>
       </c>
       <c r="C28" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B28)</f>
@@ -3554,7 +3557,7 @@
       </c>
       <c r="B29" s="149" t="str">
         <f>Futures!H13</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00376#0006</v>
       </c>
       <c r="C29" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B29)</f>
@@ -3594,7 +3597,7 @@
       </c>
       <c r="B30" s="149" t="str">
         <f>Futures!H14</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_0037f#0006</v>
       </c>
       <c r="C30" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B30)</f>
@@ -3602,11 +3605,11 @@
       </c>
       <c r="D30" s="16">
         <f>_xll.qlRateHelperQuoteValue($B30,Trigger)</f>
-        <v>98.745000000000005</v>
+        <v>98.765000000000001</v>
       </c>
       <c r="E30" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B30,Trigger)</f>
-        <v>0</v>
+        <v>4.0723022000383242E-5</v>
       </c>
       <c r="F30" s="74" t="b">
         <v>1</v>
@@ -3634,7 +3637,7 @@
       </c>
       <c r="B31" s="149" t="str">
         <f>Futures!H15</f>
-        <v>obj_00346#0001</v>
+        <v>obj_00370#0006</v>
       </c>
       <c r="C31" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B31)</f>
@@ -3642,11 +3645,11 @@
       </c>
       <c r="D31" s="16">
         <f>_xll.qlRateHelperQuoteValue($B31,Trigger)</f>
-        <v>98.534999999999997</v>
+        <v>98.545000000000002</v>
       </c>
       <c r="E31" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B31,Trigger)</f>
-        <v>0</v>
+        <v>5.9382011539265042E-5</v>
       </c>
       <c r="F31" s="74" t="b">
         <v>1</v>
@@ -3675,7 +3678,7 @@
       </c>
       <c r="B32" s="149" t="str">
         <f>Futures!H16</f>
-        <v>obj_0035c#0001</v>
+        <v>obj_00368#0006</v>
       </c>
       <c r="C32" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B32)</f>
@@ -3683,11 +3686,11 @@
       </c>
       <c r="D32" s="16">
         <f>_xll.qlRateHelperQuoteValue($B32,Trigger)</f>
-        <v>98.335000000000008</v>
+        <v>98.35499999999999</v>
       </c>
       <c r="E32" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B32,Trigger)</f>
-        <v>0</v>
+        <v>8.1479903905399813E-5</v>
       </c>
       <c r="F32" s="74" t="b">
         <v>1</v>
@@ -3716,7 +3719,7 @@
       </c>
       <c r="B33" s="149" t="str">
         <f>Futures!H17</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_0037a#0006</v>
       </c>
       <c r="C33" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B33)</f>
@@ -3724,11 +3727,11 @@
       </c>
       <c r="D33" s="16">
         <f>_xll.qlRateHelperQuoteValue($B33,Trigger)</f>
-        <v>98.155000000000001</v>
+        <v>98.175000000000011</v>
       </c>
       <c r="E33" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B33,Trigger)</f>
-        <v>0</v>
+        <v>1.065357404825213E-4</v>
       </c>
       <c r="F33" s="74" t="b">
         <v>1</v>
@@ -3757,7 +3760,7 @@
       </c>
       <c r="B34" s="149" t="str">
         <f>Futures!H18</f>
-        <v>obj_0036d#0001</v>
+        <v>obj_0037b#0006</v>
       </c>
       <c r="C34" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B34)</f>
@@ -3765,11 +3768,11 @@
       </c>
       <c r="D34" s="16">
         <f>_xll.qlRateHelperQuoteValue($B34,Trigger)</f>
-        <v>97.974999999999994</v>
+        <v>97.995000000000005</v>
       </c>
       <c r="E34" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B34,Trigger)</f>
-        <v>0</v>
+        <v>1.3665505490881717E-4</v>
       </c>
       <c r="F34" s="74" t="b">
         <v>1</v>
@@ -3798,7 +3801,7 @@
       </c>
       <c r="B35" s="149" t="str">
         <f>Futures!H19</f>
-        <v>obj_00341#0001</v>
+        <v>obj_0039c#0006</v>
       </c>
       <c r="C35" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B35)</f>
@@ -3806,11 +3809,11 @@
       </c>
       <c r="D35" s="16">
         <f>_xll.qlRateHelperQuoteValue($B35,Trigger)</f>
-        <v>97.824999999999989</v>
+        <v>97.844999999999999</v>
       </c>
       <c r="E35" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B35,Trigger)</f>
-        <v>0</v>
+        <v>1.6764426115711069E-4</v>
       </c>
       <c r="F35" s="74" t="b">
         <v>1</v>
@@ -3839,7 +3842,7 @@
       </c>
       <c r="B36" s="149" t="str">
         <f>Futures!H20</f>
-        <v>obj_00362#0001</v>
+        <v>obj_00387#0006</v>
       </c>
       <c r="C36" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B36)</f>
@@ -3847,11 +3850,11 @@
       </c>
       <c r="D36" s="16">
         <f>_xll.qlRateHelperQuoteValue($B36,Trigger)</f>
-        <v>97.715000000000003</v>
+        <v>97.734999999999999</v>
       </c>
       <c r="E36" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B36,Trigger)</f>
-        <v>0</v>
+        <v>1.9986049234161846E-4</v>
       </c>
       <c r="F36" s="74" t="b">
         <v>1</v>
@@ -3880,7 +3883,7 @@
       </c>
       <c r="B37" s="149" t="str">
         <f>Futures!H21</f>
-        <v>obj_0034d#0001</v>
+        <v>obj_00366#0006</v>
       </c>
       <c r="C37" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B37)</f>
@@ -3888,11 +3891,11 @@
       </c>
       <c r="D37" s="16">
         <f>_xll.qlRateHelperQuoteValue($B37,Trigger)</f>
-        <v>97.615000000000009</v>
+        <v>97.634999999999991</v>
       </c>
       <c r="E37" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B37,Trigger)</f>
-        <v>0</v>
+        <v>2.3973068683783518E-4</v>
       </c>
       <c r="F37" s="74" t="b">
         <v>1</v>
@@ -3921,7 +3924,7 @@
       </c>
       <c r="B38" s="149" t="str">
         <f>Futures!H22</f>
-        <v>obj_0034f#0001</v>
+        <v>obj_0037d#0006</v>
       </c>
       <c r="C38" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B38)</f>
@@ -3929,11 +3932,11 @@
       </c>
       <c r="D38" s="16">
         <f>_xll.qlRateHelperQuoteValue($B38,Trigger)</f>
-        <v>97.534999999999997</v>
+        <v>97.555000000000007</v>
       </c>
       <c r="E38" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B38,Trigger)</f>
-        <v>0</v>
+        <v>2.7920539463169351E-4</v>
       </c>
       <c r="F38" s="74" t="b">
         <v>1</v>
@@ -3962,7 +3965,7 @@
       </c>
       <c r="B39" s="149" t="str">
         <f>Futures!H23</f>
-        <v>obj_00376#0001</v>
+        <v>obj_0039e#0006</v>
       </c>
       <c r="C39" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B39)</f>
@@ -3970,11 +3973,11 @@
       </c>
       <c r="D39" s="16">
         <f>_xll.qlRateHelperQuoteValue($B39,Trigger)</f>
-        <v>97.454999999999998</v>
+        <v>97.474999999999994</v>
       </c>
       <c r="E39" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B39,Trigger)</f>
-        <v>0</v>
+        <v>3.2133859529653077E-4</v>
       </c>
       <c r="F39" s="74" t="b">
         <v>1</v>
@@ -4003,7 +4006,7 @@
       </c>
       <c r="B40" s="149" t="str">
         <f>Futures!H24</f>
-        <v>obj_00382#0001</v>
+        <v>obj_0036d#0006</v>
       </c>
       <c r="C40" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B40)</f>
@@ -4011,11 +4014,11 @@
       </c>
       <c r="D40" s="16">
         <f>_xll.qlRateHelperQuoteValue($B40,Trigger)</f>
-        <v>97.4</v>
+        <v>97.414999999999992</v>
       </c>
       <c r="E40" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B40,Trigger)</f>
-        <v>0</v>
+        <v>3.6758587335111937E-4</v>
       </c>
       <c r="F40" s="74" t="b">
         <v>1</v>
@@ -4044,7 +4047,7 @@
       </c>
       <c r="B41" s="149" t="str">
         <f>Futures!H25</f>
-        <v>obj_00355#0001</v>
+        <v>obj_00372#0006</v>
       </c>
       <c r="C41" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B41)</f>
@@ -4052,11 +4055,11 @@
       </c>
       <c r="D41" s="16">
         <f>_xll.qlRateHelperQuoteValue($B41,Trigger)</f>
-        <v>97.35</v>
+        <v>97.365000000000009</v>
       </c>
       <c r="E41" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B41,Trigger)</f>
-        <v>0</v>
+        <v>4.1546506466755192E-4</v>
       </c>
       <c r="F41" s="74" t="b">
         <v>1</v>
@@ -4085,7 +4088,7 @@
       </c>
       <c r="B42" s="149" t="str">
         <f>Futures!H26</f>
-        <v>obj_00348#0001</v>
+        <v>obj_00390#0006</v>
       </c>
       <c r="C42" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B42)</f>
@@ -4093,11 +4096,11 @@
       </c>
       <c r="D42" s="16">
         <f>_xll.qlRateHelperQuoteValue($B42,Trigger)</f>
-        <v>97.31</v>
+        <v>97.324999999999989</v>
       </c>
       <c r="E42" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B42,Trigger)</f>
-        <v>0</v>
+        <v>4.6528663456285401E-4</v>
       </c>
       <c r="F42" s="74" t="b">
         <v>1</v>
@@ -4126,7 +4129,7 @@
       </c>
       <c r="B43" s="149" t="str">
         <f>Futures!H27</f>
-        <v>obj_00369#0001</v>
+        <v>obj_003a3#0006</v>
       </c>
       <c r="C43" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B43)</f>
@@ -4134,11 +4137,11 @@
       </c>
       <c r="D43" s="16">
         <f>_xll.qlRateHelperQuoteValue($B43,Trigger)</f>
-        <v>97.254999999999995</v>
+        <v>97.275000000000006</v>
       </c>
       <c r="E43" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B43,Trigger)</f>
-        <v>0</v>
+        <v>5.1752454253955809E-4</v>
       </c>
       <c r="F43" s="74" t="b">
         <v>1</v>
@@ -4167,7 +4170,7 @@
       </c>
       <c r="B44" s="149" t="str">
         <f>Futures!H28</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_0036c#0006</v>
       </c>
       <c r="C44" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B44)</f>
@@ -4175,11 +4178,11 @@
       </c>
       <c r="D44" s="16">
         <f>_xll.qlRateHelperQuoteValue($B44,Trigger)</f>
-        <v>97.210000000000008</v>
+        <v>97.234999999999999</v>
       </c>
       <c r="E44" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B44,Trigger)</f>
-        <v>0</v>
+        <v>5.7403347067243305E-4</v>
       </c>
       <c r="F44" s="74" t="b">
         <v>1</v>
@@ -4208,7 +4211,7 @@
       </c>
       <c r="B45" s="149" t="str">
         <f>Futures!H29</f>
-        <v>obj_00350#0001</v>
+        <v>obj_00380#0006</v>
       </c>
       <c r="C45" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B45)</f>
@@ -4216,11 +4219,11 @@
       </c>
       <c r="D45" s="16">
         <f>_xll.qlRateHelperQuoteValue($B45,Trigger)</f>
-        <v>97.14</v>
+        <v>97.210000000000008</v>
       </c>
       <c r="E45" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B45,Trigger)</f>
-        <v>0</v>
+        <v>6.3164452373354351E-4</v>
       </c>
       <c r="F45" s="74" t="b">
         <v>1</v>
@@ -4249,7 +4252,7 @@
       </c>
       <c r="B46" s="149" t="str">
         <f>Futures!H30</f>
-        <v>obj_00387#0001</v>
+        <v>obj_003aa#0006</v>
       </c>
       <c r="C46" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B46)</f>
@@ -4257,11 +4260,11 @@
       </c>
       <c r="D46" s="16">
         <f>_xll.qlRateHelperQuoteValue($B46,Trigger)</f>
-        <v>97.1</v>
+        <v>97.17</v>
       </c>
       <c r="E46" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B46,Trigger)</f>
-        <v>0</v>
+        <v>6.9086013546234236E-4</v>
       </c>
       <c r="F46" s="74" t="b">
         <v>1</v>
@@ -4290,7 +4293,7 @@
       </c>
       <c r="B47" s="149" t="str">
         <f>Futures!H31</f>
-        <v>obj_0036b#0001</v>
+        <v>obj_0039a#0006</v>
       </c>
       <c r="C47" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B47)</f>
@@ -4298,11 +4301,11 @@
       </c>
       <c r="D47" s="16">
         <f>_xll.qlRateHelperQuoteValue($B47,Trigger)</f>
-        <v>97.074999999999989</v>
+        <v>97.134999999999991</v>
       </c>
       <c r="E47" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B47,Trigger)</f>
-        <v>0</v>
+        <v>7.5298225712401427E-4</v>
       </c>
       <c r="F47" s="74" t="b">
         <v>1</v>
@@ -4328,7 +4331,7 @@
       </c>
       <c r="B48" s="149" t="str">
         <f>Futures!H32</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_0038c#0006</v>
       </c>
       <c r="C48" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B48)</f>
@@ -4336,11 +4339,11 @@
       </c>
       <c r="D48" s="16">
         <f>_xll.qlRateHelperQuoteValue($B48,Trigger)</f>
-        <v>97.044999999999987</v>
+        <v>97.10499999999999</v>
       </c>
       <c r="E48" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B48,Trigger)</f>
-        <v>0</v>
+        <v>8.1804915904803868E-4</v>
       </c>
       <c r="F48" s="74" t="b">
         <v>1</v>
@@ -4366,7 +4369,7 @@
       </c>
       <c r="B49" s="149" t="str">
         <f>Futures!H33</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0038a#0006</v>
       </c>
       <c r="C49" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B49)</f>
@@ -4404,7 +4407,7 @@
       </c>
       <c r="B50" s="149" t="str">
         <f>Futures!H34</f>
-        <v>obj_0034e#0001</v>
+        <v>obj_00371#0006</v>
       </c>
       <c r="C50" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B50)</f>
@@ -4442,7 +4445,7 @@
       </c>
       <c r="B51" s="149" t="str">
         <f>Futures!H35</f>
-        <v>obj_00368#0001</v>
+        <v>obj_003a8#0006</v>
       </c>
       <c r="C51" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B51)</f>
@@ -4480,7 +4483,7 @@
       </c>
       <c r="B52" s="149" t="str">
         <f>Futures!H36</f>
-        <v>obj_0034a#0001</v>
+        <v>obj_003a2#0006</v>
       </c>
       <c r="C52" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B52)</f>
@@ -4518,7 +4521,7 @@
       </c>
       <c r="B53" s="149" t="str">
         <f>Futures!H37</f>
-        <v>obj_00384#0001</v>
+        <v>obj_0037c#0006</v>
       </c>
       <c r="C53" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B53)</f>
@@ -4556,7 +4559,7 @@
       </c>
       <c r="B54" s="149" t="str">
         <f>Futures!H38</f>
-        <v>obj_00377#0001</v>
+        <v>obj_003a1#0006</v>
       </c>
       <c r="C54" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B54)</f>
@@ -4594,7 +4597,7 @@
       </c>
       <c r="B55" s="149" t="str">
         <f>Futures!H39</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_0038e#0006</v>
       </c>
       <c r="C55" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B55)</f>
@@ -4632,7 +4635,7 @@
       </c>
       <c r="B56" s="149" t="str">
         <f>Futures!H40</f>
-        <v>obj_00361#0001</v>
+        <v>obj_00397#0006</v>
       </c>
       <c r="C56" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B56)</f>
@@ -4670,7 +4673,7 @@
       </c>
       <c r="B57" s="149" t="str">
         <f>Futures!H41</f>
-        <v>obj_0033e#0001</v>
+        <v>obj_00364#0006</v>
       </c>
       <c r="C57" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B57)</f>
@@ -4708,7 +4711,7 @@
       </c>
       <c r="B58" s="149" t="str">
         <f>Futures!H42</f>
-        <v>obj_00347#0001</v>
+        <v>obj_00378#0006</v>
       </c>
       <c r="C58" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B58)</f>
@@ -4746,7 +4749,7 @@
       </c>
       <c r="B59" s="149" t="str">
         <f>Futures!H43</f>
-        <v>obj_00366#0001</v>
+        <v>obj_0038d#0006</v>
       </c>
       <c r="C59" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B59)</f>
@@ -4784,7 +4787,7 @@
       </c>
       <c r="B60" s="149" t="str">
         <f>Futures!H44</f>
-        <v>obj_00378#0001</v>
+        <v>obj_00398#0006</v>
       </c>
       <c r="C60" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B60)</f>
@@ -4822,7 +4825,7 @@
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" s="150" t="str">
         <f>Swaps!K6</f>
-        <v>obj_00343#0001</v>
+        <v>obj_003ab#0006</v>
       </c>
       <c r="C61" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B61)</f>
@@ -4857,7 +4860,7 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="149" t="str">
         <f>Swaps!K7</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_003af#0006</v>
       </c>
       <c r="C62" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B62)</f>
@@ -4892,7 +4895,7 @@
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="149" t="str">
         <f>Swaps!K8</f>
-        <v>obj_00351#0001</v>
+        <v>obj_00384#0006</v>
       </c>
       <c r="C63" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B63)</f>
@@ -4900,7 +4903,7 @@
       </c>
       <c r="D63" s="6">
         <f>_xll.qlRateHelperQuoteValue($B63,Trigger)</f>
-        <v>1.0829999999999999E-2</v>
+        <v>1.073E-2</v>
       </c>
       <c r="E63" s="6">
         <f>_xll.qlSwapRateHelperSpread($B63,Trigger)</f>
@@ -4927,7 +4930,7 @@
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" s="149" t="str">
         <f>Swaps!K9</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_00382#0006</v>
       </c>
       <c r="C64" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B64)</f>
@@ -4962,7 +4965,7 @@
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="149" t="str">
         <f>Swaps!K10</f>
-        <v>obj_00364#0001</v>
+        <v>obj_00369#0006</v>
       </c>
       <c r="C65" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B65)</f>
@@ -4970,7 +4973,7 @@
       </c>
       <c r="D65" s="6">
         <f>_xll.qlRateHelperQuoteValue($B65,Trigger)</f>
-        <v>1.274E-2</v>
+        <v>1.2619999999999999E-2</v>
       </c>
       <c r="E65" s="6">
         <f>_xll.qlSwapRateHelperSpread($B65,Trigger)</f>
@@ -4997,7 +5000,7 @@
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="149" t="str">
         <f>Swaps!K11</f>
-        <v>obj_0033f#0001</v>
+        <v>obj_0036f#0006</v>
       </c>
       <c r="C66" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B66)</f>
@@ -5005,7 +5008,7 @@
       </c>
       <c r="D66" s="6">
         <f>_xll.qlRateHelperQuoteValue($B66,Trigger)</f>
-        <v>1.6150000000000001E-2</v>
+        <v>1.5990000000000001E-2</v>
       </c>
       <c r="E66" s="6">
         <f>_xll.qlSwapRateHelperSpread($B66,Trigger)</f>
@@ -5032,7 +5035,7 @@
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="149" t="str">
         <f>Swaps!K12</f>
-        <v>obj_00357#0001</v>
+        <v>obj_0039d#0006</v>
       </c>
       <c r="C67" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B67)</f>
@@ -5040,7 +5043,7 @@
       </c>
       <c r="D67" s="6">
         <f>_xll.qlRateHelperQuoteValue($B67,Trigger)</f>
-        <v>1.8589999999999999E-2</v>
+        <v>1.8429999999999998E-2</v>
       </c>
       <c r="E67" s="6">
         <f>_xll.qlSwapRateHelperSpread($B67,Trigger)</f>
@@ -5067,7 +5070,7 @@
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="149" t="str">
         <f>Swaps!K13</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_003a4#0006</v>
       </c>
       <c r="C68" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B68)</f>
@@ -5075,7 +5078,7 @@
       </c>
       <c r="D68" s="6">
         <f>_xll.qlRateHelperQuoteValue($B68,Trigger)</f>
-        <v>2.0380000000000002E-2</v>
+        <v>2.0209999999999999E-2</v>
       </c>
       <c r="E68" s="6">
         <f>_xll.qlSwapRateHelperSpread($B68,Trigger)</f>
@@ -5102,7 +5105,7 @@
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="149" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00349#0001</v>
+        <v>obj_003a0#0006</v>
       </c>
       <c r="C69" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B69)</f>
@@ -5110,7 +5113,7 @@
       </c>
       <c r="D69" s="6">
         <f>_xll.qlRateHelperQuoteValue($B69,Trigger)</f>
-        <v>2.1749999999999999E-2</v>
+        <v>2.1610000000000001E-2</v>
       </c>
       <c r="E69" s="6">
         <f>_xll.qlSwapRateHelperSpread($B69,Trigger)</f>
@@ -5137,7 +5140,7 @@
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="149" t="str">
         <f>Swaps!K15</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_00399#0006</v>
       </c>
       <c r="C70" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B70)</f>
@@ -5145,7 +5148,7 @@
       </c>
       <c r="D70" s="6">
         <f>_xll.qlRateHelperQuoteValue($B70,Trigger)</f>
-        <v>2.2860000000000002E-2</v>
+        <v>2.2749999999999999E-2</v>
       </c>
       <c r="E70" s="6">
         <f>_xll.qlSwapRateHelperSpread($B70,Trigger)</f>
@@ -5173,7 +5176,7 @@
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="149" t="str">
         <f>Swaps!K16</f>
-        <v>obj_00359#0001</v>
+        <v>obj_003a9#0006</v>
       </c>
       <c r="C71" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B71)</f>
@@ -5181,7 +5184,7 @@
       </c>
       <c r="D71" s="6">
         <f>_xll.qlRateHelperQuoteValue($B71,Trigger)</f>
-        <v>2.3799999999999998E-2</v>
+        <v>2.3700000000000002E-2</v>
       </c>
       <c r="E71" s="6">
         <f>_xll.qlSwapRateHelperSpread($B71,Trigger)</f>
@@ -5209,7 +5212,7 @@
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="149" t="str">
         <f>Swaps!K17</f>
-        <v>obj_00380#0001</v>
+        <v>obj_003ad#0006</v>
       </c>
       <c r="C72" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B72)</f>
@@ -5217,7 +5220,7 @@
       </c>
       <c r="D72" s="6">
         <f>_xll.qlRateHelperQuoteValue($B72,Trigger)</f>
-        <v>2.4590000000000001E-2</v>
+        <v>2.4510000000000001E-2</v>
       </c>
       <c r="E72" s="6">
         <f>_xll.qlSwapRateHelperSpread($B72,Trigger)</f>
@@ -5245,7 +5248,7 @@
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="149" t="str">
         <f>Swaps!K18</f>
-        <v>obj_00385#0001</v>
+        <v>obj_0039f#0006</v>
       </c>
       <c r="C73" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B73)</f>
@@ -5253,7 +5256,7 @@
       </c>
       <c r="D73" s="6">
         <f>_xll.qlRateHelperQuoteValue($B73,Trigger)</f>
-        <v>2.5270000000000001E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="E73" s="6">
         <f>_xll.qlSwapRateHelperSpread($B73,Trigger)</f>
@@ -5281,7 +5284,7 @@
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B74" s="149" t="str">
         <f>Swaps!K19</f>
-        <v>obj_00356#0001</v>
+        <v>obj_00379#0006</v>
       </c>
       <c r="C74" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B74)</f>
@@ -5289,7 +5292,7 @@
       </c>
       <c r="D74" s="6">
         <f>_xll.qlRateHelperQuoteValue($B74,Trigger)</f>
-        <v>2.588E-2</v>
+        <v>2.5819999999999999E-2</v>
       </c>
       <c r="E74" s="6">
         <f>_xll.qlSwapRateHelperSpread($B74,Trigger)</f>
@@ -5317,7 +5320,7 @@
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B75" s="149" t="str">
         <f>Swaps!K20</f>
-        <v>obj_00375#0001</v>
+        <v>obj_0039b#0006</v>
       </c>
       <c r="C75" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B75)</f>
@@ -5325,7 +5328,7 @@
       </c>
       <c r="D75" s="6">
         <f>_xll.qlRateHelperQuoteValue($B75,Trigger)</f>
-        <v>2.6420000000000003E-2</v>
+        <v>2.6360000000000001E-2</v>
       </c>
       <c r="E75" s="6">
         <f>_xll.qlSwapRateHelperSpread($B75,Trigger)</f>
@@ -5353,7 +5356,7 @@
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B76" s="149" t="str">
         <f>Swaps!K21</f>
-        <v>obj_00388#0001</v>
+        <v>obj_003b2#0006</v>
       </c>
       <c r="C76" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B76)</f>
@@ -5389,7 +5392,7 @@
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B77" s="149" t="str">
         <f>Swaps!K22</f>
-        <v>obj_00365#0001</v>
+        <v>obj_00374#0006</v>
       </c>
       <c r="C77" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B77)</f>
@@ -5425,7 +5428,7 @@
     <row r="78" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B78" s="149" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00374#0001</v>
+        <v>obj_00375#0006</v>
       </c>
       <c r="C78" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B78)</f>
@@ -5433,7 +5436,7 @@
       </c>
       <c r="D78" s="6">
         <f>_xll.qlRateHelperQuoteValue($B78,Trigger)</f>
-        <v>2.759E-2</v>
+        <v>2.7549999999999998E-2</v>
       </c>
       <c r="E78" s="6">
         <f>_xll.qlSwapRateHelperSpread($B78,Trigger)</f>
@@ -5461,7 +5464,7 @@
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="149" t="str">
         <f>Swaps!K24</f>
-        <v>obj_00358#0001</v>
+        <v>obj_00381#0006</v>
       </c>
       <c r="C79" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B79)</f>
@@ -5497,7 +5500,7 @@
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B80" s="149" t="str">
         <f>Swaps!K25</f>
-        <v>obj_00342#0001</v>
+        <v>obj_00396#0006</v>
       </c>
       <c r="C80" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B80)</f>
@@ -5533,7 +5536,7 @@
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B81" s="149" t="str">
         <f>Swaps!K26</f>
-        <v>obj_00354#0001</v>
+        <v>obj_00367#0006</v>
       </c>
       <c r="C81" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B81)</f>
@@ -5569,7 +5572,7 @@
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="149" t="str">
         <f>Swaps!K27</f>
-        <v>obj_00379#0001</v>
+        <v>obj_00388#0006</v>
       </c>
       <c r="C82" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B82)</f>
@@ -5605,7 +5608,7 @@
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="149" t="str">
         <f>Swaps!K28</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_0038f#0006</v>
       </c>
       <c r="C83" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B83)</f>
@@ -5613,7 +5616,7 @@
       </c>
       <c r="D83" s="6">
         <f>_xll.qlRateHelperQuoteValue($B83,Trigger)</f>
-        <v>2.8580000000000001E-2</v>
+        <v>2.8570000000000002E-2</v>
       </c>
       <c r="E83" s="6">
         <f>_xll.qlSwapRateHelperSpread($B83,Trigger)</f>
@@ -5641,7 +5644,7 @@
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="149" t="str">
         <f>Swaps!K29</f>
-        <v>obj_00345#0001</v>
+        <v>obj_00365#0006</v>
       </c>
       <c r="C84" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B84)</f>
@@ -5677,7 +5680,7 @@
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="149" t="str">
         <f>Swaps!K30</f>
-        <v>obj_00381#0001</v>
+        <v>obj_003a7#0006</v>
       </c>
       <c r="C85" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B85)</f>
@@ -5713,7 +5716,7 @@
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="149" t="str">
         <f>Swaps!K31</f>
-        <v>obj_00370#0001</v>
+        <v>obj_00385#0006</v>
       </c>
       <c r="C86" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B86)</f>
@@ -5749,7 +5752,7 @@
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B87" s="149" t="str">
         <f>Swaps!K32</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_0038b#0006</v>
       </c>
       <c r="C87" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B87)</f>
@@ -5785,7 +5788,7 @@
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="149" t="str">
         <f>Swaps!K33</f>
-        <v>obj_0034b#0001</v>
+        <v>obj_003a5#0006</v>
       </c>
       <c r="C88" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B88)</f>
@@ -5793,7 +5796,7 @@
       </c>
       <c r="D88" s="6">
         <f>_xll.qlRateHelperQuoteValue($B88,Trigger)</f>
-        <v>2.8810000000000002E-2</v>
+        <v>2.8830000000000001E-2</v>
       </c>
       <c r="E88" s="6">
         <f>_xll.qlSwapRateHelperSpread($B88,Trigger)</f>
@@ -5821,7 +5824,7 @@
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="149" t="str">
         <f>Swaps!K34</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_0036a#0006</v>
       </c>
       <c r="C89" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B89)</f>
@@ -5857,7 +5860,7 @@
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="149" t="str">
         <f>Swaps!K35</f>
-        <v>obj_00367#0001</v>
+        <v>obj_0037e#0006</v>
       </c>
       <c r="C90" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B90)</f>
@@ -5893,7 +5896,7 @@
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="149" t="str">
         <f>Swaps!K36</f>
-        <v>obj_00353#0001</v>
+        <v>obj_003b1#0006</v>
       </c>
       <c r="C91" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B91)</f>
@@ -5929,7 +5932,7 @@
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="149" t="str">
         <f>Swaps!K37</f>
-        <v>obj_0036e#0001</v>
+        <v>obj_00392#0006</v>
       </c>
       <c r="C92" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B92)</f>
@@ -5965,7 +5968,7 @@
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="149" t="str">
         <f>Swaps!K38</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_00395#0006</v>
       </c>
       <c r="C93" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B93)</f>
@@ -5973,7 +5976,7 @@
       </c>
       <c r="D93" s="6">
         <f>_xll.qlRateHelperQuoteValue($B93,Trigger)</f>
-        <v>2.8849999999999997E-2</v>
+        <v>2.8890000000000002E-2</v>
       </c>
       <c r="E93" s="6">
         <f>_xll.qlSwapRateHelperSpread($B93,Trigger)</f>
@@ -6001,7 +6004,7 @@
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="149" t="str">
         <f>Swaps!K39</f>
-        <v>obj_00372#0001</v>
+        <v>obj_003b0#0006</v>
       </c>
       <c r="C94" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B94)</f>
@@ -6037,7 +6040,7 @@
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="149" t="str">
         <f>Swaps!K40</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_00373#0006</v>
       </c>
       <c r="C95" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B95)</f>
@@ -6045,7 +6048,7 @@
       </c>
       <c r="D95" s="6">
         <f>_xll.qlRateHelperQuoteValue($B95,Trigger)</f>
-        <v>2.8670000000000001E-2</v>
+        <v>2.8730000000000002E-2</v>
       </c>
       <c r="E95" s="6">
         <f>_xll.qlSwapRateHelperSpread($B95,Trigger)</f>
@@ -6073,7 +6076,7 @@
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="149" t="str">
         <f>Swaps!K41</f>
-        <v>obj_00352#0001</v>
+        <v>obj_00386#0006</v>
       </c>
       <c r="C96" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B96)</f>
@@ -6081,7 +6084,7 @@
       </c>
       <c r="D96" s="6">
         <f>_xll.qlRateHelperQuoteValue($B96,Trigger)</f>
-        <v>2.8660000000000001E-2</v>
+        <v>2.8730000000000002E-2</v>
       </c>
       <c r="E96" s="6">
         <f>_xll.qlSwapRateHelperSpread($B96,Trigger)</f>
@@ -6109,7 +6112,7 @@
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B97" s="151" t="str">
         <f>Swaps!K42</f>
-        <v>obj_00371#0001</v>
+        <v>obj_003a6#0006</v>
       </c>
       <c r="C97" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B97)</f>
@@ -6117,7 +6120,7 @@
       </c>
       <c r="D97" s="6">
         <f>_xll.qlRateHelperQuoteValue($B97,Trigger)</f>
-        <v>2.879E-2</v>
+        <v>2.886E-2</v>
       </c>
       <c r="E97" s="6">
         <f>_xll.qlSwapRateHelperSpread($B97,Trigger)</f>
@@ -6164,10 +6167,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6181,14 +6184,16 @@
     <col min="8" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="182" t="s">
+    <row r="1" spans="1:16" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="187" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="183"/>
+      <c r="B1" s="188"/>
       <c r="D1" s="145" t="s">
         <v>59</v>
       </c>
@@ -6210,7 +6215,7 @@
         <v>4.7687688475639796E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>57</v>
       </c>
@@ -6219,7 +6224,7 @@
       </c>
       <c r="D2" s="25" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00337</v>
+        <v>obj_00357</v>
       </c>
       <c r="E2" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -6244,8 +6249,12 @@
       <c r="J2" s="24">
         <v>4.7687688475639796E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="190"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>56</v>
       </c>
@@ -6253,7 +6262,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="25" t="str">
-        <v>obj_0033a</v>
+        <v>obj_0035b</v>
       </c>
       <c r="E3" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -6278,8 +6287,12 @@
       <c r="J3" s="24">
         <v>4.8024707911612213E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="190"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>55</v>
       </c>
@@ -6287,7 +6300,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="25" t="str">
-        <v>obj_0064e</v>
+        <v>obj_00348</v>
       </c>
       <c r="E4" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -6312,8 +6325,12 @@
       <c r="J4" s="24">
         <v>4.8135778099353743E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="190"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>54</v>
       </c>
@@ -6321,7 +6338,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="25" t="str">
-        <v>obj_0033c</v>
+        <v>obj_0035f</v>
       </c>
       <c r="E5" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -6346,8 +6363,12 @@
       <c r="J5" s="24">
         <v>4.891132470681246E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="190"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>52</v>
       </c>
@@ -6356,7 +6377,7 @@
         <v/>
       </c>
       <c r="D6" s="25" t="str">
-        <v>obj_0033d</v>
+        <v>obj_00355</v>
       </c>
       <c r="E6" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -6381,18 +6402,22 @@
       <c r="J6" s="24">
         <v>5.0682738102130658E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="190"/>
+    </row>
+    <row r="7" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>GBP_YCSTDRH_RateHelpersSelected#0044</v>
+        <v>GBP_YCSTDRH_RateHelpersSelected#0007</v>
       </c>
       <c r="B7" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
       <c r="D7" s="25" t="str">
-        <v>obj_0062a</v>
+        <v>obj_00351</v>
       </c>
       <c r="E7" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -6417,10 +6442,14 @@
       <c r="J7" s="24">
         <v>5.3251297388142733E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="190"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="25" t="str">
-        <v>obj_0062b</v>
+        <v>obj_00353</v>
       </c>
       <c r="E8" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -6445,10 +6474,14 @@
       <c r="J8" s="24">
         <v>5.6371625352661147E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="190"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9" s="25" t="str">
-        <v>obj_0064c</v>
+        <v>obj_0035e</v>
       </c>
       <c r="E9" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -6473,10 +6506,14 @@
       <c r="J9" s="24">
         <v>6.1446284121358715E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="190"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D10" s="25" t="str">
-        <v>obj_00339</v>
+        <v>obj_0035d</v>
       </c>
       <c r="E10" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -6501,10 +6538,14 @@
       <c r="J10" s="24">
         <v>6.6186157202768733E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="190"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D11" s="25" t="str">
-        <v>obj_0062d</v>
+        <v>obj_0034f</v>
       </c>
       <c r="E11" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -6529,10 +6570,14 @@
       <c r="J11" s="24">
         <v>7.1248984287600424E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="190"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" s="25" t="str">
-        <v>obj_00647</v>
+        <v>obj_00360</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -6557,10 +6602,14 @@
       <c r="J12" s="24">
         <v>7.6983789349629253E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="190"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" s="25" t="str">
-        <v>obj_00648</v>
+        <v>obj_00362</v>
       </c>
       <c r="E13" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -6585,10 +6634,14 @@
       <c r="J13" s="24">
         <v>8.2712422773627142E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="190"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D14" s="25" t="str">
-        <v>obj_00649</v>
+        <v>obj_00359</v>
       </c>
       <c r="E14" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D14)</f>
@@ -6613,10 +6666,14 @@
       <c r="J14" s="24">
         <v>8.8621758969245987E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="190"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D15" s="25" t="str">
-        <v>obj_0038c</v>
+        <v>obj_00393</v>
       </c>
       <c r="E15" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D15)</f>
@@ -6624,11 +6681,11 @@
       </c>
       <c r="F15" s="24">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.045000000000007E-2</v>
+        <v>1.0324532460181812E-2</v>
       </c>
       <c r="G15" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
-        <v>0</v>
+        <v>2.5467539818158627E-5</v>
       </c>
       <c r="H15" s="23">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
@@ -6639,12 +6696,16 @@
         <v>42264</v>
       </c>
       <c r="J15" s="24">
-        <v>9.1508497813930743E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9.1186008426915217E-3</v>
+      </c>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="190"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D16" s="25" t="str">
-        <v>obj_0037d</v>
+        <v>obj_0037f</v>
       </c>
       <c r="E16" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D16)</f>
@@ -6652,11 +6713,11 @@
       </c>
       <c r="F16" s="24">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.254999999999995E-2</v>
+        <v>1.2309276977999589E-2</v>
       </c>
       <c r="G16" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
-        <v>0</v>
+        <v>4.0723022000383242E-5</v>
       </c>
       <c r="H16" s="23">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
@@ -6667,12 +6728,16 @@
         <v>42354</v>
       </c>
       <c r="J16" s="24">
-        <v>9.836121097255188E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+        <v>9.7618882806031204E-3</v>
+      </c>
+      <c r="M16" s="189"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="190"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="25" t="str">
-        <v>obj_00346</v>
+        <v>obj_00370</v>
       </c>
       <c r="E17" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D17)</f>
@@ -6680,11 +6745,11 @@
       </c>
       <c r="F17" s="24">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.4650000000000052E-2</v>
+        <v>1.4490617988460687E-2</v>
       </c>
       <c r="G17" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
-        <v>0</v>
+        <v>5.9382011539265042E-5</v>
       </c>
       <c r="H17" s="23">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
@@ -6695,12 +6760,16 @@
         <v>42445</v>
       </c>
       <c r="J17" s="24">
-        <v>1.0645850186103362E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.0557312386336169E-2</v>
+      </c>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="190"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="25" t="str">
-        <v>obj_0035c</v>
+        <v>obj_00368</v>
       </c>
       <c r="E18" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D18)</f>
@@ -6708,11 +6777,11 @@
       </c>
       <c r="F18" s="24">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.6649999999999943E-2</v>
+        <v>1.6368520096094675E-2</v>
       </c>
       <c r="G18" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
-        <v>0</v>
+        <v>8.1479903905399813E-5</v>
       </c>
       <c r="H18" s="23">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
@@ -6723,12 +6792,16 @@
         <v>42537</v>
       </c>
       <c r="J18" s="24">
-        <v>1.1517558893348061E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.1401015760112768E-2</v>
+      </c>
+      <c r="M18" s="189"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="190"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D19" s="25" t="str">
-        <v>obj_0035e</v>
+        <v>obj_0037a</v>
       </c>
       <c r="E19" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D19)</f>
@@ -6736,11 +6809,11 @@
       </c>
       <c r="F19" s="24">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.8449999999999966E-2</v>
+        <v>1.8143464259517357E-2</v>
       </c>
       <c r="G19" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
-        <v>0</v>
+        <v>1.065357404825213E-4</v>
       </c>
       <c r="H19" s="23">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
@@ -6751,12 +6824,16 @@
         <v>42628</v>
       </c>
       <c r="J19" s="24">
-        <v>1.2388419000357399E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.2248077826110296E-2</v>
+      </c>
+      <c r="M19" s="189"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="190"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D20" s="25" t="str">
-        <v>obj_0036d</v>
+        <v>obj_0037b</v>
       </c>
       <c r="E20" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D20)</f>
@@ -6764,11 +6841,11 @@
       </c>
       <c r="F20" s="24">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>2.0250000000000101E-2</v>
+        <v>1.9913344945091085E-2</v>
       </c>
       <c r="G20" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
-        <v>0</v>
+        <v>1.3665505490881717E-4</v>
       </c>
       <c r="H20" s="23">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
@@ -6779,12 +6856,16 @@
         <v>42725</v>
       </c>
       <c r="J20" s="24">
-        <v>1.3307874821787255E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.314462131061391E-2</v>
+      </c>
+      <c r="M20" s="189"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="190"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D21" s="25" t="str">
-        <v>obj_0033f</v>
+        <v>obj_0036f</v>
       </c>
       <c r="E21" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D21)</f>
@@ -6792,7 +6873,7 @@
       </c>
       <c r="F21" s="24">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.6150000000000001E-2</v>
+        <v>1.5990000000000001E-2</v>
       </c>
       <c r="G21" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -6807,12 +6888,16 @@
         <v>43003</v>
       </c>
       <c r="J21" s="24">
-        <v>1.617043087833402E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.6009953980344015E-2</v>
+      </c>
+      <c r="M21" s="189"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="190"/>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D22" s="25" t="str">
-        <v>obj_00357</v>
+        <v>obj_0039d</v>
       </c>
       <c r="E22" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D22)</f>
@@ -6820,7 +6905,7 @@
       </c>
       <c r="F22" s="24">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.8589999999999999E-2</v>
+        <v>1.8429999999999998E-2</v>
       </c>
       <c r="G22" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -6835,12 +6920,16 @@
         <v>43368</v>
       </c>
       <c r="J22" s="24">
-        <v>1.8648679222659791E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+        <v>1.8488106616672269E-2</v>
+      </c>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="190"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D23" s="25" t="str">
-        <v>obj_0037f</v>
+        <v>obj_003a4</v>
       </c>
       <c r="E23" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D23)</f>
@@ -6848,7 +6937,7 @@
       </c>
       <c r="F23" s="24">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>2.0380000000000002E-2</v>
+        <v>2.0209999999999999E-2</v>
       </c>
       <c r="G23" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -6863,12 +6952,16 @@
         <v>43733</v>
       </c>
       <c r="J23" s="24">
-        <v>2.0479958221461994E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.0308834008443223E-2</v>
+      </c>
+      <c r="M23" s="189"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="190"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D24" s="25" t="str">
-        <v>obj_00349</v>
+        <v>obj_003a0</v>
       </c>
       <c r="E24" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D24)</f>
@@ -6876,7 +6969,7 @@
       </c>
       <c r="F24" s="24">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>2.1749999999999999E-2</v>
+        <v>2.1610000000000001E-2</v>
       </c>
       <c r="G24" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -6891,12 +6984,16 @@
         <v>44099</v>
       </c>
       <c r="J24" s="24">
-        <v>2.1891640652376136E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.1752155175066092E-2</v>
+      </c>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="190"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D25" s="25" t="str">
-        <v>obj_0036a</v>
+        <v>obj_00399</v>
       </c>
       <c r="E25" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D25)</f>
@@ -6904,7 +7001,7 @@
       </c>
       <c r="F25" s="24">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.2860000000000002E-2</v>
+        <v>2.2749999999999999E-2</v>
       </c>
       <c r="G25" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -6919,12 +7016,16 @@
         <v>44466</v>
       </c>
       <c r="J25" s="24">
-        <v>2.3044606550897719E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.2937128972814427E-2</v>
+      </c>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="190"/>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D26" s="25" t="str">
-        <v>obj_00359</v>
+        <v>obj_003a9</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D26)</f>
@@ -6932,7 +7033,7 @@
       </c>
       <c r="F26" s="24">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.3799999999999998E-2</v>
+        <v>2.3700000000000002E-2</v>
       </c>
       <c r="G26" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -6947,12 +7048,16 @@
         <v>44830</v>
       </c>
       <c r="J26" s="24">
-        <v>2.4030546429328073E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.393361140079282E-2</v>
+      </c>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="190"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D27" s="25" t="str">
-        <v>obj_00380</v>
+        <v>obj_003ad</v>
       </c>
       <c r="E27" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D27)</f>
@@ -6960,7 +7065,7 @@
       </c>
       <c r="F27" s="24">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.4590000000000001E-2</v>
+        <v>2.4510000000000001E-2</v>
       </c>
       <c r="G27" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -6975,12 +7080,16 @@
         <v>45194</v>
       </c>
       <c r="J27" s="24">
-        <v>2.4865952634494273E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.4790868167667672E-2</v>
+      </c>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="190"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D28" s="25" t="str">
-        <v>obj_00385</v>
+        <v>obj_0039f</v>
       </c>
       <c r="E28" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D28)</f>
@@ -6988,7 +7097,7 @@
       </c>
       <c r="F28" s="24">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.5270000000000001E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="G28" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -7003,12 +7112,16 @@
         <v>45560</v>
       </c>
       <c r="J28" s="24">
-        <v>2.5591051807028926E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.552680710581276E-2</v>
+      </c>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="190"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D29" s="25" t="str">
-        <v>obj_00375</v>
+        <v>obj_0039b</v>
       </c>
       <c r="E29" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D29)</f>
@@ -7016,7 +7129,7 @@
       </c>
       <c r="F29" s="24">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.6420000000000003E-2</v>
+        <v>2.6360000000000001E-2</v>
       </c>
       <c r="G29" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -7031,12 +7144,16 @@
         <v>46290</v>
       </c>
       <c r="J29" s="24">
-        <v>2.6837805980087767E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.6784216483779804E-2</v>
+      </c>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
+      <c r="O29" s="73"/>
+      <c r="P29" s="190"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D30" s="25" t="str">
-        <v>obj_00374</v>
+        <v>obj_00375</v>
       </c>
       <c r="E30" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D30)</f>
@@ -7044,7 +7161,7 @@
       </c>
       <c r="F30" s="24">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.759E-2</v>
+        <v>2.7549999999999998E-2</v>
       </c>
       <c r="G30" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -7059,12 +7176,16 @@
         <v>47386</v>
       </c>
       <c r="J30" s="24">
-        <v>2.812471079464705E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.809406059200812E-2</v>
+      </c>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="190"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D31" s="25" t="str">
-        <v>obj_0038b</v>
+        <v>obj_0038f</v>
       </c>
       <c r="E31" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D31)</f>
@@ -7072,7 +7193,7 @@
       </c>
       <c r="F31" s="24">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.8580000000000001E-2</v>
+        <v>2.8570000000000002E-2</v>
       </c>
       <c r="G31" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -7087,12 +7208,16 @@
         <v>49212</v>
       </c>
       <c r="J31" s="24">
-        <v>2.9207357456557028E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.921323122106028E-2</v>
+      </c>
+      <c r="M31" s="73"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="190"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D32" s="25" t="str">
-        <v>obj_0034b</v>
+        <v>obj_003a5</v>
       </c>
       <c r="E32" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D32)</f>
@@ -7100,7 +7225,7 @@
       </c>
       <c r="F32" s="24">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.8810000000000002E-2</v>
+        <v>2.8830000000000001E-2</v>
       </c>
       <c r="G32" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -7115,12 +7240,16 @@
         <v>51039</v>
       </c>
       <c r="J32" s="24">
-        <v>2.9360550614404159E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.9405344144962379E-2</v>
+      </c>
+      <c r="M32" s="73"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="190"/>
+    </row>
+    <row r="33" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D33" s="25" t="str">
-        <v>obj_0037e</v>
+        <v>obj_00395</v>
       </c>
       <c r="E33" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D33)</f>
@@ -7128,7 +7257,7 @@
       </c>
       <c r="F33" s="24">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.8849999999999997E-2</v>
+        <v>2.8890000000000002E-2</v>
       </c>
       <c r="G33" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -7143,12 +7272,16 @@
         <v>52866</v>
       </c>
       <c r="J33" s="24">
-        <v>2.9294272642382307E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.9365177279646635E-2</v>
+      </c>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="190"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D34" s="25" t="str">
-        <v>obj_0035d</v>
+        <v>obj_00373</v>
       </c>
       <c r="E34" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D34)</f>
@@ -7156,7 +7289,7 @@
       </c>
       <c r="F34" s="24">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.8670000000000001E-2</v>
+        <v>2.8730000000000002E-2</v>
       </c>
       <c r="G34" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -7171,12 +7304,16 @@
         <v>56517</v>
       </c>
       <c r="J34" s="24">
-        <v>2.8832419498203275E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.8927712675603266E-2</v>
+      </c>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="190"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D35" s="25" t="str">
-        <v>obj_00352</v>
+        <v>obj_00386</v>
       </c>
       <c r="E35" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D35)</f>
@@ -7184,7 +7321,7 @@
       </c>
       <c r="F35" s="24">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.8660000000000001E-2</v>
+        <v>2.8730000000000002E-2</v>
       </c>
       <c r="G35" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -7199,12 +7336,16 @@
         <v>60170</v>
       </c>
       <c r="J35" s="24">
-        <v>2.873906531854814E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.8846475288294409E-2</v>
+      </c>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="190"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D36" s="25" t="str">
-        <v>obj_00371</v>
+        <v>obj_003a6</v>
       </c>
       <c r="E36" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D36)</f>
@@ -7212,7 +7353,7 @@
       </c>
       <c r="F36" s="24">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.879E-2</v>
+        <v>2.886E-2</v>
       </c>
       <c r="G36" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -7227,10 +7368,14 @@
         <v>63822</v>
       </c>
       <c r="J36" s="24">
-        <v>2.8994624103543237E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.2">
+        <v>2.9096985069627438E-2</v>
+      </c>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="190"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D37" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7257,8 +7402,12 @@
       <c r="J37" s="24" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="190"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D38" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7285,8 +7434,12 @@
       <c r="J38" s="24" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="190"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D39" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7313,8 +7466,12 @@
       <c r="J39" s="24" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="M39" s="73"/>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="190"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D40" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7342,7 +7499,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D41" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7370,7 +7527,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D42" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7398,7 +7555,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D43" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7426,7 +7583,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D44" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7454,7 +7611,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D45" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7482,7 +7639,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D46" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7510,7 +7667,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D47" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -7538,7 +7695,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D48" s="25" t="e">
         <v>#N/A</v>
       </c>
@@ -9771,9 +9928,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9860,7 +10015,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" ref="D3:D19" si="0">Calendar</f>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E3" s="84" t="s">
@@ -9872,16 +10027,16 @@
       <c r="G3" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="186" t="s">
+      <c r="H3" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="187" t="str">
+      <c r="I3" s="181" t="str">
         <f>Currency&amp;$B3&amp;"D"&amp;QuoteSuffix</f>
         <v>GBPOND_Quote</v>
       </c>
-      <c r="J3" s="188" t="str">
+      <c r="J3" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I3,H3,Permanent,Trigger)</f>
-        <v>obj_00337#0031</v>
+        <v>obj_00357#0006</v>
       </c>
       <c r="K3" s="83" t="str">
         <f>_xll.ohRangeRetrieveError(J3)</f>
@@ -9899,7 +10054,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E4" s="84" t="s">
@@ -9913,7 +10068,7 @@
       </c>
       <c r="H4" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00637#0008</v>
+        <v>obj_00349#0006</v>
       </c>
       <c r="I4" s="80" t="str">
         <f>Currency&amp;$B4&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -9921,7 +10076,7 @@
       </c>
       <c r="J4" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I4,"1D",C4,D4,E4,F4,G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033a#0008</v>
+        <v>obj_0035b#0006</v>
       </c>
       <c r="K4" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J4)</f>
@@ -9939,7 +10094,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E5" s="84" t="s">
@@ -9951,17 +10106,17 @@
       <c r="G5" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H5" s="186" t="str">
+      <c r="H5" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B5</f>
         <v>GBPLiborSW</v>
       </c>
-      <c r="I5" s="187" t="str">
+      <c r="I5" s="181" t="str">
         <f>Currency&amp;$B5&amp;"D"&amp;QuoteSuffix</f>
         <v>GBPSWD_Quote</v>
       </c>
-      <c r="J5" s="188" t="str">
+      <c r="J5" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I5,H5,Permanent,Trigger)</f>
-        <v>obj_0064e#0007</v>
+        <v>obj_00348#0006</v>
       </c>
       <c r="K5" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J5)</f>
@@ -9979,7 +10134,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E6" s="84" t="s">
@@ -9993,7 +10148,7 @@
       </c>
       <c r="H6" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0063b#0007</v>
+        <v>obj_0034e#0006</v>
       </c>
       <c r="I6" s="80" t="str">
         <f>Currency&amp;$B6&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10001,7 +10156,7 @@
       </c>
       <c r="J6" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I6,B6,C6,D6,E6,F6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033c#0005</v>
+        <v>obj_0035f#0006</v>
       </c>
       <c r="K6" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J6)</f>
@@ -10019,7 +10174,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E7" s="84" t="s">
@@ -10033,7 +10188,7 @@
       </c>
       <c r="H7" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0063d#0007</v>
+        <v>obj_00352#0006</v>
       </c>
       <c r="I7" s="80" t="str">
         <f>Currency&amp;$B7&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10041,7 +10196,7 @@
       </c>
       <c r="J7" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I7,B7,C7,D7,E7,F7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00338#0005</v>
+        <v>obj_00361#0006</v>
       </c>
       <c r="K7" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J7)</f>
@@ -10059,7 +10214,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E8" s="84" t="s">
@@ -10071,17 +10226,17 @@
       <c r="G8" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="186" t="str">
+      <c r="H8" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B8</f>
         <v>GBPLibor1M</v>
       </c>
-      <c r="I8" s="187" t="str">
+      <c r="I8" s="181" t="str">
         <f>Currency&amp;$B8&amp;"D"&amp;QuoteSuffix</f>
         <v>GBP1MD_Quote</v>
       </c>
-      <c r="J8" s="188" t="str">
+      <c r="J8" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I8,H8,Permanent,Trigger)</f>
-        <v>obj_0033d#0019</v>
+        <v>obj_00355#0006</v>
       </c>
       <c r="K8" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J8)</f>
@@ -10099,7 +10254,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E9" s="84" t="s">
@@ -10111,17 +10266,17 @@
       <c r="G9" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H9" s="186" t="str">
+      <c r="H9" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B9</f>
         <v>GBPLibor2M</v>
       </c>
-      <c r="I9" s="187" t="str">
+      <c r="I9" s="181" t="str">
         <f>Currency&amp;$B9&amp;"D"&amp;QuoteSuffix</f>
         <v>GBP2MD_Quote</v>
       </c>
-      <c r="J9" s="188" t="str">
+      <c r="J9" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I9,H9,Permanent,Trigger)</f>
-        <v>obj_0062a#0017</v>
+        <v>obj_00351#0006</v>
       </c>
       <c r="K9" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J9)</f>
@@ -10139,7 +10294,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E10" s="84" t="s">
@@ -10151,17 +10306,17 @@
       <c r="G10" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H10" s="186" t="str">
+      <c r="H10" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B10</f>
         <v>GBPLibor3M</v>
       </c>
-      <c r="I10" s="187" t="str">
+      <c r="I10" s="181" t="str">
         <f>Currency&amp;$B10&amp;"D"&amp;QuoteSuffix</f>
         <v>GBP3MD_Quote</v>
       </c>
-      <c r="J10" s="188" t="str">
+      <c r="J10" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I10,H10,Permanent,Trigger)</f>
-        <v>obj_0062b#0017</v>
+        <v>obj_00353#0006</v>
       </c>
       <c r="K10" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J10)</f>
@@ -10179,7 +10334,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E11" s="84" t="s">
@@ -10193,7 +10348,7 @@
       </c>
       <c r="H11" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00645#0007</v>
+        <v>obj_0034c#0006</v>
       </c>
       <c r="I11" s="80" t="str">
         <f>Currency&amp;$B11&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10201,7 +10356,7 @@
       </c>
       <c r="J11" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I11,B11,C11,D11,E11,F11,G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0064c#0003</v>
+        <v>obj_0035e#0006</v>
       </c>
       <c r="K11" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J11)</f>
@@ -10219,7 +10374,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E12" s="84" t="s">
@@ -10233,7 +10388,7 @@
       </c>
       <c r="H12" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00638#0007</v>
+        <v>obj_0034b#0006</v>
       </c>
       <c r="I12" s="80" t="str">
         <f>Currency&amp;$B12&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10241,7 +10396,7 @@
       </c>
       <c r="J12" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I12,B12,C12,D12,E12,F12,G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00339#0005</v>
+        <v>obj_0035d#0006</v>
       </c>
       <c r="K12" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J12)</f>
@@ -10259,7 +10414,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E13" s="84" t="s">
@@ -10271,17 +10426,17 @@
       <c r="G13" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H13" s="186" t="str">
+      <c r="H13" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B13</f>
         <v>GBPLibor6M</v>
       </c>
-      <c r="I13" s="187" t="str">
+      <c r="I13" s="181" t="str">
         <f>Currency&amp;$B13&amp;"D"&amp;QuoteSuffix</f>
         <v>GBP6MD_Quote</v>
       </c>
-      <c r="J13" s="188" t="str">
+      <c r="J13" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I13,H13,Permanent,Trigger)</f>
-        <v>obj_0062d#0017</v>
+        <v>obj_0034f#0006</v>
       </c>
       <c r="K13" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J13)</f>
@@ -10299,7 +10454,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E14" s="84" t="s">
@@ -10313,7 +10468,7 @@
       </c>
       <c r="H14" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0063c#0007</v>
+        <v>obj_00350#0006</v>
       </c>
       <c r="I14" s="80" t="str">
         <f>Currency&amp;$B14&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10321,7 +10476,7 @@
       </c>
       <c r="J14" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I14,B14,C14,D14,E14,F14,G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00647#0003</v>
+        <v>obj_00360#0006</v>
       </c>
       <c r="K14" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J14)</f>
@@ -10339,7 +10494,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E15" s="84" t="s">
@@ -10353,7 +10508,7 @@
       </c>
       <c r="H15" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0063e#0007</v>
+        <v>obj_00354#0006</v>
       </c>
       <c r="I15" s="80" t="str">
         <f>Currency&amp;$B15&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10361,7 +10516,7 @@
       </c>
       <c r="J15" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I15,B15,C15,D15,E15,F15,G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00648#0003</v>
+        <v>obj_00362#0006</v>
       </c>
       <c r="K15" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J15)</f>
@@ -10379,7 +10534,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E16" s="84" t="s">
@@ -10393,7 +10548,7 @@
       </c>
       <c r="H16" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00640#0007</v>
+        <v>obj_00356#0006</v>
       </c>
       <c r="I16" s="80" t="str">
         <f>Currency&amp;$B16&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10401,7 +10556,7 @@
       </c>
       <c r="J16" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I16,B16,C16,D16,E16,F16,G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00649#0003</v>
+        <v>obj_00359#0006</v>
       </c>
       <c r="K16" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J16)</f>
@@ -10419,7 +10574,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E17" s="84" t="s">
@@ -10433,7 +10588,7 @@
       </c>
       <c r="H17" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00642#0007</v>
+        <v>obj_00358#0006</v>
       </c>
       <c r="I17" s="80" t="str">
         <f>Currency&amp;$B17&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10441,7 +10596,7 @@
       </c>
       <c r="J17" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I17,B17,C17,D17,E17,F17,G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0064a#0003</v>
+        <v>obj_0035a#0006</v>
       </c>
       <c r="K17" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J17)</f>
@@ -10459,7 +10614,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E18" s="84" t="s">
@@ -10473,7 +10628,7 @@
       </c>
       <c r="H18" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00644#0007</v>
+        <v>obj_0034a#0006</v>
       </c>
       <c r="I18" s="80" t="str">
         <f>Currency&amp;$B18&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10481,7 +10636,7 @@
       </c>
       <c r="J18" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I18,B18,C18,D18,E18,F18,G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0064b#0003</v>
+        <v>obj_0035c#0006</v>
       </c>
       <c r="K18" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J18)</f>
@@ -10499,7 +10654,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="84" t="str">
-        <f>Calendar</f>
+        <f t="shared" si="0"/>
         <v>UnitedKingdom::Exchange</v>
       </c>
       <c r="E19" s="84" t="s">
@@ -10511,17 +10666,17 @@
       <c r="G19" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="186" t="str">
+      <c r="H19" s="180" t="str">
         <f>Currency&amp;FamilyName&amp;B19</f>
         <v>GBPLibor1Y</v>
       </c>
-      <c r="I19" s="187" t="str">
+      <c r="I19" s="181" t="str">
         <f>Currency&amp;$B19&amp;"D"&amp;QuoteSuffix</f>
         <v>GBP1YD_Quote</v>
       </c>
-      <c r="J19" s="188" t="str">
+      <c r="J19" s="182" t="str">
         <f>_xll.qlDepositRateHelper(,I19,H19,Permanent,Trigger)</f>
-        <v>obj_0062c#0017</v>
+        <v>obj_0034d#0006</v>
       </c>
       <c r="K19" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J19)</f>
@@ -10531,18 +10686,18 @@
       <c r="N19" s="76"/>
     </row>
     <row r="20" spans="1:14" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="184"/>
-      <c r="B20" s="184"/>
-      <c r="C20" s="184"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="184"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
-      <c r="K20" s="184"/>
-      <c r="L20" s="185"/>
+      <c r="A20" s="178"/>
+      <c r="B20" s="178"/>
+      <c r="C20" s="178"/>
+      <c r="D20" s="178"/>
+      <c r="E20" s="178"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="178"/>
+      <c r="J20" s="178"/>
+      <c r="K20" s="178"/>
+      <c r="L20" s="179"/>
       <c r="N20" s="76"/>
     </row>
     <row r="21" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10570,7 +10725,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10664,7 +10819,7 @@
       </c>
       <c r="H3" s="135" t="str">
         <f>_xll.qlFuturesRateHelper(,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00340#0001</v>
+        <v>obj_00377#0006</v>
       </c>
       <c r="I3" s="136" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -10698,7 +10853,7 @@
       </c>
       <c r="H4" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00391#0006</v>
       </c>
       <c r="I4" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -10732,7 +10887,7 @@
       </c>
       <c r="H5" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0036e#0006</v>
       </c>
       <c r="I5" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -10766,7 +10921,7 @@
       </c>
       <c r="H6" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00344#0001</v>
+        <v>obj_003ae#0006</v>
       </c>
       <c r="I6" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -10800,7 +10955,7 @@
       </c>
       <c r="H7" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035a#0001</v>
+        <v>obj_003ac#0006</v>
       </c>
       <c r="I7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -10834,7 +10989,7 @@
       </c>
       <c r="H8" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034c#0001</v>
+        <v>obj_00389#0006</v>
       </c>
       <c r="I8" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -10868,7 +11023,7 @@
       </c>
       <c r="H9" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00360#0001</v>
+        <v>obj_00394#0006</v>
       </c>
       <c r="I9" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -10902,7 +11057,7 @@
       </c>
       <c r="H10" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00383#0006</v>
       </c>
       <c r="I10" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -10936,7 +11091,7 @@
       </c>
       <c r="H11" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00393#0006</v>
       </c>
       <c r="I11" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -10970,7 +11125,7 @@
       </c>
       <c r="H12" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00373#0001</v>
+        <v>obj_0036b#0006</v>
       </c>
       <c r="I12" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -11004,7 +11159,7 @@
       </c>
       <c r="H13" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00376#0006</v>
       </c>
       <c r="I13" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -11038,7 +11193,7 @@
       </c>
       <c r="H14" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_0037f#0006</v>
       </c>
       <c r="I14" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H14)</f>
@@ -11072,7 +11227,7 @@
       </c>
       <c r="H15" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00346#0001</v>
+        <v>obj_00370#0006</v>
       </c>
       <c r="I15" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H15)</f>
@@ -11106,7 +11261,7 @@
       </c>
       <c r="H16" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035c#0001</v>
+        <v>obj_00368#0006</v>
       </c>
       <c r="I16" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H16)</f>
@@ -11140,7 +11295,7 @@
       </c>
       <c r="H17" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_0037a#0006</v>
       </c>
       <c r="I17" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H17)</f>
@@ -11174,7 +11329,7 @@
       </c>
       <c r="H18" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036d#0001</v>
+        <v>obj_0037b#0006</v>
       </c>
       <c r="I18" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H18)</f>
@@ -11208,7 +11363,7 @@
       </c>
       <c r="H19" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00341#0001</v>
+        <v>obj_0039c#0006</v>
       </c>
       <c r="I19" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H19)</f>
@@ -11242,7 +11397,7 @@
       </c>
       <c r="H20" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00362#0001</v>
+        <v>obj_00387#0006</v>
       </c>
       <c r="I20" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H20)</f>
@@ -11276,7 +11431,7 @@
       </c>
       <c r="H21" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034d#0001</v>
+        <v>obj_00366#0006</v>
       </c>
       <c r="I21" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H21)</f>
@@ -11310,7 +11465,7 @@
       </c>
       <c r="H22" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034f#0001</v>
+        <v>obj_0037d#0006</v>
       </c>
       <c r="I22" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H22)</f>
@@ -11344,7 +11499,7 @@
       </c>
       <c r="H23" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00376#0001</v>
+        <v>obj_0039e#0006</v>
       </c>
       <c r="I23" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H23)</f>
@@ -11378,7 +11533,7 @@
       </c>
       <c r="H24" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00382#0001</v>
+        <v>obj_0036d#0006</v>
       </c>
       <c r="I24" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H24)</f>
@@ -11412,7 +11567,7 @@
       </c>
       <c r="H25" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00355#0001</v>
+        <v>obj_00372#0006</v>
       </c>
       <c r="I25" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H25)</f>
@@ -11446,7 +11601,7 @@
       </c>
       <c r="H26" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00348#0001</v>
+        <v>obj_00390#0006</v>
       </c>
       <c r="I26" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H26)</f>
@@ -11480,7 +11635,7 @@
       </c>
       <c r="H27" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00369#0001</v>
+        <v>obj_003a3#0006</v>
       </c>
       <c r="I27" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H27)</f>
@@ -11514,7 +11669,7 @@
       </c>
       <c r="H28" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_0036c#0006</v>
       </c>
       <c r="I28" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H28)</f>
@@ -11548,7 +11703,7 @@
       </c>
       <c r="H29" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00350#0001</v>
+        <v>obj_00380#0006</v>
       </c>
       <c r="I29" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H29)</f>
@@ -11582,7 +11737,7 @@
       </c>
       <c r="H30" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00387#0001</v>
+        <v>obj_003aa#0006</v>
       </c>
       <c r="I30" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H30)</f>
@@ -11616,7 +11771,7 @@
       </c>
       <c r="H31" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036b#0001</v>
+        <v>obj_0039a#0006</v>
       </c>
       <c r="I31" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H31)</f>
@@ -11650,7 +11805,7 @@
       </c>
       <c r="H32" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_0038c#0006</v>
       </c>
       <c r="I32" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H32)</f>
@@ -11684,7 +11839,7 @@
       </c>
       <c r="H33" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0038a#0006</v>
       </c>
       <c r="I33" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H33)</f>
@@ -11718,7 +11873,7 @@
       </c>
       <c r="H34" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034e#0001</v>
+        <v>obj_00371#0006</v>
       </c>
       <c r="I34" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H34)</f>
@@ -11752,7 +11907,7 @@
       </c>
       <c r="H35" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00368#0001</v>
+        <v>obj_003a8#0006</v>
       </c>
       <c r="I35" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H35)</f>
@@ -11786,7 +11941,7 @@
       </c>
       <c r="H36" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034a#0001</v>
+        <v>obj_003a2#0006</v>
       </c>
       <c r="I36" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H36)</f>
@@ -11820,7 +11975,7 @@
       </c>
       <c r="H37" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00384#0001</v>
+        <v>obj_0037c#0006</v>
       </c>
       <c r="I37" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H37)</f>
@@ -11854,7 +12009,7 @@
       </c>
       <c r="H38" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00377#0001</v>
+        <v>obj_003a1#0006</v>
       </c>
       <c r="I38" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H38)</f>
@@ -11888,7 +12043,7 @@
       </c>
       <c r="H39" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_0038e#0006</v>
       </c>
       <c r="I39" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H39)</f>
@@ -11922,7 +12077,7 @@
       </c>
       <c r="H40" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00361#0001</v>
+        <v>obj_00397#0006</v>
       </c>
       <c r="I40" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H40)</f>
@@ -11956,7 +12111,7 @@
       </c>
       <c r="H41" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0033e#0001</v>
+        <v>obj_00364#0006</v>
       </c>
       <c r="I41" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H41)</f>
@@ -11991,7 +12146,7 @@
       </c>
       <c r="H42" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00347#0001</v>
+        <v>obj_00378#0006</v>
       </c>
       <c r="I42" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H42)</f>
@@ -12025,7 +12180,7 @@
       </c>
       <c r="H43" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00366#0001</v>
+        <v>obj_0038d#0006</v>
       </c>
       <c r="I43" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H43)</f>
@@ -12059,7 +12214,7 @@
       </c>
       <c r="H44" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00378#0001</v>
+        <v>obj_00398#0006</v>
       </c>
       <c r="I44" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H44)</f>
@@ -12199,7 +12354,7 @@
       <c r="J4" s="90"/>
       <c r="K4" s="159" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor(,$I$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor(,Currency,$I$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>obj_00336#0001</v>
+        <v>obj_00363#0006</v>
       </c>
       <c r="L4" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(K4)</f>
@@ -12258,7 +12413,7 @@
       </c>
       <c r="K6" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$4,$I6,B6,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00343#0001</v>
+        <v>obj_003ab#0006</v>
       </c>
       <c r="L6" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -12305,7 +12460,7 @@
       </c>
       <c r="K7" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$4,$I7,B7,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_003af#0006</v>
       </c>
       <c r="L7" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -12356,7 +12511,7 @@
       </c>
       <c r="K8" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$4,$I8,B8,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00351#0001</v>
+        <v>obj_00384#0006</v>
       </c>
       <c r="L8" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -12407,7 +12562,7 @@
       </c>
       <c r="K9" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$4,$I9,B9,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_00382#0006</v>
       </c>
       <c r="L9" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -12454,7 +12609,7 @@
       </c>
       <c r="K10" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$4,$I10,B10,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00364#0001</v>
+        <v>obj_00369#0006</v>
       </c>
       <c r="L10" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -12505,7 +12660,7 @@
       </c>
       <c r="K11" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$4,$I11,B11,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0033f#0001</v>
+        <v>obj_0036f#0006</v>
       </c>
       <c r="L11" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -12547,7 +12702,7 @@
       </c>
       <c r="K12" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$4,$I12,B12,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00357#0001</v>
+        <v>obj_0039d#0006</v>
       </c>
       <c r="L12" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -12589,7 +12744,7 @@
       </c>
       <c r="K13" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$4,$I13,B13,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_003a4#0006</v>
       </c>
       <c r="L13" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -12631,7 +12786,7 @@
       </c>
       <c r="K14" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$4,$I14,B14,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00349#0001</v>
+        <v>obj_003a0#0006</v>
       </c>
       <c r="L14" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -12673,7 +12828,7 @@
       </c>
       <c r="K15" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$4,$I15,B15,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_00399#0006</v>
       </c>
       <c r="L15" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -12715,7 +12870,7 @@
       </c>
       <c r="K16" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$4,$I16,B16,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00359#0001</v>
+        <v>obj_003a9#0006</v>
       </c>
       <c r="L16" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -12757,7 +12912,7 @@
       </c>
       <c r="K17" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$4,$I17,B17,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00380#0001</v>
+        <v>obj_003ad#0006</v>
       </c>
       <c r="L17" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -12799,7 +12954,7 @@
       </c>
       <c r="K18" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$4,$I18,B18,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00385#0001</v>
+        <v>obj_0039f#0006</v>
       </c>
       <c r="L18" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -12841,7 +12996,7 @@
       </c>
       <c r="K19" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$4,$I19,B19,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00356#0001</v>
+        <v>obj_00379#0006</v>
       </c>
       <c r="L19" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -12883,7 +13038,7 @@
       </c>
       <c r="K20" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$4,$I20,B20,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00375#0001</v>
+        <v>obj_0039b#0006</v>
       </c>
       <c r="L20" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -12925,7 +13080,7 @@
       </c>
       <c r="K21" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$4,$I21,B21,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00388#0001</v>
+        <v>obj_003b2#0006</v>
       </c>
       <c r="L21" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -12967,7 +13122,7 @@
       </c>
       <c r="K22" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$4,$I22,B22,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00365#0001</v>
+        <v>obj_00374#0006</v>
       </c>
       <c r="L22" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -13009,7 +13164,7 @@
       </c>
       <c r="K23" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$4,$I23,B23,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00374#0001</v>
+        <v>obj_00375#0006</v>
       </c>
       <c r="L23" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -13051,7 +13206,7 @@
       </c>
       <c r="K24" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$4,$I24,B24,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00358#0001</v>
+        <v>obj_00381#0006</v>
       </c>
       <c r="L24" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -13093,7 +13248,7 @@
       </c>
       <c r="K25" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$4,$I25,B25,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00342#0001</v>
+        <v>obj_00396#0006</v>
       </c>
       <c r="L25" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -13135,7 +13290,7 @@
       </c>
       <c r="K26" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$4,$I26,B26,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00354#0001</v>
+        <v>obj_00367#0006</v>
       </c>
       <c r="L26" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -13177,7 +13332,7 @@
       </c>
       <c r="K27" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$4,$I27,B27,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00379#0001</v>
+        <v>obj_00388#0006</v>
       </c>
       <c r="L27" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -13219,7 +13374,7 @@
       </c>
       <c r="K28" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$4,$I28,B28,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_0038f#0006</v>
       </c>
       <c r="L28" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>
@@ -13261,7 +13416,7 @@
       </c>
       <c r="K29" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J29,$C29,Calendar,$F29,$G29,$H29,$K$4,$I29,B29,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00345#0001</v>
+        <v>obj_00365#0006</v>
       </c>
       <c r="L29" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K29)</f>
@@ -13303,7 +13458,7 @@
       </c>
       <c r="K30" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J30,$C30,Calendar,$F30,$G30,$H30,$K$4,$I30,B30,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00381#0001</v>
+        <v>obj_003a7#0006</v>
       </c>
       <c r="L30" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K30)</f>
@@ -13345,7 +13500,7 @@
       </c>
       <c r="K31" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J31,$C31,Calendar,$F31,$G31,$H31,$K$4,$I31,B31,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00370#0001</v>
+        <v>obj_00385#0006</v>
       </c>
       <c r="L31" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K31)</f>
@@ -13387,7 +13542,7 @@
       </c>
       <c r="K32" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J32,$C32,Calendar,$F32,$G32,$H32,$K$4,$I32,B32,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_0038b#0006</v>
       </c>
       <c r="L32" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K32)</f>
@@ -13429,7 +13584,7 @@
       </c>
       <c r="K33" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J33,$C33,Calendar,$F33,$G33,$H33,$K$4,$I33,B33,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0034b#0001</v>
+        <v>obj_003a5#0006</v>
       </c>
       <c r="L33" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K33)</f>
@@ -13471,7 +13626,7 @@
       </c>
       <c r="K34" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J34,$C34,Calendar,$F34,$G34,$H34,$K$4,$I34,B34,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_0036a#0006</v>
       </c>
       <c r="L34" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K34)</f>
@@ -13513,7 +13668,7 @@
       </c>
       <c r="K35" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J35,$C35,Calendar,$F35,$G35,$H35,$K$4,$I35,B35,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00367#0001</v>
+        <v>obj_0037e#0006</v>
       </c>
       <c r="L35" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K35)</f>
@@ -13555,7 +13710,7 @@
       </c>
       <c r="K36" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J36,$C36,Calendar,$F36,$G36,$H36,$K$4,$I36,B36,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00353#0001</v>
+        <v>obj_003b1#0006</v>
       </c>
       <c r="L36" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K36)</f>
@@ -13597,7 +13752,7 @@
       </c>
       <c r="K37" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J37,$C37,Calendar,$F37,$G37,$H37,$K$4,$I37,B37,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036e#0001</v>
+        <v>obj_00392#0006</v>
       </c>
       <c r="L37" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K37)</f>
@@ -13639,7 +13794,7 @@
       </c>
       <c r="K38" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J38,$C38,Calendar,$F38,$G38,$H38,$K$4,$I38,B38,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_00395#0006</v>
       </c>
       <c r="L38" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K38)</f>
@@ -13681,7 +13836,7 @@
       </c>
       <c r="K39" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J39,$C39,Calendar,$F39,$G39,$H39,$K$4,$I39,B39,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00372#0001</v>
+        <v>obj_003b0#0006</v>
       </c>
       <c r="L39" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K39)</f>
@@ -13723,7 +13878,7 @@
       </c>
       <c r="K40" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J40,$C40,Calendar,$F40,$G40,$H40,$K$4,$I40,B40,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_00373#0006</v>
       </c>
       <c r="L40" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K40)</f>
@@ -13765,7 +13920,7 @@
       </c>
       <c r="K41" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J41,$C41,Calendar,$F41,$G41,$H41,$K$4,$I41,B41,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00352#0001</v>
+        <v>obj_00386#0006</v>
       </c>
       <c r="L41" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K41)</f>
@@ -13807,7 +13962,7 @@
       </c>
       <c r="K42" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J42,$C42,Calendar,$F42,$G42,$H42,$K$4,$I42,B42,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00371#0001</v>
+        <v>obj_003a6#0006</v>
       </c>
       <c r="L42" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K42)</f>

</xml_diff>

<commit_message>
GBP std using hist close for future
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15180" windowHeight="8145" activeTab="2"/>
+    <workbookView xWindow="15225" yWindow="-15" windowWidth="15270" windowHeight="8415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="D14" s="59" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_GBPYCSTD#0003</v>
+        <v>_GBPYCSTD#0005</v>
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="40"/>
@@ -2469,11 +2469,11 @@
       <c r="B23" s="43"/>
       <c r="C23" s="46">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="D23" s="120">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>2.8237341484246427E-2</v>
+        <v>2.795998665109669E-2</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="40"/>
@@ -2482,11 +2482,11 @@
       <c r="B24" s="43"/>
       <c r="C24" s="45">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>63837</v>
+        <v>63842</v>
       </c>
       <c r="D24" s="121">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>4.7437075217081001E-3</v>
+        <v>4.7437691733986558E-3</v>
       </c>
       <c r="E24" s="41"/>
       <c r="F24" s="40"/>
@@ -2630,7 +2630,7 @@
     <row r="2" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="149" t="str">
         <f>Deposits!J3</f>
-        <v>obj_00352#0001</v>
+        <v>obj_0034a#0001</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B2)</f>
@@ -2652,11 +2652,11 @@
       </c>
       <c r="I2" s="4">
         <f>_xll.qlRateHelperEarliestDate($B2,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J2" s="3">
         <f>_xll.qlRateHelperLatestDate($B2,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="K2" s="1">
         <v>10</v>
@@ -2669,7 +2669,7 @@
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="149" t="str">
         <f>Deposits!J4</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_0035a#0001</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B3)</f>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="D3" s="6">
         <f>_xll.qlRateHelperQuoteValue($B3,Trigger)</f>
-        <v>4.8313000000000002E-3</v>
+        <v>4.8063000000000003E-3</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="74" t="b">
@@ -2691,11 +2691,11 @@
       </c>
       <c r="I3" s="4">
         <f>_xll.qlRateHelperEarliestDate($B3,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J3" s="3">
         <f>_xll.qlRateHelperLatestDate($B3,Trigger)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="K3" s="1">
         <v>20</v>
@@ -2708,7 +2708,7 @@
     <row r="4" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="149" t="str">
         <f>Deposits!J5</f>
-        <v>obj_00351#0001</v>
+        <v>obj_00358#0001</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B4)</f>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="D4" s="6">
         <f>_xll.qlRateHelperQuoteValue($B4,Trigger)</f>
-        <v>4.8313000000000002E-3</v>
+        <v>4.8063000000000003E-3</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="74" t="b">
@@ -2730,17 +2730,17 @@
       </c>
       <c r="I4" s="4">
         <f>_xll.qlRateHelperEarliestDate($B4,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J4" s="3">
         <f>_xll.qlRateHelperLatestDate($B4,Trigger)</f>
-        <v>41929</v>
+        <v>41932</v>
       </c>
     </row>
     <row r="5" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="149" t="str">
         <f>Deposits!J6</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0035f#0001</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B5)</f>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="D5" s="6">
         <f>_xll.qlRateHelperQuoteValue($B5,Trigger)</f>
-        <v>4.8952624999999998E-3</v>
+        <v>4.8704038499999998E-3</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="74" t="b">
@@ -2762,17 +2762,17 @@
       </c>
       <c r="I5" s="4">
         <f>_xll.qlRateHelperEarliestDate($B5,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J5" s="3">
         <f>_xll.qlRateHelperLatestDate($B5,Trigger)</f>
-        <v>41936</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="149" t="str">
         <f>Deposits!J7</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00362#0001</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B6)</f>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D6" s="6">
         <f>_xll.qlRateHelperQuoteValue($B6,Trigger)</f>
-        <v>4.9683625000000002E-3</v>
+        <v>4.9345076900000001E-3</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="74" t="b">
@@ -2794,11 +2794,11 @@
       </c>
       <c r="I6" s="4">
         <f>_xll.qlRateHelperEarliestDate($B6,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J6" s="3">
         <f>_xll.qlRateHelperLatestDate($B6,Trigger)</f>
-        <v>41943</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="7" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -2812,7 +2812,7 @@
       </c>
       <c r="D7" s="6">
         <f>_xll.qlRateHelperQuoteValue($B7,Trigger)</f>
-        <v>5.0505999999999997E-3</v>
+        <v>5.0444000000000001E-3</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="74" t="b">
@@ -2826,17 +2826,17 @@
       </c>
       <c r="I7" s="4">
         <f>_xll.qlRateHelperEarliestDate($B7,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J7" s="3">
         <f>_xll.qlRateHelperLatestDate($B7,Trigger)</f>
-        <v>41953</v>
+        <v>41956</v>
       </c>
     </row>
     <row r="8" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="149" t="str">
         <f>Deposits!J9</f>
-        <v>obj_00349#0001</v>
+        <v>obj_00357#0001</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B8)</f>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="D8" s="6">
         <f>_xll.qlRateHelperQuoteValue($B8,Trigger)</f>
-        <v>5.2649999999999997E-3</v>
+        <v>5.2963000000000003E-3</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="74" t="b">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="I8" s="4">
         <f>_xll.qlRateHelperEarliestDate($B8,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J8" s="3">
         <f>_xll.qlRateHelperLatestDate($B8,Trigger)</f>
-        <v>41983</v>
+        <v>41988</v>
       </c>
     </row>
     <row r="9" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="149" t="str">
         <f>Deposits!J10</f>
-        <v>obj_00355#0001</v>
+        <v>obj_00350#0001</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B9)</f>
@@ -2890,17 +2890,17 @@
       </c>
       <c r="I9" s="4">
         <f>_xll.qlRateHelperEarliestDate($B9,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J9" s="3">
         <f>_xll.qlRateHelperLatestDate($B9,Trigger)</f>
-        <v>42016</v>
+        <v>42017</v>
       </c>
     </row>
     <row r="10" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="149" t="str">
         <f>Deposits!J11</f>
-        <v>obj_00362#0001</v>
+        <v>obj_0035d#0001</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B10)</f>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D10" s="6">
         <f>_xll.qlRateHelperQuoteValue($B10,Trigger)</f>
-        <v>6.0992999999999993E-3</v>
+        <v>6.0985688900000003E-3</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="74" t="b">
@@ -2922,17 +2922,17 @@
       </c>
       <c r="I10" s="4">
         <f>_xll.qlRateHelperEarliestDate($B10,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J10" s="3">
         <f>_xll.qlRateHelperLatestDate($B10,Trigger)</f>
-        <v>42045</v>
+        <v>42048</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="149" t="str">
         <f>Deposits!J12</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_0035e#0001</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B11)</f>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="D11" s="6">
         <f>_xll.qlRateHelperQuoteValue($B11,Trigger)</f>
-        <v>6.5239666699999999E-3</v>
+        <v>6.5358666700000003E-3</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="74" t="b">
@@ -2954,11 +2954,11 @@
       </c>
       <c r="I11" s="4">
         <f>_xll.qlRateHelperEarliestDate($B11,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J11" s="3">
         <f>_xll.qlRateHelperLatestDate($B11,Trigger)</f>
-        <v>42073</v>
+        <v>42076</v>
       </c>
       <c r="K11" s="1">
         <v>30</v>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="D12" s="6">
         <f>_xll.qlRateHelperQuoteValue($B12,Trigger)</f>
-        <v>6.9638E-3</v>
+        <v>7.0043999999999992E-3</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="74" t="b">
@@ -2993,11 +2993,11 @@
       </c>
       <c r="I12" s="4">
         <f>_xll.qlRateHelperEarliestDate($B12,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J12" s="3">
         <f>_xll.qlRateHelperLatestDate($B12,Trigger)</f>
-        <v>42104</v>
+        <v>42107</v>
       </c>
       <c r="K12" s="1">
         <v>40</v>
@@ -3010,7 +3010,7 @@
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="149" t="str">
         <f>Deposits!J14</f>
-        <v>obj_00360#0001</v>
+        <v>obj_00363#0001</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B13)</f>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D13" s="6">
         <f>_xll.qlRateHelperQuoteValue($B13,Trigger)</f>
-        <v>7.4849967200000004E-3</v>
+        <v>7.5338098399999999E-3</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="74" t="b">
@@ -3032,11 +3032,11 @@
       </c>
       <c r="I13" s="4">
         <f>_xll.qlRateHelperEarliestDate($B13,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J13" s="3">
         <f>_xll.qlRateHelperLatestDate($B13,Trigger)</f>
-        <v>42135</v>
+        <v>42137</v>
       </c>
       <c r="K13" s="1">
         <v>50</v>
@@ -3049,7 +3049,7 @@
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="149" t="str">
         <f>Deposits!J15</f>
-        <v>obj_0035a#0001</v>
+        <v>obj_00361#0001</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B14)</f>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="D14" s="6">
         <f>_xll.qlRateHelperQuoteValue($B14,Trigger)</f>
-        <v>8.0409398899999995E-3</v>
+        <v>8.080866669999999E-3</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="74" t="b">
@@ -3071,11 +3071,11 @@
       </c>
       <c r="I14" s="4">
         <f>_xll.qlRateHelperEarliestDate($B14,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J14" s="3">
         <f>_xll.qlRateHelperLatestDate($B14,Trigger)</f>
-        <v>42165</v>
+        <v>42170</v>
       </c>
       <c r="K14" s="1">
         <v>60</v>
@@ -3088,7 +3088,7 @@
     <row r="15" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="149" t="str">
         <f>Deposits!J16</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_00360#0001</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B15)</f>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="D15" s="6">
         <f>_xll.qlRateHelperQuoteValue($B15,Trigger)</f>
-        <v>8.5447633899999997E-3</v>
+        <v>8.6102764999999998E-3</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="74" t="b">
@@ -3110,17 +3110,17 @@
       </c>
       <c r="I15" s="4">
         <f>_xll.qlRateHelperEarliestDate($B15,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J15" s="3">
         <f>_xll.qlRateHelperLatestDate($B15,Trigger)</f>
-        <v>42195</v>
+        <v>42198</v>
       </c>
     </row>
     <row r="16" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="149" t="str">
         <f>Deposits!J17</f>
-        <v>obj_00361#0001</v>
+        <v>obj_0035b#0001</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B16)</f>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="D16" s="6">
         <f>_xll.qlRateHelperQuoteValue($B16,Trigger)</f>
-        <v>9.0833333300000003E-3</v>
+        <v>9.1926273200000005E-3</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="74" t="b">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="I16" s="4">
         <f>_xll.qlRateHelperEarliestDate($B16,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J16" s="3">
         <f>_xll.qlRateHelperLatestDate($B16,Trigger)</f>
-        <v>42226</v>
+        <v>42229</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="D17" s="6">
         <f>_xll.qlRateHelperQuoteValue($B17,Trigger)</f>
-        <v>9.62190328E-3</v>
+        <v>9.7043901599999996E-3</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="74" t="b">
@@ -3174,17 +3174,17 @@
       </c>
       <c r="I17" s="4">
         <f>_xll.qlRateHelperEarliestDate($B17,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J17" s="3">
         <f>_xll.qlRateHelperLatestDate($B17,Trigger)</f>
-        <v>42257</v>
+        <v>42261</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="149" t="str">
         <f>Deposits!J19</f>
-        <v>obj_0034f#0001</v>
+        <v>obj_00353#0001</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B18)</f>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D18" s="6">
         <f>_xll.qlRateHelperQuoteValue($B18,Trigger)</f>
-        <v>1.01431E-2</v>
+        <v>1.0233799999999999E-2</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="74" t="b">
@@ -3206,11 +3206,11 @@
       </c>
       <c r="I18" s="4">
         <f>_xll.qlRateHelperEarliestDate($B18,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J18" s="3">
         <f>_xll.qlRateHelperLatestDate($B18,Trigger)</f>
-        <v>42289</v>
+        <v>42290</v>
       </c>
       <c r="K18" s="1">
         <v>70</v>
@@ -3223,7 +3223,7 @@
     <row r="19" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="149" t="str">
         <f>Deposits!J20</f>
-        <v>obj_003b4#0003</v>
+        <v>obj_003b4#0001</v>
       </c>
       <c r="C19" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B19)</f>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="D19" s="6">
         <f>_xll.qlRateHelperQuoteValue($B19,Trigger)</f>
-        <v>8.0756863400000007E-3</v>
+        <v>8.1161606599999998E-3</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="74" t="b">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="I19" s="4">
         <f>_xll.qlRateHelperEarliestDate($B19,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J19" s="3">
         <f>_xll.qlRateHelperLatestDate($B19,Trigger)</f>
@@ -3258,15 +3258,15 @@
       </c>
       <c r="B20" s="150" t="str">
         <f>Futures!H3</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_00367#0002</v>
       </c>
       <c r="C20" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B20)</f>
-        <v>GBPFUT3MV4_Quote</v>
-      </c>
-      <c r="D20" s="147" t="e">
+        <v>GBPFUT3MV4_HST_CLOSE_Quote</v>
+      </c>
+      <c r="D20" s="147">
         <f>_xll.qlRateHelperQuoteValue($B20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>99.47</v>
       </c>
       <c r="E20" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B20,Trigger)</f>
@@ -3297,15 +3297,15 @@
       </c>
       <c r="B21" s="149" t="str">
         <f>Futures!H4</f>
-        <v>obj_00389#0001</v>
+        <v>obj_003a3#0004</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B21)</f>
-        <v>GBPFUT3MX4_Quote</v>
-      </c>
-      <c r="D21" s="16" t="e">
+        <v>GBPFUT3MX4_HST_CLOSE_Quote</v>
+      </c>
+      <c r="D21" s="16">
         <f>_xll.qlRateHelperQuoteValue($B21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>99.42</v>
       </c>
       <c r="E21" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B21,Trigger)</f>
@@ -3336,15 +3336,15 @@
       </c>
       <c r="B22" s="149" t="str">
         <f>Futures!H5</f>
-        <v>obj_00371#0001</v>
+        <v>obj_0039e#0004</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B22)</f>
-        <v>GBPFUT3MZ4_Quote</v>
+        <v>GBPFUT3MZ4_HST_CLOSE_Quote</v>
       </c>
       <c r="D22" s="16">
         <f>_xll.qlRateHelperQuoteValue($B22,Trigger)</f>
-        <v>99.39500000000001</v>
+        <v>99.39</v>
       </c>
       <c r="E22" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B22,Trigger)</f>
@@ -3375,11 +3375,11 @@
       </c>
       <c r="B23" s="149" t="str">
         <f>Futures!H6</f>
-        <v>obj_00373#0001</v>
+        <v>obj_00390#0004</v>
       </c>
       <c r="C23" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B23)</f>
-        <v>GBPFUT3MF5_Quote</v>
+        <v>GBPFUT3MF5_HST_CLOSE_Quote</v>
       </c>
       <c r="D23" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B23,Trigger)</f>
@@ -3414,11 +3414,11 @@
       </c>
       <c r="B24" s="149" t="str">
         <f>Futures!H7</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_003a2#0004</v>
       </c>
       <c r="C24" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B24)</f>
-        <v>GBPFUT3MG5_Quote</v>
+        <v>GBPFUT3MG5_HST_CLOSE_Quote</v>
       </c>
       <c r="D24" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B24,Trigger)</f>
@@ -3453,15 +3453,15 @@
       </c>
       <c r="B25" s="149" t="str">
         <f>Futures!H8</f>
-        <v>obj_00392#0001</v>
+        <v>obj_00392#0004</v>
       </c>
       <c r="C25" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B25)</f>
-        <v>GBPFUT3MH5_Quote</v>
+        <v>GBPFUT3MH5_HST_CLOSE_Quote</v>
       </c>
       <c r="D25" s="16">
         <f>_xll.qlRateHelperQuoteValue($B25,Trigger)</f>
-        <v>99.265000000000001</v>
+        <v>99.25</v>
       </c>
       <c r="E25" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B25,Trigger)</f>
@@ -3492,11 +3492,11 @@
       </c>
       <c r="B26" s="149" t="str">
         <f>Futures!H9</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00398#0004</v>
       </c>
       <c r="C26" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B26)</f>
-        <v>GBPFUT3MJ5_Quote</v>
+        <v>GBPFUT3MJ5_HST_CLOSE_Quote</v>
       </c>
       <c r="D26" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B26,Trigger)</f>
@@ -3531,11 +3531,11 @@
       </c>
       <c r="B27" s="149" t="str">
         <f>Futures!H10</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_003a8#0004</v>
       </c>
       <c r="C27" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B27)</f>
-        <v>GBPFUT3MK5_Quote</v>
+        <v>GBPFUT3MK5_HST_CLOSE_Quote</v>
       </c>
       <c r="D27" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B27,Trigger)</f>
@@ -3570,15 +3570,15 @@
       </c>
       <c r="B28" s="149" t="str">
         <f>Futures!H11</f>
-        <v>obj_00372#0001</v>
+        <v>obj_0038b#0004</v>
       </c>
       <c r="C28" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B28)</f>
-        <v>GBPFUT3MM5_Quote</v>
+        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
       </c>
       <c r="D28" s="16">
         <f>_xll.qlRateHelperQuoteValue($B28,Trigger)</f>
-        <v>99.125</v>
+        <v>99.094999999999999</v>
       </c>
       <c r="E28" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B28,Trigger)</f>
@@ -3610,11 +3610,11 @@
       </c>
       <c r="B29" s="149" t="str">
         <f>Futures!H12</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_003a5#0004</v>
       </c>
       <c r="C29" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B29)</f>
-        <v>GBPFUT3MN5_Quote</v>
+        <v>GBPFUT3MN5_HST_CLOSE_Quote</v>
       </c>
       <c r="D29" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B29,Trigger)</f>
@@ -3650,11 +3650,11 @@
       </c>
       <c r="B30" s="149" t="str">
         <f>Futures!H13</f>
-        <v>obj_0039e#0001</v>
+        <v>obj_00386#0004</v>
       </c>
       <c r="C30" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B30)</f>
-        <v>GBPFUT3MQ5_Quote</v>
+        <v>GBPFUT3MQ5_HST_CLOSE_Quote</v>
       </c>
       <c r="D30" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B30,Trigger)</f>
@@ -3690,15 +3690,15 @@
       </c>
       <c r="B31" s="149" t="str">
         <f>Futures!H14</f>
-        <v>obj_00393#0001</v>
+        <v>obj_003ae#0004</v>
       </c>
       <c r="C31" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B31)</f>
-        <v>GBPFUT3MU5_Quote</v>
+        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
       </c>
       <c r="D31" s="16">
         <f>_xll.qlRateHelperQuoteValue($B31,Trigger)</f>
-        <v>98.965000000000003</v>
+        <v>98.93</v>
       </c>
       <c r="E31" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B31,Trigger)</f>
@@ -3730,15 +3730,15 @@
       </c>
       <c r="B32" s="149" t="str">
         <f>Futures!H15</f>
-        <v>obj_00395#0001</v>
+        <v>obj_00375#0004</v>
       </c>
       <c r="C32" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B32)</f>
-        <v>GBPFUT3MZ5_Quote</v>
+        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
       </c>
       <c r="D32" s="16">
         <f>_xll.qlRateHelperQuoteValue($B32,Trigger)</f>
-        <v>98.805000000000007</v>
+        <v>98.765000000000001</v>
       </c>
       <c r="E32" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B32,Trigger)</f>
@@ -3771,15 +3771,15 @@
       </c>
       <c r="B33" s="149" t="str">
         <f>Futures!H16</f>
-        <v>obj_0036e#0001</v>
+        <v>obj_00370#0004</v>
       </c>
       <c r="C33" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B33)</f>
-        <v>GBPFUT3MH6_Quote</v>
+        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
       </c>
       <c r="D33" s="16">
         <f>_xll.qlRateHelperQuoteValue($B33,Trigger)</f>
-        <v>98.64500000000001</v>
+        <v>98.61</v>
       </c>
       <c r="E33" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B33,Trigger)</f>
@@ -3812,15 +3812,15 @@
       </c>
       <c r="B34" s="149" t="str">
         <f>Futures!H17</f>
-        <v>obj_003ab#0001</v>
+        <v>obj_0036d#0004</v>
       </c>
       <c r="C34" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B34)</f>
-        <v>GBPFUT3MM6_Quote</v>
+        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
       </c>
       <c r="D34" s="16">
         <f>_xll.qlRateHelperQuoteValue($B34,Trigger)</f>
-        <v>98.495000000000005</v>
+        <v>98.454999999999998</v>
       </c>
       <c r="E34" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B34,Trigger)</f>
@@ -3853,15 +3853,15 @@
       </c>
       <c r="B35" s="149" t="str">
         <f>Futures!H18</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00391#0004</v>
       </c>
       <c r="C35" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B35)</f>
-        <v>GBPFUT3MU6_Quote</v>
+        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
       </c>
       <c r="D35" s="16">
         <f>_xll.qlRateHelperQuoteValue($B35,Trigger)</f>
-        <v>98.35499999999999</v>
+        <v>98.31</v>
       </c>
       <c r="E35" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B35,Trigger)</f>
@@ -3894,15 +3894,15 @@
       </c>
       <c r="B36" s="149" t="str">
         <f>Futures!H19</f>
-        <v>obj_0036d#0001</v>
+        <v>obj_00365#0004</v>
       </c>
       <c r="C36" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B36)</f>
-        <v>GBPFUT3MZ6_Quote</v>
+        <v>GBPFUT3MZ6_HST_CLOSE_Quote</v>
       </c>
       <c r="D36" s="16">
         <f>_xll.qlRateHelperQuoteValue($B36,Trigger)</f>
-        <v>98.215000000000003</v>
+        <v>98.174999999999997</v>
       </c>
       <c r="E36" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B36,Trigger)</f>
@@ -3935,15 +3935,15 @@
       </c>
       <c r="B37" s="149" t="str">
         <f>Futures!H20</f>
-        <v>obj_003b0#0001</v>
+        <v>obj_003b0#0004</v>
       </c>
       <c r="C37" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B37)</f>
-        <v>GBPFUT3MH7_Quote</v>
+        <v>GBPFUT3MH7_HST_CLOSE_Quote</v>
       </c>
       <c r="D37" s="16">
         <f>_xll.qlRateHelperQuoteValue($B37,Trigger)</f>
-        <v>98.115000000000009</v>
+        <v>98.07</v>
       </c>
       <c r="E37" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B37,Trigger)</f>
@@ -3976,15 +3976,15 @@
       </c>
       <c r="B38" s="149" t="str">
         <f>Futures!H21</f>
-        <v>obj_003a2#0001</v>
+        <v>obj_003b3#0004</v>
       </c>
       <c r="C38" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B38)</f>
-        <v>GBPFUT3MM7_Quote</v>
+        <v>GBPFUT3MM7_HST_CLOSE_Quote</v>
       </c>
       <c r="D38" s="16">
         <f>_xll.qlRateHelperQuoteValue($B38,Trigger)</f>
-        <v>98.015000000000001</v>
+        <v>97.97</v>
       </c>
       <c r="E38" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B38,Trigger)</f>
@@ -4017,15 +4017,15 @@
       </c>
       <c r="B39" s="149" t="str">
         <f>Futures!H22</f>
-        <v>obj_00396#0001</v>
+        <v>obj_0037f#0004</v>
       </c>
       <c r="C39" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B39)</f>
-        <v>GBPFUT3MU7_Quote</v>
+        <v>GBPFUT3MU7_HST_CLOSE_Quote</v>
       </c>
       <c r="D39" s="16">
         <f>_xll.qlRateHelperQuoteValue($B39,Trigger)</f>
-        <v>97.935000000000002</v>
+        <v>97.89</v>
       </c>
       <c r="E39" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B39,Trigger)</f>
@@ -4058,15 +4058,15 @@
       </c>
       <c r="B40" s="149" t="str">
         <f>Futures!H23</f>
-        <v>obj_0038e#0001</v>
+        <v>obj_0037e#0004</v>
       </c>
       <c r="C40" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B40)</f>
-        <v>GBPFUT3MZ7_Quote</v>
+        <v>GBPFUT3MZ7_HST_CLOSE_Quote</v>
       </c>
       <c r="D40" s="16">
         <f>_xll.qlRateHelperQuoteValue($B40,Trigger)</f>
-        <v>97.85499999999999</v>
+        <v>97.814999999999998</v>
       </c>
       <c r="E40" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B40,Trigger)</f>
@@ -4099,15 +4099,15 @@
       </c>
       <c r="B41" s="149" t="str">
         <f>Futures!H24</f>
-        <v>obj_00379#0001</v>
+        <v>obj_00388#0004</v>
       </c>
       <c r="C41" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B41)</f>
-        <v>GBPFUT3MH8_Quote</v>
+        <v>GBPFUT3MH8_HST_CLOSE_Quote</v>
       </c>
       <c r="D41" s="16">
         <f>_xll.qlRateHelperQuoteValue($B41,Trigger)</f>
-        <v>97.789999999999992</v>
+        <v>97.745000000000005</v>
       </c>
       <c r="E41" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B41,Trigger)</f>
@@ -4140,15 +4140,15 @@
       </c>
       <c r="B42" s="149" t="str">
         <f>Futures!H25</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_00380#0004</v>
       </c>
       <c r="C42" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B42)</f>
-        <v>GBPFUT3MM8_Quote</v>
+        <v>GBPFUT3MM8_HST_CLOSE_Quote</v>
       </c>
       <c r="D42" s="16">
         <f>_xll.qlRateHelperQuoteValue($B42,Trigger)</f>
-        <v>97.72</v>
+        <v>97.68</v>
       </c>
       <c r="E42" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B42,Trigger)</f>
@@ -4181,15 +4181,15 @@
       </c>
       <c r="B43" s="149" t="str">
         <f>Futures!H26</f>
-        <v>obj_00380#0001</v>
+        <v>obj_0039f#0004</v>
       </c>
       <c r="C43" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B43)</f>
-        <v>GBPFUT3MU8_Quote</v>
+        <v>GBPFUT3MU8_HST_CLOSE_Quote</v>
       </c>
       <c r="D43" s="16">
         <f>_xll.qlRateHelperQuoteValue($B43,Trigger)</f>
-        <v>97.65</v>
+        <v>97.62</v>
       </c>
       <c r="E43" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B43,Trigger)</f>
@@ -4222,15 +4222,15 @@
       </c>
       <c r="B44" s="149" t="str">
         <f>Futures!H27</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00374#0004</v>
       </c>
       <c r="C44" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B44)</f>
-        <v>GBPFUT3MZ8_Quote</v>
+        <v>GBPFUT3MZ8_HST_CLOSE_Quote</v>
       </c>
       <c r="D44" s="16">
         <f>_xll.qlRateHelperQuoteValue($B44,Trigger)</f>
-        <v>97.594999999999999</v>
+        <v>97.56</v>
       </c>
       <c r="E44" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B44,Trigger)</f>
@@ -4263,15 +4263,15 @@
       </c>
       <c r="B45" s="149" t="str">
         <f>Futures!H28</f>
-        <v>obj_00399#0001</v>
+        <v>obj_003aa#0004</v>
       </c>
       <c r="C45" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B45)</f>
-        <v>GBPFUT3MH9_Quote</v>
+        <v>GBPFUT3MH9_HST_CLOSE_Quote</v>
       </c>
       <c r="D45" s="16">
         <f>_xll.qlRateHelperQuoteValue($B45,Trigger)</f>
-        <v>97.55</v>
+        <v>97.51</v>
       </c>
       <c r="E45" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B45,Trigger)</f>
@@ -4304,15 +4304,15 @@
       </c>
       <c r="B46" s="149" t="str">
         <f>Futures!H29</f>
-        <v>obj_003a7#0001</v>
+        <v>obj_003a1#0004</v>
       </c>
       <c r="C46" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B46)</f>
-        <v>GBPFUT3MM9_Quote</v>
+        <v>GBPFUT3MM9_HST_CLOSE_Quote</v>
       </c>
       <c r="D46" s="16">
         <f>_xll.qlRateHelperQuoteValue($B46,Trigger)</f>
-        <v>97.509999999999991</v>
+        <v>97.46</v>
       </c>
       <c r="E46" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B46,Trigger)</f>
@@ -4345,15 +4345,15 @@
       </c>
       <c r="B47" s="149" t="str">
         <f>Futures!H30</f>
-        <v>obj_00378#0001</v>
+        <v>obj_00383#0004</v>
       </c>
       <c r="C47" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B47)</f>
-        <v>GBPFUT3MU9_Quote</v>
+        <v>GBPFUT3MU9_HST_CLOSE_Quote</v>
       </c>
       <c r="D47" s="16">
         <f>_xll.qlRateHelperQuoteValue($B47,Trigger)</f>
-        <v>97.47</v>
+        <v>97.415000000000006</v>
       </c>
       <c r="E47" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B47,Trigger)</f>
@@ -4386,15 +4386,15 @@
       </c>
       <c r="B48" s="149" t="str">
         <f>Futures!H31</f>
-        <v>obj_00387#0001</v>
+        <v>obj_00384#0004</v>
       </c>
       <c r="C48" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B48)</f>
-        <v>GBPFUT3MZ9_Quote</v>
+        <v>GBPFUT3MZ9_HST_CLOSE_Quote</v>
       </c>
       <c r="D48" s="16">
         <f>_xll.qlRateHelperQuoteValue($B48,Trigger)</f>
-        <v>97.435000000000002</v>
+        <v>97.38</v>
       </c>
       <c r="E48" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B48,Trigger)</f>
@@ -4425,15 +4425,15 @@
       </c>
       <c r="B49" s="149" t="str">
         <f>Futures!H32</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_00377#0004</v>
       </c>
       <c r="C49" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B49)</f>
-        <v>GBPFUT3MH0_Quote</v>
+        <v>GBPFUT3MH0_HST_CLOSE_Quote</v>
       </c>
       <c r="D49" s="16">
         <f>_xll.qlRateHelperQuoteValue($B49,Trigger)</f>
-        <v>97.414999999999992</v>
+        <v>97.344999999999999</v>
       </c>
       <c r="E49" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B49,Trigger)</f>
@@ -4464,15 +4464,15 @@
       </c>
       <c r="B50" s="149" t="str">
         <f>Futures!H33</f>
-        <v>obj_00384#0001</v>
+        <v>obj_00368#0004</v>
       </c>
       <c r="C50" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B50)</f>
-        <v>GBPFUT3MM0_Quote</v>
-      </c>
-      <c r="D50" s="16" t="e">
+        <v>GBPFUT3MM0_HST_CLOSE_Quote</v>
+      </c>
+      <c r="D50" s="16">
         <f>_xll.qlRateHelperQuoteValue($B50,Trigger)</f>
-        <v>#NUM!</v>
+        <v>97.35</v>
       </c>
       <c r="E50" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B50,Trigger)</f>
@@ -4503,15 +4503,15 @@
       </c>
       <c r="B51" s="149" t="str">
         <f>Futures!H34</f>
-        <v>obj_00370#0001</v>
+        <v>obj_0039a#0004</v>
       </c>
       <c r="C51" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B51)</f>
-        <v>GBPFUT3MU0_Quote</v>
-      </c>
-      <c r="D51" s="16" t="e">
+        <v>GBPFUT3MU0_HST_CLOSE_Quote</v>
+      </c>
+      <c r="D51" s="16">
         <f>_xll.qlRateHelperQuoteValue($B51,Trigger)</f>
-        <v>#NUM!</v>
+        <v>97.35</v>
       </c>
       <c r="E51" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B51,Trigger)</f>
@@ -4542,11 +4542,11 @@
       </c>
       <c r="B52" s="149" t="str">
         <f>Futures!H35</f>
-        <v>obj_003b2#0001</v>
+        <v>obj_0036e#0004</v>
       </c>
       <c r="C52" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B52)</f>
-        <v>GBPFUT3MZ0_Quote</v>
+        <v>GBPFUT3MZ0_HST_CLOSE_Quote</v>
       </c>
       <c r="D52" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B52,Trigger)</f>
@@ -4581,11 +4581,11 @@
       </c>
       <c r="B53" s="149" t="str">
         <f>Futures!H36</f>
-        <v>obj_003b3#0001</v>
+        <v>obj_00379#0004</v>
       </c>
       <c r="C53" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B53)</f>
-        <v>GBPFUT3MH1_Quote</v>
+        <v>GBPFUT3MH1_HST_CLOSE_Quote</v>
       </c>
       <c r="D53" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B53,Trigger)</f>
@@ -4620,11 +4620,11 @@
       </c>
       <c r="B54" s="149" t="str">
         <f>Futures!H37</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_003a9#0004</v>
       </c>
       <c r="C54" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B54)</f>
-        <v>GBPFUT3MM1_Quote</v>
+        <v>GBPFUT3MM1_HST_CLOSE_Quote</v>
       </c>
       <c r="D54" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B54,Trigger)</f>
@@ -4659,11 +4659,11 @@
       </c>
       <c r="B55" s="149" t="str">
         <f>Futures!H38</f>
-        <v>obj_003a8#0001</v>
+        <v>obj_0038e#0004</v>
       </c>
       <c r="C55" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B55)</f>
-        <v>GBPFUT3MU1_Quote</v>
+        <v>GBPFUT3MU1_HST_CLOSE_Quote</v>
       </c>
       <c r="D55" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B55,Trigger)</f>
@@ -4698,11 +4698,11 @@
       </c>
       <c r="B56" s="149" t="str">
         <f>Futures!H39</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_0036b#0004</v>
       </c>
       <c r="C56" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B56)</f>
-        <v>GBPFUT3MZ1_Quote</v>
+        <v>GBPFUT3MZ1_HST_CLOSE_Quote</v>
       </c>
       <c r="D56" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B56,Trigger)</f>
@@ -4737,11 +4737,11 @@
       </c>
       <c r="B57" s="149" t="str">
         <f>Futures!H40</f>
-        <v>obj_003af#0001</v>
+        <v>obj_003a6#0004</v>
       </c>
       <c r="C57" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B57)</f>
-        <v>GBPFUT3MH2_Quote</v>
+        <v>GBPFUT3MH2_HST_CLOSE_Quote</v>
       </c>
       <c r="D57" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B57,Trigger)</f>
@@ -4776,11 +4776,11 @@
       </c>
       <c r="B58" s="149" t="str">
         <f>Futures!H41</f>
-        <v>obj_003ad#0001</v>
+        <v>obj_00381#0004</v>
       </c>
       <c r="C58" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B58)</f>
-        <v>GBPFUT3MM2_Quote</v>
+        <v>GBPFUT3MM2_HST_CLOSE_Quote</v>
       </c>
       <c r="D58" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B58,Trigger)</f>
@@ -4815,11 +4815,11 @@
       </c>
       <c r="B59" s="149" t="str">
         <f>Futures!H42</f>
-        <v>obj_003a9#0001</v>
+        <v>obj_003ab#0004</v>
       </c>
       <c r="C59" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B59)</f>
-        <v>GBPFUT3MU2_Quote</v>
+        <v>GBPFUT3MU2_HST_CLOSE_Quote</v>
       </c>
       <c r="D59" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B59,Trigger)</f>
@@ -4854,11 +4854,11 @@
       </c>
       <c r="B60" s="149" t="str">
         <f>Futures!H43</f>
-        <v>obj_003a5#0001</v>
+        <v>obj_00399#0004</v>
       </c>
       <c r="C60" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B60)</f>
-        <v>GBPFUT3MZ2_Quote</v>
+        <v>GBPFUT3MZ2_HST_CLOSE_Quote</v>
       </c>
       <c r="D60" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B60,Trigger)</f>
@@ -4893,11 +4893,11 @@
       </c>
       <c r="B61" s="149" t="str">
         <f>Futures!H44</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_003b2#0004</v>
       </c>
       <c r="C61" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B61)</f>
-        <v>GBPFUT3MH3_Quote</v>
+        <v>GBPFUT3MH3_HST_CLOSE_Quote</v>
       </c>
       <c r="D61" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B61,Trigger)</f>
@@ -4931,7 +4931,7 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="150" t="str">
         <f>Swaps!K6</f>
-        <v>obj_00381#0001</v>
+        <v>obj_0038c#0001</v>
       </c>
       <c r="C62" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B62)</f>
@@ -4956,17 +4956,17 @@
       </c>
       <c r="I62" s="11">
         <f>_xll.qlRateHelperEarliestDate($B62,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J62" s="10">
         <f>_xll.qlRateHelperLatestDate($B62,Trigger)</f>
-        <v>42289</v>
+        <v>42290</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="149" t="str">
         <f>Swaps!K7</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00369#0001</v>
       </c>
       <c r="C63" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B63)</f>
@@ -4991,17 +4991,17 @@
       </c>
       <c r="I63" s="4">
         <f>_xll.qlRateHelperEarliestDate($B63,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J63" s="3">
         <f>_xll.qlRateHelperLatestDate($B63,Trigger)</f>
-        <v>42380</v>
+        <v>42382</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" s="149" t="str">
         <f>Swaps!K8</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_00385#0001</v>
       </c>
       <c r="C64" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B64)</f>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="D64" s="6">
         <f>_xll.qlRateHelperQuoteValue($B64,Trigger)</f>
-        <v>9.6200000000000001E-3</v>
+        <v>9.6399999999999993E-3</v>
       </c>
       <c r="E64" s="6">
         <f>_xll.qlSwapRateHelperSpread($B64,Trigger)</f>
@@ -5026,17 +5026,17 @@
       </c>
       <c r="I64" s="4">
         <f>_xll.qlRateHelperEarliestDate($B64,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J64" s="3">
         <f>_xll.qlRateHelperLatestDate($B64,Trigger)</f>
-        <v>42471</v>
+        <v>42473</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="149" t="str">
         <f>Swaps!K9</f>
-        <v>obj_00388#0001</v>
+        <v>obj_00389#0001</v>
       </c>
       <c r="C65" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B65)</f>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="I65" s="4">
         <f>_xll.qlRateHelperEarliestDate($B65,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J65" s="3">
         <f>_xll.qlRateHelperLatestDate($B65,Trigger)</f>
-        <v>42562</v>
+        <v>42564</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="149" t="str">
         <f>Swaps!K10</f>
-        <v>obj_003b1#0001</v>
+        <v>obj_00397#0001</v>
       </c>
       <c r="C66" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B66)</f>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="D66" s="6">
         <f>_xll.qlRateHelperQuoteValue($B66,Trigger)</f>
-        <v>1.107E-2</v>
+        <v>1.111E-2</v>
       </c>
       <c r="E66" s="6">
         <f>_xll.qlSwapRateHelperSpread($B66,Trigger)</f>
@@ -5096,17 +5096,17 @@
       </c>
       <c r="I66" s="4">
         <f>_xll.qlRateHelperEarliestDate($B66,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J66" s="3">
         <f>_xll.qlRateHelperLatestDate($B66,Trigger)</f>
-        <v>42653</v>
+        <v>42656</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="149" t="str">
         <f>Swaps!K11</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_00372#0001</v>
       </c>
       <c r="C67" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B67)</f>
@@ -5131,17 +5131,17 @@
       </c>
       <c r="I67" s="4">
         <f>_xll.qlRateHelperEarliestDate($B67,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J67" s="3">
         <f>_xll.qlRateHelperLatestDate($B67,Trigger)</f>
-        <v>43018</v>
+        <v>43021</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="149" t="str">
         <f>Swaps!K12</f>
-        <v>obj_00391#0001</v>
+        <v>obj_003a4#0001</v>
       </c>
       <c r="C68" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B68)</f>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="D68" s="6">
         <f>_xll.qlRateHelperQuoteValue($B68,Trigger)</f>
-        <v>1.5870000000000002E-2</v>
+        <v>1.5819999999999997E-2</v>
       </c>
       <c r="E68" s="6">
         <f>_xll.qlSwapRateHelperSpread($B68,Trigger)</f>
@@ -5166,17 +5166,17 @@
       </c>
       <c r="I68" s="4">
         <f>_xll.qlRateHelperEarliestDate($B68,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J68" s="3">
         <f>_xll.qlRateHelperLatestDate($B68,Trigger)</f>
-        <v>43383</v>
+        <v>43388</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="149" t="str">
         <f>Swaps!K13</f>
-        <v>obj_0039a#0001</v>
+        <v>obj_00396#0001</v>
       </c>
       <c r="C69" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B69)</f>
@@ -5184,7 +5184,7 @@
       </c>
       <c r="D69" s="6">
         <f>_xll.qlRateHelperQuoteValue($B69,Trigger)</f>
-        <v>1.755E-2</v>
+        <v>1.746E-2</v>
       </c>
       <c r="E69" s="6">
         <f>_xll.qlSwapRateHelperSpread($B69,Trigger)</f>
@@ -5201,17 +5201,17 @@
       </c>
       <c r="I69" s="4">
         <f>_xll.qlRateHelperEarliestDate($B69,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J69" s="3">
         <f>_xll.qlRateHelperLatestDate($B69,Trigger)</f>
-        <v>43748</v>
+        <v>43752</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="149" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00385#0001</v>
+        <v>obj_00373#0001</v>
       </c>
       <c r="C70" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B70)</f>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="D70" s="6">
         <f>_xll.qlRateHelperQuoteValue($B70,Trigger)</f>
-        <v>1.8970000000000001E-2</v>
+        <v>1.8860000000000002E-2</v>
       </c>
       <c r="E70" s="6">
         <f>_xll.qlSwapRateHelperSpread($B70,Trigger)</f>
@@ -5236,17 +5236,17 @@
       </c>
       <c r="I70" s="4">
         <f>_xll.qlRateHelperEarliestDate($B70,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J70" s="3">
         <f>_xll.qlRateHelperLatestDate($B70,Trigger)</f>
-        <v>44116</v>
+        <v>44117</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="149" t="str">
         <f>Swaps!K15</f>
-        <v>obj_00390#0001</v>
+        <v>obj_003a0#0001</v>
       </c>
       <c r="C71" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B71)</f>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="D71" s="6">
         <f>_xll.qlRateHelperQuoteValue($B71,Trigger)</f>
-        <v>2.017E-2</v>
+        <v>2.0049999999999998E-2</v>
       </c>
       <c r="E71" s="6">
         <f>_xll.qlSwapRateHelperSpread($B71,Trigger)</f>
@@ -5271,18 +5271,18 @@
       </c>
       <c r="I71" s="4">
         <f>_xll.qlRateHelperEarliestDate($B71,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J71" s="3">
         <f>_xll.qlRateHelperLatestDate($B71,Trigger)</f>
-        <v>44480</v>
+        <v>44482</v>
       </c>
       <c r="L71" s="9"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="149" t="str">
         <f>Swaps!K16</f>
-        <v>obj_0036b#0001</v>
+        <v>obj_003a7#0001</v>
       </c>
       <c r="C72" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B72)</f>
@@ -5290,7 +5290,7 @@
       </c>
       <c r="D72" s="6">
         <f>_xll.qlRateHelperQuoteValue($B72,Trigger)</f>
-        <v>2.1219999999999999E-2</v>
+        <v>2.1090000000000001E-2</v>
       </c>
       <c r="E72" s="6">
         <f>_xll.qlSwapRateHelperSpread($B72,Trigger)</f>
@@ -5307,18 +5307,18 @@
       </c>
       <c r="I72" s="4">
         <f>_xll.qlRateHelperEarliestDate($B72,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J72" s="3">
         <f>_xll.qlRateHelperLatestDate($B72,Trigger)</f>
-        <v>44844</v>
+        <v>44847</v>
       </c>
       <c r="L72" s="9"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="149" t="str">
         <f>Swaps!K17</f>
-        <v>obj_00366#0001</v>
+        <v>obj_003ac#0001</v>
       </c>
       <c r="C73" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B73)</f>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="D73" s="6">
         <f>_xll.qlRateHelperQuoteValue($B73,Trigger)</f>
-        <v>2.213E-2</v>
+        <v>2.2000000000000002E-2</v>
       </c>
       <c r="E73" s="6">
         <f>_xll.qlSwapRateHelperSpread($B73,Trigger)</f>
@@ -5343,18 +5343,18 @@
       </c>
       <c r="I73" s="4">
         <f>_xll.qlRateHelperEarliestDate($B73,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J73" s="3">
         <f>_xll.qlRateHelperLatestDate($B73,Trigger)</f>
-        <v>45209</v>
+        <v>45212</v>
       </c>
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B74" s="149" t="str">
         <f>Swaps!K18</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_0037b#0001</v>
       </c>
       <c r="C74" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B74)</f>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="D74" s="6">
         <f>_xll.qlRateHelperQuoteValue($B74,Trigger)</f>
-        <v>2.2930000000000002E-2</v>
+        <v>2.2800000000000001E-2</v>
       </c>
       <c r="E74" s="6">
         <f>_xll.qlSwapRateHelperSpread($B74,Trigger)</f>
@@ -5379,18 +5379,18 @@
       </c>
       <c r="I74" s="4">
         <f>_xll.qlRateHelperEarliestDate($B74,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J74" s="3">
         <f>_xll.qlRateHelperLatestDate($B74,Trigger)</f>
-        <v>45575</v>
+        <v>45579</v>
       </c>
       <c r="L74" s="9"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B75" s="149" t="str">
         <f>Swaps!K19</f>
-        <v>obj_003a6#0001</v>
+        <v>obj_0039d#0001</v>
       </c>
       <c r="C75" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B75)</f>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="D75" s="6">
         <f>_xll.qlRateHelperQuoteValue($B75,Trigger)</f>
-        <v>2.3620000000000002E-2</v>
+        <v>2.3479999999999997E-2</v>
       </c>
       <c r="E75" s="6">
         <f>_xll.qlSwapRateHelperSpread($B75,Trigger)</f>
@@ -5415,18 +5415,18 @@
       </c>
       <c r="I75" s="4">
         <f>_xll.qlRateHelperEarliestDate($B75,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J75" s="3">
         <f>_xll.qlRateHelperLatestDate($B75,Trigger)</f>
-        <v>45940</v>
+        <v>45943</v>
       </c>
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B76" s="149" t="str">
         <f>Swaps!K20</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_0037d#0001</v>
       </c>
       <c r="C76" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B76)</f>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="D76" s="6">
         <f>_xll.qlRateHelperQuoteValue($B76,Trigger)</f>
-        <v>2.4219999999999998E-2</v>
+        <v>2.4080000000000004E-2</v>
       </c>
       <c r="E76" s="6">
         <f>_xll.qlSwapRateHelperSpread($B76,Trigger)</f>
@@ -5451,18 +5451,18 @@
       </c>
       <c r="I76" s="4">
         <f>_xll.qlRateHelperEarliestDate($B76,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J76" s="3">
         <f>_xll.qlRateHelperLatestDate($B76,Trigger)</f>
-        <v>46307</v>
+        <v>46308</v>
       </c>
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B77" s="149" t="str">
         <f>Swaps!K21</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00395#0001</v>
       </c>
       <c r="C77" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B77)</f>
@@ -5487,18 +5487,18 @@
       </c>
       <c r="I77" s="4">
         <f>_xll.qlRateHelperEarliestDate($B77,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J77" s="3">
         <f>_xll.qlRateHelperLatestDate($B77,Trigger)</f>
-        <v>46671</v>
+        <v>46673</v>
       </c>
       <c r="L77" s="9"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B78" s="149" t="str">
         <f>Swaps!K22</f>
-        <v>obj_00368#0001</v>
+        <v>obj_0037a#0001</v>
       </c>
       <c r="C78" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B78)</f>
@@ -5523,18 +5523,18 @@
       </c>
       <c r="I78" s="4">
         <f>_xll.qlRateHelperEarliestDate($B78,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J78" s="3">
         <f>_xll.qlRateHelperLatestDate($B78,Trigger)</f>
-        <v>47036</v>
+        <v>47039</v>
       </c>
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="149" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00375#0001</v>
+        <v>obj_00366#0001</v>
       </c>
       <c r="C79" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B79)</f>
@@ -5542,7 +5542,7 @@
       </c>
       <c r="D79" s="6">
         <f>_xll.qlRateHelperQuoteValue($B79,Trigger)</f>
-        <v>2.5549999999999996E-2</v>
+        <v>2.5390000000000003E-2</v>
       </c>
       <c r="E79" s="6">
         <f>_xll.qlSwapRateHelperSpread($B79,Trigger)</f>
@@ -5559,18 +5559,18 @@
       </c>
       <c r="I79" s="4">
         <f>_xll.qlRateHelperEarliestDate($B79,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J79" s="3">
         <f>_xll.qlRateHelperLatestDate($B79,Trigger)</f>
-        <v>47401</v>
+        <v>47406</v>
       </c>
       <c r="L79" s="9"/>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B80" s="149" t="str">
         <f>Swaps!K24</f>
-        <v>obj_00377#0001</v>
+        <v>obj_0037c#0001</v>
       </c>
       <c r="C80" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B80)</f>
@@ -5595,18 +5595,18 @@
       </c>
       <c r="I80" s="4">
         <f>_xll.qlRateHelperEarliestDate($B80,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J80" s="3">
         <f>_xll.qlRateHelperLatestDate($B80,Trigger)</f>
-        <v>47766</v>
+        <v>47770</v>
       </c>
       <c r="L80" s="9"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B81" s="149" t="str">
         <f>Swaps!K25</f>
-        <v>obj_003ae#0001</v>
+        <v>obj_00387#0001</v>
       </c>
       <c r="C81" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B81)</f>
@@ -5631,18 +5631,18 @@
       </c>
       <c r="I81" s="4">
         <f>_xll.qlRateHelperEarliestDate($B81,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J81" s="3">
         <f>_xll.qlRateHelperLatestDate($B81,Trigger)</f>
-        <v>48131</v>
+        <v>48134</v>
       </c>
       <c r="L81" s="9"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="149" t="str">
         <f>Swaps!K26</f>
-        <v>obj_00376#0001</v>
+        <v>obj_00371#0001</v>
       </c>
       <c r="C82" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B82)</f>
@@ -5667,18 +5667,18 @@
       </c>
       <c r="I82" s="4">
         <f>_xll.qlRateHelperEarliestDate($B82,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J82" s="3">
         <f>_xll.qlRateHelperLatestDate($B82,Trigger)</f>
-        <v>48498</v>
+        <v>48500</v>
       </c>
       <c r="L82" s="9"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="149" t="str">
         <f>Swaps!K27</f>
-        <v>obj_003aa#0001</v>
+        <v>obj_003af#0001</v>
       </c>
       <c r="C83" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B83)</f>
@@ -5703,18 +5703,18 @@
       </c>
       <c r="I83" s="4">
         <f>_xll.qlRateHelperEarliestDate($B83,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J83" s="3">
         <f>_xll.qlRateHelperLatestDate($B83,Trigger)</f>
-        <v>48862</v>
+        <v>48865</v>
       </c>
       <c r="L83" s="9"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="149" t="str">
         <f>Swaps!K28</f>
-        <v>obj_003a3#0001</v>
+        <v>obj_0036c#0001</v>
       </c>
       <c r="C84" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B84)</f>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="D84" s="6">
         <f>_xll.qlRateHelperQuoteValue($B84,Trigger)</f>
-        <v>2.683E-2</v>
+        <v>2.665E-2</v>
       </c>
       <c r="E84" s="6">
         <f>_xll.qlSwapRateHelperSpread($B84,Trigger)</f>
@@ -5739,18 +5739,18 @@
       </c>
       <c r="I84" s="4">
         <f>_xll.qlRateHelperEarliestDate($B84,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J84" s="3">
         <f>_xll.qlRateHelperLatestDate($B84,Trigger)</f>
-        <v>49227</v>
+        <v>49230</v>
       </c>
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="149" t="str">
         <f>Swaps!K29</f>
-        <v>obj_003a1#0001</v>
+        <v>obj_00393#0001</v>
       </c>
       <c r="C85" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B85)</f>
@@ -5775,18 +5775,18 @@
       </c>
       <c r="I85" s="4">
         <f>_xll.qlRateHelperEarliestDate($B85,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J85" s="3">
         <f>_xll.qlRateHelperLatestDate($B85,Trigger)</f>
-        <v>49592</v>
+        <v>49597</v>
       </c>
       <c r="L85" s="9"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="149" t="str">
         <f>Swaps!K30</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_003ad#0001</v>
       </c>
       <c r="C86" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B86)</f>
@@ -5811,18 +5811,18 @@
       </c>
       <c r="I86" s="4">
         <f>_xll.qlRateHelperEarliestDate($B86,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J86" s="3">
         <f>_xll.qlRateHelperLatestDate($B86,Trigger)</f>
-        <v>49958</v>
+        <v>49961</v>
       </c>
       <c r="L86" s="9"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B87" s="149" t="str">
         <f>Swaps!K31</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_00376#0001</v>
       </c>
       <c r="C87" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B87)</f>
@@ -5847,18 +5847,18 @@
       </c>
       <c r="I87" s="4">
         <f>_xll.qlRateHelperEarliestDate($B87,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J87" s="3">
         <f>_xll.qlRateHelperLatestDate($B87,Trigger)</f>
-        <v>50325</v>
+        <v>50326</v>
       </c>
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="149" t="str">
         <f>Swaps!K32</f>
-        <v>obj_00365#0001</v>
+        <v>obj_0038f#0001</v>
       </c>
       <c r="C88" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B88)</f>
@@ -5883,18 +5883,18 @@
       </c>
       <c r="I88" s="4">
         <f>_xll.qlRateHelperEarliestDate($B88,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J88" s="3">
         <f>_xll.qlRateHelperLatestDate($B88,Trigger)</f>
-        <v>50689</v>
+        <v>50691</v>
       </c>
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="149" t="str">
         <f>Swaps!K33</f>
-        <v>obj_00374#0001</v>
+        <v>obj_003b1#0001</v>
       </c>
       <c r="C89" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B89)</f>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="D89" s="6">
         <f>_xll.qlRateHelperQuoteValue($B89,Trigger)</f>
-        <v>2.7309999999999997E-2</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="E89" s="6">
         <f>_xll.qlSwapRateHelperSpread($B89,Trigger)</f>
@@ -5919,18 +5919,18 @@
       </c>
       <c r="I89" s="4">
         <f>_xll.qlRateHelperEarliestDate($B89,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J89" s="3">
         <f>_xll.qlRateHelperLatestDate($B89,Trigger)</f>
-        <v>51053</v>
+        <v>51056</v>
       </c>
       <c r="L89" s="9"/>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="149" t="str">
         <f>Swaps!K34</f>
-        <v>obj_003ac#0001</v>
+        <v>obj_00378#0001</v>
       </c>
       <c r="C90" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B90)</f>
@@ -5955,18 +5955,18 @@
       </c>
       <c r="I90" s="4">
         <f>_xll.qlRateHelperEarliestDate($B90,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J90" s="3">
         <f>_xll.qlRateHelperLatestDate($B90,Trigger)</f>
-        <v>51419</v>
+        <v>51424</v>
       </c>
       <c r="L90" s="9"/>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="149" t="str">
         <f>Swaps!K35</f>
-        <v>obj_0039f#0001</v>
+        <v>obj_0038a#0001</v>
       </c>
       <c r="C91" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B91)</f>
@@ -5991,18 +5991,18 @@
       </c>
       <c r="I91" s="4">
         <f>_xll.qlRateHelperEarliestDate($B91,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J91" s="3">
         <f>_xll.qlRateHelperLatestDate($B91,Trigger)</f>
-        <v>51784</v>
+        <v>51788</v>
       </c>
       <c r="L91" s="9"/>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="149" t="str">
         <f>Swaps!K36</f>
-        <v>obj_00394#0001</v>
+        <v>obj_0036a#0001</v>
       </c>
       <c r="C92" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B92)</f>
@@ -6027,18 +6027,18 @@
       </c>
       <c r="I92" s="4">
         <f>_xll.qlRateHelperEarliestDate($B92,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J92" s="3">
         <f>_xll.qlRateHelperLatestDate($B92,Trigger)</f>
-        <v>52149</v>
+        <v>52152</v>
       </c>
       <c r="L92" s="9"/>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="149" t="str">
         <f>Swaps!K37</f>
-        <v>obj_00398#0001</v>
+        <v>obj_0038d#0001</v>
       </c>
       <c r="C93" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B93)</f>
@@ -6063,18 +6063,18 @@
       </c>
       <c r="I93" s="4">
         <f>_xll.qlRateHelperEarliestDate($B93,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J93" s="3">
         <f>_xll.qlRateHelperLatestDate($B93,Trigger)</f>
-        <v>52516</v>
+        <v>52517</v>
       </c>
       <c r="L93" s="9"/>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="149" t="str">
         <f>Swaps!K38</f>
-        <v>obj_00367#0001</v>
+        <v>obj_0036f#0001</v>
       </c>
       <c r="C94" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B94)</f>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="D94" s="6">
         <f>_xll.qlRateHelperQuoteValue($B94,Trigger)</f>
-        <v>2.7549999999999998E-2</v>
+        <v>2.7309999999999997E-2</v>
       </c>
       <c r="E94" s="6">
         <f>_xll.qlSwapRateHelperSpread($B94,Trigger)</f>
@@ -6099,18 +6099,18 @@
       </c>
       <c r="I94" s="4">
         <f>_xll.qlRateHelperEarliestDate($B94,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J94" s="3">
         <f>_xll.qlRateHelperLatestDate($B94,Trigger)</f>
-        <v>52880</v>
+        <v>52883</v>
       </c>
       <c r="L94" s="9"/>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="149" t="str">
         <f>Swaps!K39</f>
-        <v>obj_00397#0001</v>
+        <v>obj_0039c#0001</v>
       </c>
       <c r="C95" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B95)</f>
@@ -6135,18 +6135,18 @@
       </c>
       <c r="I95" s="4">
         <f>_xll.qlRateHelperEarliestDate($B95,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J95" s="3">
         <f>_xll.qlRateHelperLatestDate($B95,Trigger)</f>
-        <v>54707</v>
+        <v>54709</v>
       </c>
       <c r="L95" s="9"/>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="149" t="str">
         <f>Swaps!K40</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_0039b#0001</v>
       </c>
       <c r="C96" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B96)</f>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="D96" s="6">
         <f>_xll.qlRateHelperQuoteValue($B96,Trigger)</f>
-        <v>2.7439999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="E96" s="6">
         <f>_xll.qlSwapRateHelperSpread($B96,Trigger)</f>
@@ -6171,18 +6171,18 @@
       </c>
       <c r="I96" s="4">
         <f>_xll.qlRateHelperEarliestDate($B96,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J96" s="3">
         <f>_xll.qlRateHelperLatestDate($B96,Trigger)</f>
-        <v>56534</v>
+        <v>56535</v>
       </c>
       <c r="L96" s="9"/>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B97" s="149" t="str">
         <f>Swaps!K41</f>
-        <v>obj_00369#0001</v>
+        <v>obj_00382#0001</v>
       </c>
       <c r="C97" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B97)</f>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D97" s="6">
         <f>_xll.qlRateHelperQuoteValue($B97,Trigger)</f>
-        <v>2.7439999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="E97" s="6">
         <f>_xll.qlSwapRateHelperSpread($B97,Trigger)</f>
@@ -6207,18 +6207,18 @@
       </c>
       <c r="I97" s="4">
         <f>_xll.qlRateHelperEarliestDate($B97,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J97" s="3">
         <f>_xll.qlRateHelperLatestDate($B97,Trigger)</f>
-        <v>60185</v>
+        <v>60188</v>
       </c>
       <c r="L97" s="9"/>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B98" s="151" t="str">
         <f>Swaps!K42</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_00394#0001</v>
       </c>
       <c r="C98" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B98)</f>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="D98" s="6">
         <f>_xll.qlRateHelperQuoteValue($B98,Trigger)</f>
-        <v>2.7570000000000001E-2</v>
+        <v>2.733E-2</v>
       </c>
       <c r="E98" s="6">
         <f>_xll.qlSwapRateHelperSpread($B98,Trigger)</f>
@@ -6243,11 +6243,11 @@
       </c>
       <c r="I98" s="4">
         <f>_xll.qlRateHelperEarliestDate($B98,Trigger)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="J98" s="3">
         <f>_xll.qlRateHelperLatestDate($B98,Trigger)</f>
-        <v>63837</v>
+        <v>63842</v>
       </c>
       <c r="L98" s="9"/>
     </row>
@@ -6285,7 +6285,7 @@
     <col min="2" max="2" width="41" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -6318,7 +6318,7 @@
       </c>
       <c r="J1" s="24">
         <f t="array" ref="J1:J126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>4.7437075217081001E-3</v>
+        <v>4.7437691733986558E-3</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -6330,7 +6330,7 @@
       </c>
       <c r="D2" s="25" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00352</v>
+        <v>obj_0034a</v>
       </c>
       <c r="E2" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -6346,14 +6346,14 @@
       </c>
       <c r="H2" s="23">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I2" s="22">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J2" s="24">
-        <v>4.7437075217081001E-3</v>
+        <v>4.7437691733986558E-3</v>
       </c>
       <c r="M2" s="73"/>
       <c r="N2" s="73"/>
@@ -6368,7 +6368,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="25" t="str">
-        <v>obj_0035b</v>
+        <v>obj_0035a</v>
       </c>
       <c r="E3" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -6376,7 +6376,7 @@
       </c>
       <c r="F3" s="24">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.8313000000000002E-3</v>
+        <v>4.8063000000000003E-3</v>
       </c>
       <c r="G3" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -6384,14 +6384,14 @@
       </c>
       <c r="H3" s="23">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I3" s="22">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="J3" s="24">
-        <v>4.7655976476932557E-3</v>
+        <v>4.7750187645798194E-3</v>
       </c>
       <c r="M3" s="73"/>
       <c r="N3" s="73"/>
@@ -6406,7 +6406,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="25" t="str">
-        <v>obj_00351</v>
+        <v>obj_00358</v>
       </c>
       <c r="E4" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="F4" s="24">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>4.8313000000000002E-3</v>
+        <v>4.8063000000000003E-3</v>
       </c>
       <c r="G4" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -6422,14 +6422,14 @@
       </c>
       <c r="H4" s="23">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I4" s="22">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41929</v>
+        <v>41932</v>
       </c>
       <c r="J4" s="24">
-        <v>4.8310761916065988E-3</v>
+        <v>4.8060785017727259E-3</v>
       </c>
       <c r="M4" s="73"/>
       <c r="N4" s="73"/>
@@ -6444,7 +6444,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="25" t="str">
-        <v>obj_00363</v>
+        <v>obj_0035f</v>
       </c>
       <c r="E5" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="F5" s="24">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>4.8952624999999998E-3</v>
+        <v>4.8704038499999998E-3</v>
       </c>
       <c r="G5" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -6460,14 +6460,14 @@
       </c>
       <c r="H5" s="23">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I5" s="22">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41936</v>
+        <v>41939</v>
       </c>
       <c r="J5" s="24">
-        <v>4.8948029817231968E-3</v>
+        <v>4.8699489865515096E-3</v>
       </c>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="F6" s="24">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>5.0505999999999997E-3</v>
+        <v>5.0444000000000001E-3</v>
       </c>
       <c r="G6" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -6499,14 +6499,14 @@
       </c>
       <c r="H6" s="23">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I6" s="22">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41953</v>
+        <v>41956</v>
       </c>
       <c r="J6" s="24">
-        <v>5.0495170694408375E-3</v>
+        <v>5.0433197262215205E-3</v>
       </c>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
@@ -6516,14 +6516,14 @@
     <row r="7" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>GBP_YCSTDRH_RateHelpersSelected#0003</v>
+        <v>GBP_YCSTDRH_RateHelpersSelected#0005</v>
       </c>
       <c r="B7" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
       <c r="D7" s="25" t="str">
-        <v>obj_00349</v>
+        <v>obj_00357</v>
       </c>
       <c r="E7" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -6531,7 +6531,7 @@
       </c>
       <c r="F7" s="24">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>5.2649999999999997E-3</v>
+        <v>5.2963000000000003E-3</v>
       </c>
       <c r="G7" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -6539,14 +6539,14 @@
       </c>
       <c r="H7" s="23">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I7" s="22">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41983</v>
+        <v>41988</v>
       </c>
       <c r="J7" s="24">
-        <v>5.2626850103116218E-3</v>
+        <v>5.2938806524068429E-3</v>
       </c>
       <c r="M7" s="73"/>
       <c r="N7" s="73"/>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="25" t="str">
-        <v>obj_00355</v>
+        <v>obj_00350</v>
       </c>
       <c r="E8" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -6571,14 +6571,14 @@
       </c>
       <c r="H8" s="23">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I8" s="22">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42016</v>
+        <v>42017</v>
       </c>
       <c r="J8" s="24">
-        <v>5.5947674692837773E-3</v>
+        <v>5.5948531871852E-3</v>
       </c>
       <c r="M8" s="73"/>
       <c r="N8" s="73"/>
@@ -6587,7 +6587,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9" s="25" t="str">
-        <v>obj_00362</v>
+        <v>obj_0035d</v>
       </c>
       <c r="E9" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="F9" s="24">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>6.0992999999999993E-3</v>
+        <v>6.0985688900000003E-3</v>
       </c>
       <c r="G9" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -6603,14 +6603,14 @@
       </c>
       <c r="H9" s="23">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I9" s="22">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42045</v>
+        <v>42048</v>
       </c>
       <c r="J9" s="24">
-        <v>6.0930403845047016E-3</v>
+        <v>6.0923107740422948E-3</v>
       </c>
       <c r="M9" s="73"/>
       <c r="N9" s="73"/>
@@ -6619,7 +6619,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D10" s="25" t="str">
-        <v>obj_0035d</v>
+        <v>obj_0035e</v>
       </c>
       <c r="E10" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="F10" s="24">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>6.5239666699999999E-3</v>
+        <v>6.5358666700000003E-3</v>
       </c>
       <c r="G10" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -6635,14 +6635,14 @@
       </c>
       <c r="H10" s="23">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I10" s="22">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42073</v>
+        <v>42076</v>
       </c>
       <c r="J10" s="24">
-        <v>6.5151785292494394E-3</v>
+        <v>6.5270464689880184E-3</v>
       </c>
       <c r="M10" s="73"/>
       <c r="N10" s="73"/>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="F11" s="24">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>6.9638E-3</v>
+        <v>7.0043999999999992E-3</v>
       </c>
       <c r="G11" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -6667,14 +6667,14 @@
       </c>
       <c r="H11" s="23">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I11" s="22">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42104</v>
+        <v>42107</v>
       </c>
       <c r="J11" s="24">
-        <v>6.9517375033014825E-3</v>
+        <v>6.992196605178711E-3</v>
       </c>
       <c r="M11" s="73"/>
       <c r="N11" s="73"/>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" s="25" t="str">
-        <v>obj_00360</v>
+        <v>obj_00363</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="F12" s="24">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>7.4849967200000004E-3</v>
+        <v>7.5338098399999999E-3</v>
       </c>
       <c r="G12" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -6699,14 +6699,14 @@
       </c>
       <c r="H12" s="23">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I12" s="22">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42135</v>
+        <v>42137</v>
       </c>
       <c r="J12" s="24">
-        <v>7.4686970949316362E-3</v>
+        <v>7.5173745380108757E-3</v>
       </c>
       <c r="M12" s="73"/>
       <c r="N12" s="73"/>
@@ -6715,7 +6715,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" s="25" t="str">
-        <v>obj_0035a</v>
+        <v>obj_00361</v>
       </c>
       <c r="E13" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="F13" s="24">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>8.0409398899999995E-3</v>
+        <v>8.080866669999999E-3</v>
       </c>
       <c r="G13" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -6731,14 +6731,14 @@
       </c>
       <c r="H13" s="23">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I13" s="22">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42165</v>
+        <v>42170</v>
       </c>
       <c r="J13" s="24">
-        <v>8.0194936798865125E-3</v>
+        <v>8.059029709216162E-3</v>
       </c>
       <c r="M13" s="73"/>
       <c r="N13" s="73"/>
@@ -6755,7 +6755,7 @@
       </c>
       <c r="F14" s="24">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>8.0756863400000007E-3</v>
+        <v>8.1161606599999998E-3</v>
       </c>
       <c r="G14" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -6763,14 +6763,14 @@
       </c>
       <c r="H14" s="23">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I14" s="22">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
         <v>42172</v>
       </c>
       <c r="J14" s="24">
-        <v>8.0534338692183592E-3</v>
+        <v>8.0939537157482984E-3</v>
       </c>
       <c r="M14" s="73"/>
       <c r="N14" s="73"/>
@@ -6779,15 +6779,15 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D15" s="25" t="str">
-        <v>obj_00372</v>
+        <v>obj_0038b</v>
       </c>
       <c r="E15" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D15)</f>
-        <v>GBPFUT3MM5_Quote</v>
+        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
       </c>
       <c r="F15" s="24">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>8.7100000000000354E-3</v>
+        <v>9.0100000000000024E-3</v>
       </c>
       <c r="G15" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -6802,7 +6802,7 @@
         <v>42264</v>
       </c>
       <c r="J15" s="24">
-        <v>8.2274858032596963E-3</v>
+        <v>8.3397839118799222E-3</v>
       </c>
       <c r="M15" s="73"/>
       <c r="N15" s="73"/>
@@ -6811,15 +6811,15 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D16" s="25" t="str">
-        <v>obj_00393</v>
+        <v>obj_003ae</v>
       </c>
       <c r="E16" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D16)</f>
-        <v>GBPFUT3MU5_Quote</v>
+        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
       </c>
       <c r="F16" s="24">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.028499999999997E-2</v>
+        <v>1.0634999999999931E-2</v>
       </c>
       <c r="G16" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -6834,7 +6834,7 @@
         <v>42354</v>
       </c>
       <c r="J16" s="24">
-        <v>8.6566310513285158E-3</v>
+        <v>8.8215572085989999E-3</v>
       </c>
       <c r="M16" s="182"/>
       <c r="N16" s="73"/>
@@ -6843,15 +6843,15 @@
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="25" t="str">
-        <v>obj_00395</v>
+        <v>obj_00375</v>
       </c>
       <c r="E17" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D17)</f>
-        <v>GBPFUT3MZ5_Quote</v>
+        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
       </c>
       <c r="F17" s="24">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.1853999999999905E-2</v>
+        <v>1.2253999999999972E-2</v>
       </c>
       <c r="G17" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -6866,7 +6866,7 @@
         <v>42445</v>
       </c>
       <c r="J17" s="24">
-        <v>9.209919201532064E-3</v>
+        <v>9.4189655916399728E-3</v>
       </c>
       <c r="M17" s="73"/>
       <c r="N17" s="73"/>
@@ -6875,15 +6875,15 @@
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="25" t="str">
-        <v>obj_0036e</v>
+        <v>obj_00370</v>
       </c>
       <c r="E18" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D18)</f>
-        <v>GBPFUT3MH6_Quote</v>
+        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
       </c>
       <c r="F18" s="24">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.3417999999999951E-2</v>
+        <v>1.3768000000000023E-2</v>
       </c>
       <c r="G18" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -6898,7 +6898,7 @@
         <v>42537</v>
       </c>
       <c r="J18" s="24">
-        <v>9.8360340294847276E-3</v>
+        <v>1.0069159063892717E-2</v>
       </c>
       <c r="M18" s="182"/>
       <c r="N18" s="73"/>
@@ -6907,15 +6907,15 @@
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D19" s="25" t="str">
-        <v>obj_003ab</v>
+        <v>obj_0036d</v>
       </c>
       <c r="E19" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D19)</f>
-        <v>GBPFUT3MM6_Quote</v>
+        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
       </c>
       <c r="F19" s="24">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.4877000000000008E-2</v>
+        <v>1.5276999999999964E-2</v>
       </c>
       <c r="G19" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -6930,7 +6930,7 @@
         <v>42628</v>
       </c>
       <c r="J19" s="24">
-        <v>1.0483385972415851E-2</v>
+        <v>1.0740715468917861E-2</v>
       </c>
       <c r="M19" s="182"/>
       <c r="N19" s="73"/>
@@ -6939,15 +6939,15 @@
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D20" s="25" t="str">
-        <v>obj_00382</v>
+        <v>obj_00391</v>
       </c>
       <c r="E20" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D20)</f>
-        <v>GBPFUT3MU6_Quote</v>
+        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
       </c>
       <c r="F20" s="24">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.6227000000000075E-2</v>
+        <v>1.6677000000000025E-2</v>
       </c>
       <c r="G20" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -6962,7 +6962,7 @@
         <v>42725</v>
       </c>
       <c r="J20" s="24">
-        <v>1.1168126600908587E-2</v>
+        <v>1.1450970925656452E-2</v>
       </c>
       <c r="M20" s="182"/>
       <c r="N20" s="73"/>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D21" s="25" t="str">
-        <v>obj_0037d</v>
+        <v>obj_00372</v>
       </c>
       <c r="E21" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D21)</f>
@@ -6987,14 +6987,14 @@
       </c>
       <c r="H21" s="23">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I21" s="22">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43018</v>
+        <v>43021</v>
       </c>
       <c r="J21" s="24">
-        <v>1.3771805428938268E-2</v>
+        <v>1.3768142894347073E-2</v>
       </c>
       <c r="M21" s="182"/>
       <c r="N21" s="73"/>
@@ -7003,7 +7003,7 @@
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D22" s="25" t="str">
-        <v>obj_00391</v>
+        <v>obj_003a4</v>
       </c>
       <c r="E22" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D22)</f>
@@ -7011,7 +7011,7 @@
       </c>
       <c r="F22" s="24">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.5870000000000002E-2</v>
+        <v>1.5819999999999997E-2</v>
       </c>
       <c r="G22" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -7019,14 +7019,14 @@
       </c>
       <c r="H22" s="23">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I22" s="22">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43383</v>
+        <v>43388</v>
       </c>
       <c r="J22" s="24">
-        <v>1.591051723401914E-2</v>
+        <v>1.585598711548427E-2</v>
       </c>
       <c r="M22" s="73"/>
       <c r="N22" s="73"/>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D23" s="25" t="str">
-        <v>obj_0039a</v>
+        <v>obj_00396</v>
       </c>
       <c r="E23" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D23)</f>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="F23" s="24">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.755E-2</v>
+        <v>1.746E-2</v>
       </c>
       <c r="G23" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -7051,14 +7051,14 @@
       </c>
       <c r="H23" s="23">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I23" s="22">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>43748</v>
+        <v>43752</v>
       </c>
       <c r="J23" s="24">
-        <v>1.7626111143867567E-2</v>
+        <v>1.7530765286243154E-2</v>
       </c>
       <c r="M23" s="182"/>
       <c r="N23" s="73"/>
@@ -7067,7 +7067,7 @@
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D24" s="25" t="str">
-        <v>obj_00385</v>
+        <v>obj_00373</v>
       </c>
       <c r="E24" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D24)</f>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="F24" s="24">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.8970000000000001E-2</v>
+        <v>1.8860000000000002E-2</v>
       </c>
       <c r="G24" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -7083,14 +7083,14 @@
       </c>
       <c r="H24" s="23">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I24" s="22">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44116</v>
+        <v>44117</v>
       </c>
       <c r="J24" s="24">
-        <v>1.9088433490059741E-2</v>
+        <v>1.8972807795900316E-2</v>
       </c>
       <c r="M24" s="73"/>
       <c r="N24" s="73"/>
@@ -7099,7 +7099,7 @@
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D25" s="25" t="str">
-        <v>obj_00390</v>
+        <v>obj_003a0</v>
       </c>
       <c r="E25" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D25)</f>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="F25" s="24">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.017E-2</v>
+        <v>2.0049999999999998E-2</v>
       </c>
       <c r="G25" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -7115,14 +7115,14 @@
       </c>
       <c r="H25" s="23">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I25" s="22">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44480</v>
+        <v>44482</v>
       </c>
       <c r="J25" s="24">
-        <v>2.0335635057223248E-2</v>
+        <v>2.0209359354211084E-2</v>
       </c>
       <c r="M25" s="73"/>
       <c r="N25" s="73"/>
@@ -7131,7 +7131,7 @@
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D26" s="25" t="str">
-        <v>obj_0036b</v>
+        <v>obj_003a7</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D26)</f>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="F26" s="24">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.1219999999999999E-2</v>
+        <v>2.1090000000000001E-2</v>
       </c>
       <c r="G26" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -7147,14 +7147,14 @@
       </c>
       <c r="H26" s="23">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I26" s="22">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>44844</v>
+        <v>44847</v>
       </c>
       <c r="J26" s="24">
-        <v>2.1437581930970229E-2</v>
+        <v>2.1300469833425605E-2</v>
       </c>
       <c r="M26" s="73"/>
       <c r="N26" s="73"/>
@@ -7163,7 +7163,7 @@
     </row>
     <row r="27" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D27" s="25" t="str">
-        <v>obj_00366</v>
+        <v>obj_003ac</v>
       </c>
       <c r="E27" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D27)</f>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="F27" s="24">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.213E-2</v>
+        <v>2.2000000000000002E-2</v>
       </c>
       <c r="G27" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -7179,14 +7179,14 @@
       </c>
       <c r="H27" s="23">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I27" s="22">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>45209</v>
+        <v>45212</v>
       </c>
       <c r="J27" s="24">
-        <v>2.2401365922016282E-2</v>
+        <v>2.2264414797843718E-2</v>
       </c>
       <c r="M27" s="73"/>
       <c r="N27" s="73"/>
@@ -7195,7 +7195,7 @@
     </row>
     <row r="28" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D28" s="25" t="str">
-        <v>obj_0036f</v>
+        <v>obj_0037b</v>
       </c>
       <c r="E28" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D28)</f>
@@ -7203,7 +7203,7 @@
       </c>
       <c r="F28" s="24">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.2930000000000002E-2</v>
+        <v>2.2800000000000001E-2</v>
       </c>
       <c r="G28" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -7211,14 +7211,14 @@
       </c>
       <c r="H28" s="23">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I28" s="22">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>45575</v>
+        <v>45579</v>
       </c>
       <c r="J28" s="24">
-        <v>2.3256768620420774E-2</v>
+        <v>2.3119771037523034E-2</v>
       </c>
       <c r="M28" s="73"/>
       <c r="N28" s="73"/>
@@ -7227,7 +7227,7 @@
     </row>
     <row r="29" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D29" s="25" t="str">
-        <v>obj_0037e</v>
+        <v>obj_0037d</v>
       </c>
       <c r="E29" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D29)</f>
@@ -7235,7 +7235,7 @@
       </c>
       <c r="F29" s="24">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.4219999999999998E-2</v>
+        <v>2.4080000000000004E-2</v>
       </c>
       <c r="G29" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -7243,14 +7243,14 @@
       </c>
       <c r="H29" s="23">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I29" s="22">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>46307</v>
+        <v>46308</v>
       </c>
       <c r="J29" s="24">
-        <v>2.4653956993317936E-2</v>
+        <v>2.4506030132746694E-2</v>
       </c>
       <c r="M29" s="73"/>
       <c r="N29" s="73"/>
@@ -7259,7 +7259,7 @@
     </row>
     <row r="30" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D30" s="25" t="str">
-        <v>obj_00375</v>
+        <v>obj_00366</v>
       </c>
       <c r="E30" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D30)</f>
@@ -7267,7 +7267,7 @@
       </c>
       <c r="F30" s="24">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.5549999999999996E-2</v>
+        <v>2.5390000000000003E-2</v>
       </c>
       <c r="G30" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -7275,14 +7275,14 @@
       </c>
       <c r="H30" s="23">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I30" s="22">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>47401</v>
+        <v>47406</v>
       </c>
       <c r="J30" s="24">
-        <v>2.6118323473934623E-2</v>
+        <v>2.5945965184275315E-2</v>
       </c>
       <c r="M30" s="73"/>
       <c r="N30" s="73"/>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="31" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D31" s="25" t="str">
-        <v>obj_003a3</v>
+        <v>obj_0036c</v>
       </c>
       <c r="E31" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D31)</f>
@@ -7299,7 +7299,7 @@
       </c>
       <c r="F31" s="24">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.683E-2</v>
+        <v>2.665E-2</v>
       </c>
       <c r="G31" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -7307,14 +7307,14 @@
       </c>
       <c r="H31" s="23">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I31" s="22">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>49227</v>
+        <v>49230</v>
       </c>
       <c r="J31" s="24">
-        <v>2.7550724035049858E-2</v>
+        <v>2.7354101537435081E-2</v>
       </c>
       <c r="M31" s="73"/>
       <c r="N31" s="73"/>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="32" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D32" s="25" t="str">
-        <v>obj_00374</v>
+        <v>obj_003b1</v>
       </c>
       <c r="E32" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D32)</f>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="F32" s="24">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.7309999999999997E-2</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="G32" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -7339,14 +7339,14 @@
       </c>
       <c r="H32" s="23">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I32" s="22">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>51053</v>
+        <v>51056</v>
       </c>
       <c r="J32" s="24">
-        <v>2.803043907759047E-2</v>
+        <v>2.7794512069043518E-2</v>
       </c>
       <c r="M32" s="73"/>
       <c r="N32" s="73"/>
@@ -7355,7 +7355,7 @@
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D33" s="25" t="str">
-        <v>obj_00367</v>
+        <v>obj_0036f</v>
       </c>
       <c r="E33" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D33)</f>
@@ -7363,7 +7363,7 @@
       </c>
       <c r="F33" s="24">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.7549999999999998E-2</v>
+        <v>2.7309999999999997E-2</v>
       </c>
       <c r="G33" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -7371,14 +7371,14 @@
       </c>
       <c r="H33" s="23">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I33" s="22">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>52880</v>
+        <v>52883</v>
       </c>
       <c r="J33" s="24">
-        <v>2.8237341484246427E-2</v>
+        <v>2.795998665109669E-2</v>
       </c>
       <c r="M33" s="73"/>
       <c r="N33" s="73"/>
@@ -7387,7 +7387,7 @@
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D34" s="25" t="str">
-        <v>obj_0037f</v>
+        <v>obj_0039b</v>
       </c>
       <c r="E34" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D34)</f>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="F34" s="24">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.7439999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="G34" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -7403,14 +7403,14 @@
       </c>
       <c r="H34" s="23">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I34" s="22">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>56534</v>
+        <v>56535</v>
       </c>
       <c r="J34" s="24">
-        <v>2.7836128428323455E-2</v>
+        <v>2.7570241720796279E-2</v>
       </c>
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
@@ -7419,7 +7419,7 @@
     </row>
     <row r="35" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D35" s="25" t="str">
-        <v>obj_00369</v>
+        <v>obj_00382</v>
       </c>
       <c r="E35" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D35)</f>
@@ -7427,7 +7427,7 @@
       </c>
       <c r="F35" s="24">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.7439999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="G35" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -7435,14 +7435,14 @@
       </c>
       <c r="H35" s="23">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I35" s="22">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>60185</v>
+        <v>60188</v>
       </c>
       <c r="J35" s="24">
-        <v>2.7718575045670765E-2</v>
+        <v>2.7458485495838431E-2</v>
       </c>
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="36" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D36" s="25" t="str">
-        <v>obj_0036c</v>
+        <v>obj_00394</v>
       </c>
       <c r="E36" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D36)</f>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="F36" s="24">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.7570000000000001E-2</v>
+        <v>2.733E-2</v>
       </c>
       <c r="G36" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -7467,14 +7467,14 @@
       </c>
       <c r="H36" s="23">
         <f>_xll.qlRateHelperEarliestDate($D36)</f>
-        <v>41922</v>
+        <v>41925</v>
       </c>
       <c r="I36" s="22">
         <f>_xll.qlRateHelperLatestDate($D36)</f>
-        <v>63837</v>
+        <v>63842</v>
       </c>
       <c r="J36" s="24">
-        <v>2.7935169414655847E-2</v>
+        <v>2.7676292114762923E-2</v>
       </c>
       <c r="M36" s="73"/>
       <c r="N36" s="73"/>
@@ -10143,7 +10143,7 @@
       </c>
       <c r="J3" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I3,H3,Permanent,Trigger)</f>
-        <v>obj_00352#0001</v>
+        <v>obj_0034a#0001</v>
       </c>
       <c r="K3" s="83" t="str">
         <f>_xll.ohRangeRetrieveError(J3)</f>
@@ -10174,7 +10174,7 @@
       </c>
       <c r="H4" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034a#0001</v>
+        <v>obj_00349#0001</v>
       </c>
       <c r="I4" s="80" t="str">
         <f>Currency&amp;$B4&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10182,7 +10182,7 @@
       </c>
       <c r="J4" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I4,"1D",C4,D4,E4,F4,G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_0035a#0001</v>
       </c>
       <c r="K4" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J4)</f>
@@ -10222,7 +10222,7 @@
       </c>
       <c r="J5" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I5,H5,Permanent,Trigger)</f>
-        <v>obj_00351#0001</v>
+        <v>obj_00358#0001</v>
       </c>
       <c r="K5" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J5)</f>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="H6" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00350#0001</v>
+        <v>obj_00355#0001</v>
       </c>
       <c r="I6" s="80" t="str">
         <f>Currency&amp;$B6&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10262,7 +10262,7 @@
       </c>
       <c r="J6" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I6,B6,C6,D6,E6,F6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0035f#0001</v>
       </c>
       <c r="K6" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J6)</f>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="H7" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00354#0001</v>
+        <v>obj_0034e#0001</v>
       </c>
       <c r="I7" s="80" t="str">
         <f>Currency&amp;$B7&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10302,7 +10302,7 @@
       </c>
       <c r="J7" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I7,B7,C7,D7,E7,F7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00362#0001</v>
       </c>
       <c r="K7" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J7)</f>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="J9" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I9,H9,Permanent,Trigger)</f>
-        <v>obj_00349#0001</v>
+        <v>obj_00357#0001</v>
       </c>
       <c r="K9" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J9)</f>
@@ -10422,7 +10422,7 @@
       </c>
       <c r="J10" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I10,H10,Permanent,Trigger)</f>
-        <v>obj_00355#0001</v>
+        <v>obj_00350#0001</v>
       </c>
       <c r="K10" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J10)</f>
@@ -10454,7 +10454,7 @@
       </c>
       <c r="H11" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034c#0001</v>
+        <v>obj_0034d#0001</v>
       </c>
       <c r="I11" s="80" t="str">
         <f>Currency&amp;$B11&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10462,7 +10462,7 @@
       </c>
       <c r="J11" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I11,B11,C11,D11,E11,F11,G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00362#0001</v>
+        <v>obj_0035d#0001</v>
       </c>
       <c r="K11" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J11)</f>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="H12" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034d#0001</v>
+        <v>obj_0034f#0001</v>
       </c>
       <c r="I12" s="80" t="str">
         <f>Currency&amp;$B12&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="J12" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I12,B12,C12,D12,E12,F12,G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_0035e#0001</v>
       </c>
       <c r="K12" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J12)</f>
@@ -10574,7 +10574,7 @@
       </c>
       <c r="H14" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00353#0001</v>
+        <v>obj_0034c#0001</v>
       </c>
       <c r="I14" s="80" t="str">
         <f>Currency&amp;$B14&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10582,7 +10582,7 @@
       </c>
       <c r="J14" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I14,B14,C14,D14,E14,F14,G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00360#0001</v>
+        <v>obj_00363#0001</v>
       </c>
       <c r="K14" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J14)</f>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="H15" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00356#0001</v>
+        <v>obj_00352#0001</v>
       </c>
       <c r="I15" s="80" t="str">
         <f>Currency&amp;$B15&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10622,7 +10622,7 @@
       </c>
       <c r="J15" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I15,B15,C15,D15,E15,F15,G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035a#0001</v>
+        <v>obj_00361#0001</v>
       </c>
       <c r="K15" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J15)</f>
@@ -10654,7 +10654,7 @@
       </c>
       <c r="H16" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00358#0001</v>
+        <v>obj_00356#0001</v>
       </c>
       <c r="I16" s="80" t="str">
         <f>Currency&amp;$B16&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10662,7 +10662,7 @@
       </c>
       <c r="J16" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I16,B16,C16,D16,E16,F16,G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_00360#0001</v>
       </c>
       <c r="K16" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J16)</f>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="H17" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034e#0001</v>
+        <v>obj_00351#0001</v>
       </c>
       <c r="I17" s="80" t="str">
         <f>Currency&amp;$B17&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="J17" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I17,B17,C17,D17,E17,F17,G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00361#0001</v>
+        <v>obj_0035b#0001</v>
       </c>
       <c r="K17" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J17)</f>
@@ -10734,7 +10734,7 @@
       </c>
       <c r="H18" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00357#0001</v>
+        <v>obj_00354#0001</v>
       </c>
       <c r="I18" s="80" t="str">
         <f>Currency&amp;$B18&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="J19" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I19,H19,Permanent,Trigger)</f>
-        <v>obj_0034f#0001</v>
+        <v>obj_00353#0001</v>
       </c>
       <c r="K19" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J19)</f>
@@ -10795,7 +10795,7 @@
       <c r="A20" s="82"/>
       <c r="B20" s="81">
         <f>_xll.qlCalendarBusinessDaysBetween(Calendar,_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),C20&amp;"D",,,Trigger),D24,Trigger)-1</f>
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="84">
         <v>0</v>
@@ -10820,7 +10820,7 @@
       </c>
       <c r="J20" s="181" t="str">
         <f>_xll.qlDepositRateHelper2(,I20,B20&amp;"D",C20,Deposits!D20,E20,F20,G20)</f>
-        <v>obj_003b4#0003</v>
+        <v>obj_003b4#0001</v>
       </c>
       <c r="K20" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J20)</f>
@@ -10892,9 +10892,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10903,7 +10901,7 @@
     <col min="3" max="3" width="6" style="72" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="72" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="72" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.7109375" style="72" customWidth="1"/>
@@ -10986,8 +10984,8 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F3" s="134" t="str">
-        <f t="shared" ref="F3:F34" si="1">Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;QuoteSuffix</f>
-        <v>GBPFUT3MV4_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MV4_HST_CLOSE_Quote</v>
       </c>
       <c r="G3" s="193">
         <f>IFERROR(INDEX($N$3:$N$8,MATCH(D3,$M$3:$M$8,0))/100,0)</f>
@@ -10995,7 +10993,7 @@
       </c>
       <c r="H3" s="135" t="str">
         <f>_xll.qlFuturesRateHelper(,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_00367#0002</v>
       </c>
       <c r="I3" s="136" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -11032,16 +11030,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F4" s="134" t="str">
-        <f t="shared" si="1"/>
-        <v>GBPFUT3MX4_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D4&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MX4_HST_CLOSE_Quote</v>
       </c>
       <c r="G4" s="193">
-        <f t="shared" ref="G4:G44" si="2">IFERROR(INDEX($N$3:$N$8,MATCH(D4,$M$3:$M$8,0))/100,0)</f>
+        <f t="shared" ref="G4:G44" si="1">IFERROR(INDEX($N$3:$N$8,MATCH(D4,$M$3:$M$8,0))/100,0)</f>
         <v>0</v>
       </c>
       <c r="H4" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00389#0001</v>
+        <v>obj_003a3#0004</v>
       </c>
       <c r="I4" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -11078,16 +11076,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F5" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D5&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ4_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G5" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ4_Quote</v>
-      </c>
-      <c r="G5" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00371#0001</v>
+        <v>obj_0039e#0004</v>
       </c>
       <c r="I5" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -11120,16 +11118,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F6" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D6&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MF5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G6" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MF5_Quote</v>
-      </c>
-      <c r="G6" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H6" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00373#0001</v>
+        <v>obj_00390#0004</v>
       </c>
       <c r="I6" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -11162,16 +11160,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F7" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D7&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MG5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G7" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MG5_Quote</v>
-      </c>
-      <c r="G7" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_003a2#0004</v>
       </c>
       <c r="I7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -11204,16 +11202,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F8" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D8&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G8" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH5_Quote</v>
-      </c>
-      <c r="G8" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H8" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00392#0001</v>
+        <v>obj_00392#0004</v>
       </c>
       <c r="I8" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -11246,16 +11244,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F9" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D9&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MJ5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G9" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MJ5_Quote</v>
-      </c>
-      <c r="G9" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H9" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00386#0001</v>
+        <v>obj_00398#0004</v>
       </c>
       <c r="I9" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -11280,16 +11278,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F10" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D10&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MK5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G10" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MK5_Quote</v>
-      </c>
-      <c r="G10" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_003a8#0004</v>
       </c>
       <c r="I10" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -11314,16 +11312,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F11" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D11&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G11" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM5_Quote</v>
-      </c>
-      <c r="G11" s="193">
-        <f t="shared" si="2"/>
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="H11" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00372#0001</v>
+        <v>obj_0038b#0004</v>
       </c>
       <c r="I11" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -11348,16 +11346,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F12" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D12&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MN5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G12" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MN5_Quote</v>
-      </c>
-      <c r="G12" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_003a5#0004</v>
       </c>
       <c r="I12" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -11382,16 +11380,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F13" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D13&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MQ5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G13" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MQ5_Quote</v>
-      </c>
-      <c r="G13" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039e#0001</v>
+        <v>obj_00386#0004</v>
       </c>
       <c r="I13" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -11416,16 +11414,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F14" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D14&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G14" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU5_Quote</v>
-      </c>
-      <c r="G14" s="193">
-        <f t="shared" si="2"/>
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="H14" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00393#0001</v>
+        <v>obj_003ae#0004</v>
       </c>
       <c r="I14" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H14)</f>
@@ -11450,16 +11448,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F15" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D15&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G15" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ5_Quote</v>
-      </c>
-      <c r="G15" s="193">
-        <f t="shared" si="2"/>
         <v>9.5999999999999989E-5</v>
       </c>
       <c r="H15" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00395#0001</v>
+        <v>obj_00375#0004</v>
       </c>
       <c r="I15" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H15)</f>
@@ -11484,16 +11482,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F16" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D16&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G16" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH6_Quote</v>
-      </c>
-      <c r="G16" s="193">
-        <f t="shared" si="2"/>
         <v>1.3200000000000001E-4</v>
       </c>
       <c r="H16" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036e#0001</v>
+        <v>obj_00370#0004</v>
       </c>
       <c r="I16" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H16)</f>
@@ -11518,16 +11516,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F17" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D17&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G17" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM6_Quote</v>
-      </c>
-      <c r="G17" s="193">
-        <f t="shared" si="2"/>
         <v>1.73E-4</v>
       </c>
       <c r="H17" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003ab#0001</v>
+        <v>obj_0036d#0004</v>
       </c>
       <c r="I17" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H17)</f>
@@ -11552,16 +11550,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F18" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D18&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G18" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU6_Quote</v>
-      </c>
-      <c r="G18" s="193">
-        <f t="shared" si="2"/>
         <v>2.23E-4</v>
       </c>
       <c r="H18" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00391#0004</v>
       </c>
       <c r="I18" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H18)</f>
@@ -11586,16 +11584,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F19" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D19&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ6_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G19" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ6_Quote</v>
-      </c>
-      <c r="G19" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H19" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036d#0001</v>
+        <v>obj_00365#0004</v>
       </c>
       <c r="I19" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H19)</f>
@@ -11620,16 +11618,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F20" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D20&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH7_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G20" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH7_Quote</v>
-      </c>
-      <c r="G20" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H20" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b0#0001</v>
+        <v>obj_003b0#0004</v>
       </c>
       <c r="I20" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H20)</f>
@@ -11654,16 +11652,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F21" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D21&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM7_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G21" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM7_Quote</v>
-      </c>
-      <c r="G21" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H21" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a2#0001</v>
+        <v>obj_003b3#0004</v>
       </c>
       <c r="I21" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H21)</f>
@@ -11688,16 +11686,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F22" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D22&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU7_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G22" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU7_Quote</v>
-      </c>
-      <c r="G22" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H22" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00396#0001</v>
+        <v>obj_0037f#0004</v>
       </c>
       <c r="I22" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H22)</f>
@@ -11722,16 +11720,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F23" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D23&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ7_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G23" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ7_Quote</v>
-      </c>
-      <c r="G23" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H23" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038e#0001</v>
+        <v>obj_0037e#0004</v>
       </c>
       <c r="I23" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H23)</f>
@@ -11756,16 +11754,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F24" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D24&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH8_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G24" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH8_Quote</v>
-      </c>
-      <c r="G24" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H24" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00379#0001</v>
+        <v>obj_00388#0004</v>
       </c>
       <c r="I24" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H24)</f>
@@ -11790,16 +11788,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F25" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D25&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM8_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G25" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM8_Quote</v>
-      </c>
-      <c r="G25" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_00380#0004</v>
       </c>
       <c r="I25" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H25)</f>
@@ -11824,16 +11822,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F26" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D26&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU8_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G26" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU8_Quote</v>
-      </c>
-      <c r="G26" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H26" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00380#0001</v>
+        <v>obj_0039f#0004</v>
       </c>
       <c r="I26" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H26)</f>
@@ -11858,16 +11856,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F27" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D27&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ8_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G27" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ8_Quote</v>
-      </c>
-      <c r="G27" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00374#0004</v>
       </c>
       <c r="I27" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H27)</f>
@@ -11892,16 +11890,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F28" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D28&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH9_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G28" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH9_Quote</v>
-      </c>
-      <c r="G28" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H28" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00399#0001</v>
+        <v>obj_003aa#0004</v>
       </c>
       <c r="I28" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H28)</f>
@@ -11926,16 +11924,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F29" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D29&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM9_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G29" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM9_Quote</v>
-      </c>
-      <c r="G29" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H29" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a7#0001</v>
+        <v>obj_003a1#0004</v>
       </c>
       <c r="I29" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H29)</f>
@@ -11960,16 +11958,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F30" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D30&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU9_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G30" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU9_Quote</v>
-      </c>
-      <c r="G30" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H30" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00378#0001</v>
+        <v>obj_00383#0004</v>
       </c>
       <c r="I30" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H30)</f>
@@ -11994,16 +11992,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F31" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D31&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ9_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G31" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MZ9_Quote</v>
-      </c>
-      <c r="G31" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H31" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00387#0001</v>
+        <v>obj_00384#0004</v>
       </c>
       <c r="I31" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H31)</f>
@@ -12028,16 +12026,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F32" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D32&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH0_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G32" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MH0_Quote</v>
-      </c>
-      <c r="G32" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H32" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_00377#0004</v>
       </c>
       <c r="I32" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H32)</f>
@@ -12062,16 +12060,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F33" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D33&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM0_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G33" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MM0_Quote</v>
-      </c>
-      <c r="G33" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H33" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00384#0001</v>
+        <v>obj_00368#0004</v>
       </c>
       <c r="I33" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H33)</f>
@@ -12096,16 +12094,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F34" s="134" t="str">
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D34&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU0_HST_CLOSE_Quote</v>
+      </c>
+      <c r="G34" s="193">
         <f t="shared" si="1"/>
-        <v>GBPFUT3MU0_Quote</v>
-      </c>
-      <c r="G34" s="193">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H34" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00370#0001</v>
+        <v>obj_0039a#0004</v>
       </c>
       <c r="I34" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H34)</f>
@@ -12126,20 +12124,20 @@
         <v>Z0</v>
       </c>
       <c r="E35" s="132" t="str">
-        <f t="shared" ref="E35:E44" si="3">PROPER(Currency)&amp;FamilyName&amp;$E$1</f>
+        <f t="shared" ref="E35:E44" si="2">PROPER(Currency)&amp;FamilyName&amp;$E$1</f>
         <v>GbpLibor3M</v>
       </c>
       <c r="F35" s="134" t="str">
-        <f t="shared" ref="F35:F44" si="4">Currency&amp;"FUT"&amp;$E$1&amp;$D35&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ0_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D35&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ0_HST_CLOSE_Quote</v>
       </c>
       <c r="G35" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H35" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b2#0001</v>
+        <v>obj_0036e#0004</v>
       </c>
       <c r="I35" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H35)</f>
@@ -12160,20 +12158,20 @@
         <v>H1</v>
       </c>
       <c r="E36" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F36" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MH1_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D36&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH1_HST_CLOSE_Quote</v>
       </c>
       <c r="G36" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H36" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b3#0001</v>
+        <v>obj_00379#0004</v>
       </c>
       <c r="I36" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H36)</f>
@@ -12194,20 +12192,20 @@
         <v>M1</v>
       </c>
       <c r="E37" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F37" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MM1_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D37&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM1_HST_CLOSE_Quote</v>
       </c>
       <c r="G37" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H37" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_003a9#0004</v>
       </c>
       <c r="I37" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H37)</f>
@@ -12228,20 +12226,20 @@
         <v>U1</v>
       </c>
       <c r="E38" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F38" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MU1_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D38&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU1_HST_CLOSE_Quote</v>
       </c>
       <c r="G38" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H38" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a8#0001</v>
+        <v>obj_0038e#0004</v>
       </c>
       <c r="I38" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H38)</f>
@@ -12262,20 +12260,20 @@
         <v>Z1</v>
       </c>
       <c r="E39" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F39" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MZ1_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D39&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ1_HST_CLOSE_Quote</v>
       </c>
       <c r="G39" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H39" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_0036b#0004</v>
       </c>
       <c r="I39" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H39)</f>
@@ -12296,20 +12294,20 @@
         <v>H2</v>
       </c>
       <c r="E40" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F40" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MH2_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D40&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH2_HST_CLOSE_Quote</v>
       </c>
       <c r="G40" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003af#0001</v>
+        <v>obj_003a6#0004</v>
       </c>
       <c r="I40" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H40)</f>
@@ -12330,20 +12328,20 @@
         <v>M2</v>
       </c>
       <c r="E41" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F41" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MM2_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D41&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MM2_HST_CLOSE_Quote</v>
       </c>
       <c r="G41" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003ad#0001</v>
+        <v>obj_00381#0004</v>
       </c>
       <c r="I41" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H41)</f>
@@ -12365,20 +12363,20 @@
         <v>U2</v>
       </c>
       <c r="E42" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F42" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MU2_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D42&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MU2_HST_CLOSE_Quote</v>
       </c>
       <c r="G42" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a9#0001</v>
+        <v>obj_003ab#0004</v>
       </c>
       <c r="I42" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H42)</f>
@@ -12399,20 +12397,20 @@
         <v>Z2</v>
       </c>
       <c r="E43" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F43" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MZ2_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D43&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MZ2_HST_CLOSE_Quote</v>
       </c>
       <c r="G43" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a5#0001</v>
+        <v>obj_00399#0004</v>
       </c>
       <c r="I43" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H43)</f>
@@ -12433,20 +12431,20 @@
         <v>H3</v>
       </c>
       <c r="E44" s="132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>GbpLibor3M</v>
       </c>
       <c r="F44" s="134" t="str">
-        <f t="shared" si="4"/>
-        <v>GBPFUT3MH3_Quote</v>
+        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D44&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
+        <v>GBPFUT3MH3_HST_CLOSE_Quote</v>
       </c>
       <c r="G44" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038b#0001</v>
+        <v>obj_003b2#0004</v>
       </c>
       <c r="I44" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H44)</f>
@@ -12645,7 +12643,7 @@
       </c>
       <c r="K6" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$4,$I6,B6,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00381#0001</v>
+        <v>obj_0038c#0001</v>
       </c>
       <c r="L6" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -12692,7 +12690,7 @@
       </c>
       <c r="K7" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$4,$I7,B7,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00369#0001</v>
       </c>
       <c r="L7" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -12743,7 +12741,7 @@
       </c>
       <c r="K8" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$4,$I8,B8,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_00385#0001</v>
       </c>
       <c r="L8" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -12794,7 +12792,7 @@
       </c>
       <c r="K9" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$4,$I9,B9,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00388#0001</v>
+        <v>obj_00389#0001</v>
       </c>
       <c r="L9" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -12841,7 +12839,7 @@
       </c>
       <c r="K10" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$4,$I10,B10,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b1#0001</v>
+        <v>obj_00397#0001</v>
       </c>
       <c r="L10" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -12892,7 +12890,7 @@
       </c>
       <c r="K11" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$4,$I11,B11,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_00372#0001</v>
       </c>
       <c r="L11" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -12934,7 +12932,7 @@
       </c>
       <c r="K12" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$4,$I12,B12,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00391#0001</v>
+        <v>obj_003a4#0001</v>
       </c>
       <c r="L12" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -12976,7 +12974,7 @@
       </c>
       <c r="K13" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$4,$I13,B13,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039a#0001</v>
+        <v>obj_00396#0001</v>
       </c>
       <c r="L13" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -13018,7 +13016,7 @@
       </c>
       <c r="K14" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$4,$I14,B14,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00385#0001</v>
+        <v>obj_00373#0001</v>
       </c>
       <c r="L14" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -13060,7 +13058,7 @@
       </c>
       <c r="K15" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$4,$I15,B15,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00390#0001</v>
+        <v>obj_003a0#0001</v>
       </c>
       <c r="L15" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -13102,7 +13100,7 @@
       </c>
       <c r="K16" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$4,$I16,B16,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036b#0001</v>
+        <v>obj_003a7#0001</v>
       </c>
       <c r="L16" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -13144,7 +13142,7 @@
       </c>
       <c r="K17" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$4,$I17,B17,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00366#0001</v>
+        <v>obj_003ac#0001</v>
       </c>
       <c r="L17" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -13186,7 +13184,7 @@
       </c>
       <c r="K18" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$4,$I18,B18,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_0037b#0001</v>
       </c>
       <c r="L18" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -13228,7 +13226,7 @@
       </c>
       <c r="K19" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$4,$I19,B19,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a6#0001</v>
+        <v>obj_0039d#0001</v>
       </c>
       <c r="L19" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -13270,7 +13268,7 @@
       </c>
       <c r="K20" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$4,$I20,B20,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037e#0001</v>
+        <v>obj_0037d#0001</v>
       </c>
       <c r="L20" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -13312,7 +13310,7 @@
       </c>
       <c r="K21" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$4,$I21,B21,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00383#0001</v>
+        <v>obj_00395#0001</v>
       </c>
       <c r="L21" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -13354,7 +13352,7 @@
       </c>
       <c r="K22" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$4,$I22,B22,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00368#0001</v>
+        <v>obj_0037a#0001</v>
       </c>
       <c r="L22" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -13396,7 +13394,7 @@
       </c>
       <c r="K23" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$4,$I23,B23,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00375#0001</v>
+        <v>obj_00366#0001</v>
       </c>
       <c r="L23" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -13438,7 +13436,7 @@
       </c>
       <c r="K24" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$4,$I24,B24,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00377#0001</v>
+        <v>obj_0037c#0001</v>
       </c>
       <c r="L24" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -13480,7 +13478,7 @@
       </c>
       <c r="K25" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$4,$I25,B25,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ae#0001</v>
+        <v>obj_00387#0001</v>
       </c>
       <c r="L25" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -13522,7 +13520,7 @@
       </c>
       <c r="K26" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$4,$I26,B26,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00376#0001</v>
+        <v>obj_00371#0001</v>
       </c>
       <c r="L26" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -13564,7 +13562,7 @@
       </c>
       <c r="K27" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$4,$I27,B27,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003aa#0001</v>
+        <v>obj_003af#0001</v>
       </c>
       <c r="L27" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -13606,7 +13604,7 @@
       </c>
       <c r="K28" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$4,$I28,B28,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a3#0001</v>
+        <v>obj_0036c#0001</v>
       </c>
       <c r="L28" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>
@@ -13648,7 +13646,7 @@
       </c>
       <c r="K29" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J29,$C29,Calendar,$F29,$G29,$H29,$K$4,$I29,B29,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a1#0001</v>
+        <v>obj_00393#0001</v>
       </c>
       <c r="L29" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K29)</f>
@@ -13690,7 +13688,7 @@
       </c>
       <c r="K30" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J30,$C30,Calendar,$F30,$G30,$H30,$K$4,$I30,B30,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_003ad#0001</v>
       </c>
       <c r="L30" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K30)</f>
@@ -13732,7 +13730,7 @@
       </c>
       <c r="K31" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J31,$C31,Calendar,$F31,$G31,$H31,$K$4,$I31,B31,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_00376#0001</v>
       </c>
       <c r="L31" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K31)</f>
@@ -13774,7 +13772,7 @@
       </c>
       <c r="K32" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J32,$C32,Calendar,$F32,$G32,$H32,$K$4,$I32,B32,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00365#0001</v>
+        <v>obj_0038f#0001</v>
       </c>
       <c r="L32" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K32)</f>
@@ -13816,7 +13814,7 @@
       </c>
       <c r="K33" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J33,$C33,Calendar,$F33,$G33,$H33,$K$4,$I33,B33,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00374#0001</v>
+        <v>obj_003b1#0001</v>
       </c>
       <c r="L33" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K33)</f>
@@ -13858,7 +13856,7 @@
       </c>
       <c r="K34" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J34,$C34,Calendar,$F34,$G34,$H34,$K$4,$I34,B34,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ac#0001</v>
+        <v>obj_00378#0001</v>
       </c>
       <c r="L34" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K34)</f>
@@ -13900,7 +13898,7 @@
       </c>
       <c r="K35" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J35,$C35,Calendar,$F35,$G35,$H35,$K$4,$I35,B35,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039f#0001</v>
+        <v>obj_0038a#0001</v>
       </c>
       <c r="L35" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K35)</f>
@@ -13942,7 +13940,7 @@
       </c>
       <c r="K36" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J36,$C36,Calendar,$F36,$G36,$H36,$K$4,$I36,B36,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00394#0001</v>
+        <v>obj_0036a#0001</v>
       </c>
       <c r="L36" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K36)</f>
@@ -13984,7 +13982,7 @@
       </c>
       <c r="K37" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J37,$C37,Calendar,$F37,$G37,$H37,$K$4,$I37,B37,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00398#0001</v>
+        <v>obj_0038d#0001</v>
       </c>
       <c r="L37" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K37)</f>
@@ -14026,7 +14024,7 @@
       </c>
       <c r="K38" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J38,$C38,Calendar,$F38,$G38,$H38,$K$4,$I38,B38,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00367#0001</v>
+        <v>obj_0036f#0001</v>
       </c>
       <c r="L38" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K38)</f>
@@ -14068,7 +14066,7 @@
       </c>
       <c r="K39" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J39,$C39,Calendar,$F39,$G39,$H39,$K$4,$I39,B39,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00397#0001</v>
+        <v>obj_0039c#0001</v>
       </c>
       <c r="L39" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K39)</f>
@@ -14110,7 +14108,7 @@
       </c>
       <c r="K40" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J40,$C40,Calendar,$F40,$G40,$H40,$K$4,$I40,B40,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037f#0001</v>
+        <v>obj_0039b#0001</v>
       </c>
       <c r="L40" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K40)</f>
@@ -14152,7 +14150,7 @@
       </c>
       <c r="K41" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J41,$C41,Calendar,$F41,$G41,$H41,$K$4,$I41,B41,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00369#0001</v>
+        <v>obj_00382#0001</v>
       </c>
       <c r="L41" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K41)</f>
@@ -14194,7 +14192,7 @@
       </c>
       <c r="K42" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J42,$C42,Calendar,$F42,$G42,$H42,$K$4,$I42,B42,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_00394#0001</v>
       </c>
       <c r="L42" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K42)</f>

</xml_diff>

<commit_message>
GBP std with live futures
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15225" yWindow="-15" windowWidth="15270" windowHeight="8415" activeTab="2"/>
+    <workbookView xWindow="15225" yWindow="-15" windowWidth="15270" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2111,7 +2111,7 @@
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="111" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Oct  1 2014 18:48:11</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Oct 13 2014 15:51:57</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="D14" s="59" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_GBPYCSTD#0005</v>
+        <v>_GBPYCSTD#0001</v>
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="40"/>
@@ -2469,11 +2469,11 @@
       <c r="B23" s="43"/>
       <c r="C23" s="46">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="D23" s="120">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
-        <v>2.795998665109669E-2</v>
+        <v>2.730723634639955E-2</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="40"/>
@@ -2630,7 +2630,7 @@
     <row r="2" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="149" t="str">
         <f>Deposits!J3</f>
-        <v>obj_0034a#0001</v>
+        <v>obj_00351#0001</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B2)</f>
@@ -2652,11 +2652,11 @@
       </c>
       <c r="I2" s="4">
         <f>_xll.qlRateHelperEarliestDate($B2,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J2" s="3">
         <f>_xll.qlRateHelperLatestDate($B2,Trigger)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="K2" s="1">
         <v>10</v>
@@ -2691,11 +2691,11 @@
       </c>
       <c r="I3" s="4">
         <f>_xll.qlRateHelperEarliestDate($B3,Trigger)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="J3" s="3">
         <f>_xll.qlRateHelperLatestDate($B3,Trigger)</f>
-        <v>41927</v>
+        <v>41928</v>
       </c>
       <c r="K3" s="1">
         <v>20</v>
@@ -2708,7 +2708,7 @@
     <row r="4" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="149" t="str">
         <f>Deposits!J5</f>
-        <v>obj_00358#0001</v>
+        <v>obj_0034f#0001</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B4)</f>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="I4" s="4">
         <f>_xll.qlRateHelperEarliestDate($B4,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J4" s="3">
         <f>_xll.qlRateHelperLatestDate($B4,Trigger)</f>
-        <v>41932</v>
+        <v>41933</v>
       </c>
     </row>
     <row r="5" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="149" t="str">
         <f>Deposits!J6</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00361#0001</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B5)</f>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="D5" s="6">
         <f>_xll.qlRateHelperQuoteValue($B5,Trigger)</f>
-        <v>4.8704038499999998E-3</v>
+        <v>4.8747040000000005E-3</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="74" t="b">
@@ -2762,17 +2762,17 @@
       </c>
       <c r="I5" s="4">
         <f>_xll.qlRateHelperEarliestDate($B5,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J5" s="3">
         <f>_xll.qlRateHelperLatestDate($B5,Trigger)</f>
-        <v>41939</v>
+        <v>41940</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="149" t="str">
         <f>Deposits!J7</f>
-        <v>obj_00362#0001</v>
+        <v>obj_0035f#0001</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B6)</f>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D6" s="6">
         <f>_xll.qlRateHelperQuoteValue($B6,Trigger)</f>
-        <v>4.9345076900000001E-3</v>
+        <v>4.9431079999999999E-3</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="74" t="b">
@@ -2794,17 +2794,17 @@
       </c>
       <c r="I6" s="4">
         <f>_xll.qlRateHelperEarliestDate($B6,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J6" s="3">
         <f>_xll.qlRateHelperLatestDate($B6,Trigger)</f>
-        <v>41946</v>
+        <v>41947</v>
       </c>
     </row>
     <row r="7" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="149" t="str">
         <f>Deposits!J8</f>
-        <v>obj_0034b#0001</v>
+        <v>obj_00352#0001</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B7)</f>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="D7" s="6">
         <f>_xll.qlRateHelperQuoteValue($B7,Trigger)</f>
-        <v>5.0444000000000001E-3</v>
+        <v>5.0505999999999997E-3</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="74" t="b">
@@ -2826,17 +2826,17 @@
       </c>
       <c r="I7" s="4">
         <f>_xll.qlRateHelperEarliestDate($B7,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J7" s="3">
         <f>_xll.qlRateHelperLatestDate($B7,Trigger)</f>
-        <v>41956</v>
+        <v>41957</v>
       </c>
     </row>
     <row r="8" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="149" t="str">
         <f>Deposits!J9</f>
-        <v>obj_00357#0001</v>
+        <v>obj_0034a#0001</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B8)</f>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="D8" s="6">
         <f>_xll.qlRateHelperQuoteValue($B8,Trigger)</f>
-        <v>5.2963000000000003E-3</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="74" t="b">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="I8" s="4">
         <f>_xll.qlRateHelperEarliestDate($B8,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J8" s="3">
         <f>_xll.qlRateHelperLatestDate($B8,Trigger)</f>
@@ -2868,7 +2868,7 @@
     <row r="9" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="149" t="str">
         <f>Deposits!J10</f>
-        <v>obj_00350#0001</v>
+        <v>obj_00359#0001</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B9)</f>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="D9" s="6">
         <f>_xll.qlRateHelperQuoteValue($B9,Trigger)</f>
-        <v>5.5988000000000001E-3</v>
+        <v>5.5962999999999994E-3</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="74" t="b">
@@ -2890,17 +2890,17 @@
       </c>
       <c r="I9" s="4">
         <f>_xll.qlRateHelperEarliestDate($B9,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J9" s="3">
         <f>_xll.qlRateHelperLatestDate($B9,Trigger)</f>
-        <v>42017</v>
+        <v>42018</v>
       </c>
     </row>
     <row r="10" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="149" t="str">
         <f>Deposits!J11</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_00362#0001</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B10)</f>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D10" s="6">
         <f>_xll.qlRateHelperQuoteValue($B10,Trigger)</f>
-        <v>6.0985688900000003E-3</v>
+        <v>6.08258667E-3</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="74" t="b">
@@ -2922,17 +2922,17 @@
       </c>
       <c r="I10" s="4">
         <f>_xll.qlRateHelperEarliestDate($B10,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J10" s="3">
         <f>_xll.qlRateHelperLatestDate($B10,Trigger)</f>
-        <v>42048</v>
+        <v>42051</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="149" t="str">
         <f>Deposits!J12</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_0035d#0001</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B11)</f>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="D11" s="6">
         <f>_xll.qlRateHelperQuoteValue($B11,Trigger)</f>
-        <v>6.5358666700000003E-3</v>
+        <v>6.52181333E-3</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="74" t="b">
@@ -2954,11 +2954,11 @@
       </c>
       <c r="I11" s="4">
         <f>_xll.qlRateHelperEarliestDate($B11,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J11" s="3">
         <f>_xll.qlRateHelperLatestDate($B11,Trigger)</f>
-        <v>42076</v>
+        <v>42079</v>
       </c>
       <c r="K11" s="1">
         <v>30</v>
@@ -2971,7 +2971,7 @@
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="149" t="str">
         <f>Deposits!J13</f>
-        <v>obj_00359#0001</v>
+        <v>obj_00357#0001</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B12)</f>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="D12" s="6">
         <f>_xll.qlRateHelperQuoteValue($B12,Trigger)</f>
-        <v>7.0043999999999992E-3</v>
+        <v>7.0081000000000006E-3</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="74" t="b">
@@ -2993,11 +2993,11 @@
       </c>
       <c r="I12" s="4">
         <f>_xll.qlRateHelperEarliestDate($B12,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J12" s="3">
         <f>_xll.qlRateHelperLatestDate($B12,Trigger)</f>
-        <v>42107</v>
+        <v>42108</v>
       </c>
       <c r="K12" s="1">
         <v>40</v>
@@ -3010,7 +3010,7 @@
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="149" t="str">
         <f>Deposits!J14</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0035b#0001</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B13)</f>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D13" s="6">
         <f>_xll.qlRateHelperQuoteValue($B13,Trigger)</f>
-        <v>7.5338098399999999E-3</v>
+        <v>7.5726989099999999E-3</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="74" t="b">
@@ -3032,11 +3032,11 @@
       </c>
       <c r="I13" s="4">
         <f>_xll.qlRateHelperEarliestDate($B13,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J13" s="3">
         <f>_xll.qlRateHelperLatestDate($B13,Trigger)</f>
-        <v>42137</v>
+        <v>42138</v>
       </c>
       <c r="K13" s="1">
         <v>50</v>
@@ -3049,7 +3049,7 @@
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="149" t="str">
         <f>Deposits!J15</f>
-        <v>obj_00361#0001</v>
+        <v>obj_00363#0001</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B14)</f>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="D14" s="6">
         <f>_xll.qlRateHelperQuoteValue($B14,Trigger)</f>
-        <v>8.080866669999999E-3</v>
+        <v>8.0843666700000007E-3</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="74" t="b">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="I14" s="4">
         <f>_xll.qlRateHelperEarliestDate($B14,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J14" s="3">
         <f>_xll.qlRateHelperLatestDate($B14,Trigger)</f>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="D15" s="6">
         <f>_xll.qlRateHelperQuoteValue($B15,Trigger)</f>
-        <v>8.6102764999999998E-3</v>
+        <v>8.6136781399999991E-3</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="74" t="b">
@@ -3110,17 +3110,17 @@
       </c>
       <c r="I15" s="4">
         <f>_xll.qlRateHelperEarliestDate($B15,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J15" s="3">
         <f>_xll.qlRateHelperLatestDate($B15,Trigger)</f>
-        <v>42198</v>
+        <v>42199</v>
       </c>
     </row>
     <row r="16" spans="2:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="149" t="str">
         <f>Deposits!J17</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_0035c#0001</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B16)</f>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="D16" s="6">
         <f>_xll.qlRateHelperQuoteValue($B16,Trigger)</f>
-        <v>9.1926273200000005E-3</v>
+        <v>9.1782770499999992E-3</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="74" t="b">
@@ -3142,17 +3142,17 @@
       </c>
       <c r="I16" s="4">
         <f>_xll.qlRateHelperEarliestDate($B16,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J16" s="3">
         <f>_xll.qlRateHelperLatestDate($B16,Trigger)</f>
-        <v>42229</v>
+        <v>42230</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="149" t="str">
         <f>Deposits!J18</f>
-        <v>obj_0035c#0001</v>
+        <v>obj_0035e#0001</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B17)</f>
@@ -3160,7 +3160,7 @@
       </c>
       <c r="D17" s="6">
         <f>_xll.qlRateHelperQuoteValue($B17,Trigger)</f>
-        <v>9.7043901599999996E-3</v>
+        <v>9.7075885199999993E-3</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="74" t="b">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="I17" s="4">
         <f>_xll.qlRateHelperEarliestDate($B17,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J17" s="3">
         <f>_xll.qlRateHelperLatestDate($B17,Trigger)</f>
@@ -3184,7 +3184,7 @@
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="149" t="str">
         <f>Deposits!J19</f>
-        <v>obj_00353#0001</v>
+        <v>obj_00355#0001</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B18)</f>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D18" s="6">
         <f>_xll.qlRateHelperQuoteValue($B18,Trigger)</f>
-        <v>1.0233799999999999E-2</v>
+        <v>1.02369E-2</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="74" t="b">
@@ -3206,11 +3206,11 @@
       </c>
       <c r="I18" s="4">
         <f>_xll.qlRateHelperEarliestDate($B18,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J18" s="3">
         <f>_xll.qlRateHelperLatestDate($B18,Trigger)</f>
-        <v>42290</v>
+        <v>42291</v>
       </c>
       <c r="K18" s="1">
         <v>70</v>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="D19" s="6">
         <f>_xll.qlRateHelperQuoteValue($B19,Trigger)</f>
-        <v>8.1161606599999998E-3</v>
+        <v>8.10201038E-3</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="74" t="b">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="I19" s="4">
         <f>_xll.qlRateHelperEarliestDate($B19,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J19" s="3">
         <f>_xll.qlRateHelperLatestDate($B19,Trigger)</f>
@@ -3258,15 +3258,15 @@
       </c>
       <c r="B20" s="150" t="str">
         <f>Futures!H3</f>
-        <v>obj_00367#0002</v>
+        <v>obj_00382#0001</v>
       </c>
       <c r="C20" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B20)</f>
-        <v>GBPFUT3MV4_HST_CLOSE_Quote</v>
-      </c>
-      <c r="D20" s="147">
+        <v>GBPFUT3MV4_Quote</v>
+      </c>
+      <c r="D20" s="147" t="e">
         <f>_xll.qlRateHelperQuoteValue($B20,Trigger)</f>
-        <v>99.47</v>
+        <v>#NUM!</v>
       </c>
       <c r="E20" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B20,Trigger)</f>
@@ -3297,15 +3297,15 @@
       </c>
       <c r="B21" s="149" t="str">
         <f>Futures!H4</f>
-        <v>obj_003a3#0004</v>
+        <v>obj_00386#0001</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B21)</f>
-        <v>GBPFUT3MX4_HST_CLOSE_Quote</v>
-      </c>
-      <c r="D21" s="16">
+        <v>GBPFUT3MX4_Quote</v>
+      </c>
+      <c r="D21" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B21,Trigger)</f>
-        <v>99.42</v>
+        <v>#NUM!</v>
       </c>
       <c r="E21" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B21,Trigger)</f>
@@ -3336,15 +3336,15 @@
       </c>
       <c r="B22" s="149" t="str">
         <f>Futures!H5</f>
-        <v>obj_0039e#0004</v>
+        <v>obj_0037f#0001</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B22)</f>
-        <v>GBPFUT3MZ4_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ4_Quote</v>
       </c>
       <c r="D22" s="16">
         <f>_xll.qlRateHelperQuoteValue($B22,Trigger)</f>
-        <v>99.39</v>
+        <v>99.414999999999992</v>
       </c>
       <c r="E22" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B22,Trigger)</f>
@@ -3375,11 +3375,11 @@
       </c>
       <c r="B23" s="149" t="str">
         <f>Futures!H6</f>
-        <v>obj_00390#0004</v>
+        <v>obj_00389#0001</v>
       </c>
       <c r="C23" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B23)</f>
-        <v>GBPFUT3MF5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MF5_Quote</v>
       </c>
       <c r="D23" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B23,Trigger)</f>
@@ -3414,11 +3414,11 @@
       </c>
       <c r="B24" s="149" t="str">
         <f>Futures!H7</f>
-        <v>obj_003a2#0004</v>
+        <v>obj_003a6#0001</v>
       </c>
       <c r="C24" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B24)</f>
-        <v>GBPFUT3MG5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MG5_Quote</v>
       </c>
       <c r="D24" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B24,Trigger)</f>
@@ -3453,15 +3453,15 @@
       </c>
       <c r="B25" s="149" t="str">
         <f>Futures!H8</f>
-        <v>obj_00392#0004</v>
+        <v>obj_003b1#0001</v>
       </c>
       <c r="C25" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B25)</f>
-        <v>GBPFUT3MH5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH5_Quote</v>
       </c>
       <c r="D25" s="16">
         <f>_xll.qlRateHelperQuoteValue($B25,Trigger)</f>
-        <v>99.25</v>
+        <v>99.335000000000008</v>
       </c>
       <c r="E25" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B25,Trigger)</f>
@@ -3492,11 +3492,11 @@
       </c>
       <c r="B26" s="149" t="str">
         <f>Futures!H9</f>
-        <v>obj_00398#0004</v>
+        <v>obj_003a0#0001</v>
       </c>
       <c r="C26" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B26)</f>
-        <v>GBPFUT3MJ5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MJ5_Quote</v>
       </c>
       <c r="D26" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B26,Trigger)</f>
@@ -3531,11 +3531,11 @@
       </c>
       <c r="B27" s="149" t="str">
         <f>Futures!H10</f>
-        <v>obj_003a8#0004</v>
+        <v>obj_0038a#0001</v>
       </c>
       <c r="C27" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B27)</f>
-        <v>GBPFUT3MK5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MK5_Quote</v>
       </c>
       <c r="D27" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B27,Trigger)</f>
@@ -3570,15 +3570,15 @@
       </c>
       <c r="B28" s="149" t="str">
         <f>Futures!H11</f>
-        <v>obj_0038b#0004</v>
+        <v>obj_0036c#0001</v>
       </c>
       <c r="C28" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B28)</f>
-        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM5_Quote</v>
       </c>
       <c r="D28" s="16">
         <f>_xll.qlRateHelperQuoteValue($B28,Trigger)</f>
-        <v>99.094999999999999</v>
+        <v>99.224999999999994</v>
       </c>
       <c r="E28" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B28,Trigger)</f>
@@ -3610,11 +3610,11 @@
       </c>
       <c r="B29" s="149" t="str">
         <f>Futures!H12</f>
-        <v>obj_003a5#0004</v>
+        <v>obj_00371#0001</v>
       </c>
       <c r="C29" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B29)</f>
-        <v>GBPFUT3MN5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MN5_Quote</v>
       </c>
       <c r="D29" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B29,Trigger)</f>
@@ -3650,11 +3650,11 @@
       </c>
       <c r="B30" s="149" t="str">
         <f>Futures!H13</f>
-        <v>obj_00386#0004</v>
+        <v>obj_00388#0001</v>
       </c>
       <c r="C30" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B30)</f>
-        <v>GBPFUT3MQ5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MQ5_Quote</v>
       </c>
       <c r="D30" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B30,Trigger)</f>
@@ -3690,15 +3690,15 @@
       </c>
       <c r="B31" s="149" t="str">
         <f>Futures!H14</f>
-        <v>obj_003ae#0004</v>
+        <v>obj_00397#0001</v>
       </c>
       <c r="C31" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B31)</f>
-        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU5_Quote</v>
       </c>
       <c r="D31" s="16">
         <f>_xll.qlRateHelperQuoteValue($B31,Trigger)</f>
-        <v>98.93</v>
+        <v>99.094999999999999</v>
       </c>
       <c r="E31" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B31,Trigger)</f>
@@ -3730,15 +3730,15 @@
       </c>
       <c r="B32" s="149" t="str">
         <f>Futures!H15</f>
-        <v>obj_00375#0004</v>
+        <v>obj_0037c#0001</v>
       </c>
       <c r="C32" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B32)</f>
-        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ5_Quote</v>
       </c>
       <c r="D32" s="16">
         <f>_xll.qlRateHelperQuoteValue($B32,Trigger)</f>
-        <v>98.765000000000001</v>
+        <v>98.954999999999998</v>
       </c>
       <c r="E32" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B32,Trigger)</f>
@@ -3771,15 +3771,15 @@
       </c>
       <c r="B33" s="149" t="str">
         <f>Futures!H16</f>
-        <v>obj_00370#0004</v>
+        <v>obj_003af#0001</v>
       </c>
       <c r="C33" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B33)</f>
-        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH6_Quote</v>
       </c>
       <c r="D33" s="16">
         <f>_xll.qlRateHelperQuoteValue($B33,Trigger)</f>
-        <v>98.61</v>
+        <v>98.814999999999998</v>
       </c>
       <c r="E33" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B33,Trigger)</f>
@@ -3812,15 +3812,15 @@
       </c>
       <c r="B34" s="149" t="str">
         <f>Futures!H17</f>
-        <v>obj_0036d#0004</v>
+        <v>obj_00372#0001</v>
       </c>
       <c r="C34" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B34)</f>
-        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM6_Quote</v>
       </c>
       <c r="D34" s="16">
         <f>_xll.qlRateHelperQuoteValue($B34,Trigger)</f>
-        <v>98.454999999999998</v>
+        <v>98.685000000000002</v>
       </c>
       <c r="E34" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B34,Trigger)</f>
@@ -3853,15 +3853,15 @@
       </c>
       <c r="B35" s="149" t="str">
         <f>Futures!H18</f>
-        <v>obj_00391#0004</v>
+        <v>obj_003a8#0001</v>
       </c>
       <c r="C35" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B35)</f>
-        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU6_Quote</v>
       </c>
       <c r="D35" s="16">
         <f>_xll.qlRateHelperQuoteValue($B35,Trigger)</f>
-        <v>98.31</v>
+        <v>98.534999999999997</v>
       </c>
       <c r="E35" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B35,Trigger)</f>
@@ -3894,15 +3894,15 @@
       </c>
       <c r="B36" s="149" t="str">
         <f>Futures!H19</f>
-        <v>obj_00365#0004</v>
+        <v>obj_00368#0001</v>
       </c>
       <c r="C36" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B36)</f>
-        <v>GBPFUT3MZ6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ6_Quote</v>
       </c>
       <c r="D36" s="16">
         <f>_xll.qlRateHelperQuoteValue($B36,Trigger)</f>
-        <v>98.174999999999997</v>
+        <v>98.414999999999992</v>
       </c>
       <c r="E36" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B36,Trigger)</f>
@@ -3935,15 +3935,15 @@
       </c>
       <c r="B37" s="149" t="str">
         <f>Futures!H20</f>
-        <v>obj_003b0#0004</v>
+        <v>obj_003a5#0001</v>
       </c>
       <c r="C37" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B37)</f>
-        <v>GBPFUT3MH7_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH7_Quote</v>
       </c>
       <c r="D37" s="16">
         <f>_xll.qlRateHelperQuoteValue($B37,Trigger)</f>
-        <v>98.07</v>
+        <v>98.305000000000007</v>
       </c>
       <c r="E37" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B37,Trigger)</f>
@@ -3976,15 +3976,15 @@
       </c>
       <c r="B38" s="149" t="str">
         <f>Futures!H21</f>
-        <v>obj_003b3#0004</v>
+        <v>obj_003a9#0001</v>
       </c>
       <c r="C38" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B38)</f>
-        <v>GBPFUT3MM7_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM7_Quote</v>
       </c>
       <c r="D38" s="16">
         <f>_xll.qlRateHelperQuoteValue($B38,Trigger)</f>
-        <v>97.97</v>
+        <v>98.194999999999993</v>
       </c>
       <c r="E38" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B38,Trigger)</f>
@@ -4017,15 +4017,15 @@
       </c>
       <c r="B39" s="149" t="str">
         <f>Futures!H22</f>
-        <v>obj_0037f#0004</v>
+        <v>obj_003a1#0001</v>
       </c>
       <c r="C39" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B39)</f>
-        <v>GBPFUT3MU7_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU7_Quote</v>
       </c>
       <c r="D39" s="16">
         <f>_xll.qlRateHelperQuoteValue($B39,Trigger)</f>
-        <v>97.89</v>
+        <v>98.1</v>
       </c>
       <c r="E39" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B39,Trigger)</f>
@@ -4058,15 +4058,15 @@
       </c>
       <c r="B40" s="149" t="str">
         <f>Futures!H23</f>
-        <v>obj_0037e#0004</v>
+        <v>obj_003a2#0001</v>
       </c>
       <c r="C40" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B40)</f>
-        <v>GBPFUT3MZ7_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ7_Quote</v>
       </c>
       <c r="D40" s="16">
         <f>_xll.qlRateHelperQuoteValue($B40,Trigger)</f>
-        <v>97.814999999999998</v>
+        <v>98.015000000000001</v>
       </c>
       <c r="E40" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B40,Trigger)</f>
@@ -4099,15 +4099,15 @@
       </c>
       <c r="B41" s="149" t="str">
         <f>Futures!H24</f>
-        <v>obj_00388#0004</v>
+        <v>obj_00367#0001</v>
       </c>
       <c r="C41" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B41)</f>
-        <v>GBPFUT3MH8_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH8_Quote</v>
       </c>
       <c r="D41" s="16">
         <f>_xll.qlRateHelperQuoteValue($B41,Trigger)</f>
-        <v>97.745000000000005</v>
+        <v>97.935000000000002</v>
       </c>
       <c r="E41" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B41,Trigger)</f>
@@ -4140,15 +4140,15 @@
       </c>
       <c r="B42" s="149" t="str">
         <f>Futures!H25</f>
-        <v>obj_00380#0004</v>
+        <v>obj_00398#0001</v>
       </c>
       <c r="C42" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B42)</f>
-        <v>GBPFUT3MM8_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM8_Quote</v>
       </c>
       <c r="D42" s="16">
         <f>_xll.qlRateHelperQuoteValue($B42,Trigger)</f>
-        <v>97.68</v>
+        <v>97.86</v>
       </c>
       <c r="E42" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B42,Trigger)</f>
@@ -4181,15 +4181,15 @@
       </c>
       <c r="B43" s="149" t="str">
         <f>Futures!H26</f>
-        <v>obj_0039f#0004</v>
+        <v>obj_003ae#0001</v>
       </c>
       <c r="C43" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B43)</f>
-        <v>GBPFUT3MU8_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU8_Quote</v>
       </c>
       <c r="D43" s="16">
         <f>_xll.qlRateHelperQuoteValue($B43,Trigger)</f>
-        <v>97.62</v>
+        <v>97.795000000000002</v>
       </c>
       <c r="E43" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B43,Trigger)</f>
@@ -4222,15 +4222,15 @@
       </c>
       <c r="B44" s="149" t="str">
         <f>Futures!H27</f>
-        <v>obj_00374#0004</v>
+        <v>obj_0038e#0001</v>
       </c>
       <c r="C44" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B44)</f>
-        <v>GBPFUT3MZ8_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ8_Quote</v>
       </c>
       <c r="D44" s="16">
         <f>_xll.qlRateHelperQuoteValue($B44,Trigger)</f>
-        <v>97.56</v>
+        <v>97.740000000000009</v>
       </c>
       <c r="E44" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B44,Trigger)</f>
@@ -4263,15 +4263,15 @@
       </c>
       <c r="B45" s="149" t="str">
         <f>Futures!H28</f>
-        <v>obj_003aa#0004</v>
+        <v>obj_00376#0001</v>
       </c>
       <c r="C45" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B45)</f>
-        <v>GBPFUT3MH9_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH9_Quote</v>
       </c>
       <c r="D45" s="16">
         <f>_xll.qlRateHelperQuoteValue($B45,Trigger)</f>
-        <v>97.51</v>
+        <v>97.694999999999993</v>
       </c>
       <c r="E45" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B45,Trigger)</f>
@@ -4304,15 +4304,15 @@
       </c>
       <c r="B46" s="149" t="str">
         <f>Futures!H29</f>
-        <v>obj_003a1#0004</v>
+        <v>obj_00396#0001</v>
       </c>
       <c r="C46" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B46)</f>
-        <v>GBPFUT3MM9_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM9_Quote</v>
       </c>
       <c r="D46" s="16">
         <f>_xll.qlRateHelperQuoteValue($B46,Trigger)</f>
-        <v>97.46</v>
+        <v>97.65</v>
       </c>
       <c r="E46" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B46,Trigger)</f>
@@ -4345,15 +4345,15 @@
       </c>
       <c r="B47" s="149" t="str">
         <f>Futures!H30</f>
-        <v>obj_00383#0004</v>
+        <v>obj_0038b#0001</v>
       </c>
       <c r="C47" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B47)</f>
-        <v>GBPFUT3MU9_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU9_Quote</v>
       </c>
       <c r="D47" s="16">
         <f>_xll.qlRateHelperQuoteValue($B47,Trigger)</f>
-        <v>97.415000000000006</v>
+        <v>97.61</v>
       </c>
       <c r="E47" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B47,Trigger)</f>
@@ -4386,15 +4386,15 @@
       </c>
       <c r="B48" s="149" t="str">
         <f>Futures!H31</f>
-        <v>obj_00384#0004</v>
+        <v>obj_0036f#0001</v>
       </c>
       <c r="C48" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B48)</f>
-        <v>GBPFUT3MZ9_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ9_Quote</v>
       </c>
       <c r="D48" s="16">
         <f>_xll.qlRateHelperQuoteValue($B48,Trigger)</f>
-        <v>97.38</v>
+        <v>97.575000000000003</v>
       </c>
       <c r="E48" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B48,Trigger)</f>
@@ -4425,15 +4425,15 @@
       </c>
       <c r="B49" s="149" t="str">
         <f>Futures!H32</f>
-        <v>obj_00377#0004</v>
+        <v>obj_00374#0001</v>
       </c>
       <c r="C49" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B49)</f>
-        <v>GBPFUT3MH0_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH0_Quote</v>
       </c>
       <c r="D49" s="16">
         <f>_xll.qlRateHelperQuoteValue($B49,Trigger)</f>
-        <v>97.344999999999999</v>
+        <v>97.555000000000007</v>
       </c>
       <c r="E49" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B49,Trigger)</f>
@@ -4464,15 +4464,15 @@
       </c>
       <c r="B50" s="149" t="str">
         <f>Futures!H33</f>
-        <v>obj_00368#0004</v>
+        <v>obj_00394#0001</v>
       </c>
       <c r="C50" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B50)</f>
-        <v>GBPFUT3MM0_HST_CLOSE_Quote</v>
-      </c>
-      <c r="D50" s="16">
+        <v>GBPFUT3MM0_Quote</v>
+      </c>
+      <c r="D50" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B50,Trigger)</f>
-        <v>97.35</v>
+        <v>#NUM!</v>
       </c>
       <c r="E50" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B50,Trigger)</f>
@@ -4503,15 +4503,15 @@
       </c>
       <c r="B51" s="149" t="str">
         <f>Futures!H34</f>
-        <v>obj_0039a#0004</v>
+        <v>obj_003b2#0001</v>
       </c>
       <c r="C51" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B51)</f>
-        <v>GBPFUT3MU0_HST_CLOSE_Quote</v>
-      </c>
-      <c r="D51" s="16">
+        <v>GBPFUT3MU0_Quote</v>
+      </c>
+      <c r="D51" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B51,Trigger)</f>
-        <v>97.35</v>
+        <v>#NUM!</v>
       </c>
       <c r="E51" s="6">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($B51,Trigger)</f>
@@ -4542,11 +4542,11 @@
       </c>
       <c r="B52" s="149" t="str">
         <f>Futures!H35</f>
-        <v>obj_0036e#0004</v>
+        <v>obj_00390#0001</v>
       </c>
       <c r="C52" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B52)</f>
-        <v>GBPFUT3MZ0_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ0_Quote</v>
       </c>
       <c r="D52" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B52,Trigger)</f>
@@ -4581,11 +4581,11 @@
       </c>
       <c r="B53" s="149" t="str">
         <f>Futures!H36</f>
-        <v>obj_00379#0004</v>
+        <v>obj_0036d#0001</v>
       </c>
       <c r="C53" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B53)</f>
-        <v>GBPFUT3MH1_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH1_Quote</v>
       </c>
       <c r="D53" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B53,Trigger)</f>
@@ -4620,11 +4620,11 @@
       </c>
       <c r="B54" s="149" t="str">
         <f>Futures!H37</f>
-        <v>obj_003a9#0004</v>
+        <v>obj_00369#0001</v>
       </c>
       <c r="C54" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B54)</f>
-        <v>GBPFUT3MM1_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM1_Quote</v>
       </c>
       <c r="D54" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B54,Trigger)</f>
@@ -4659,11 +4659,11 @@
       </c>
       <c r="B55" s="149" t="str">
         <f>Futures!H38</f>
-        <v>obj_0038e#0004</v>
+        <v>obj_0036b#0001</v>
       </c>
       <c r="C55" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B55)</f>
-        <v>GBPFUT3MU1_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU1_Quote</v>
       </c>
       <c r="D55" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B55,Trigger)</f>
@@ -4698,11 +4698,11 @@
       </c>
       <c r="B56" s="149" t="str">
         <f>Futures!H39</f>
-        <v>obj_0036b#0004</v>
+        <v>obj_00393#0001</v>
       </c>
       <c r="C56" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B56)</f>
-        <v>GBPFUT3MZ1_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ1_Quote</v>
       </c>
       <c r="D56" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B56,Trigger)</f>
@@ -4737,11 +4737,11 @@
       </c>
       <c r="B57" s="149" t="str">
         <f>Futures!H40</f>
-        <v>obj_003a6#0004</v>
+        <v>obj_00399#0001</v>
       </c>
       <c r="C57" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B57)</f>
-        <v>GBPFUT3MH2_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH2_Quote</v>
       </c>
       <c r="D57" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B57,Trigger)</f>
@@ -4776,11 +4776,11 @@
       </c>
       <c r="B58" s="149" t="str">
         <f>Futures!H41</f>
-        <v>obj_00381#0004</v>
+        <v>obj_00377#0001</v>
       </c>
       <c r="C58" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B58)</f>
-        <v>GBPFUT3MM2_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM2_Quote</v>
       </c>
       <c r="D58" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B58,Trigger)</f>
@@ -4815,11 +4815,11 @@
       </c>
       <c r="B59" s="149" t="str">
         <f>Futures!H42</f>
-        <v>obj_003ab#0004</v>
+        <v>obj_003ad#0001</v>
       </c>
       <c r="C59" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B59)</f>
-        <v>GBPFUT3MU2_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU2_Quote</v>
       </c>
       <c r="D59" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B59,Trigger)</f>
@@ -4854,11 +4854,11 @@
       </c>
       <c r="B60" s="149" t="str">
         <f>Futures!H43</f>
-        <v>obj_00399#0004</v>
+        <v>obj_00383#0001</v>
       </c>
       <c r="C60" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B60)</f>
-        <v>GBPFUT3MZ2_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ2_Quote</v>
       </c>
       <c r="D60" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B60,Trigger)</f>
@@ -4893,11 +4893,11 @@
       </c>
       <c r="B61" s="149" t="str">
         <f>Futures!H44</f>
-        <v>obj_003b2#0004</v>
+        <v>obj_0036a#0001</v>
       </c>
       <c r="C61" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B61)</f>
-        <v>GBPFUT3MH3_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH3_Quote</v>
       </c>
       <c r="D61" s="16" t="e">
         <f>_xll.qlRateHelperQuoteValue($B61,Trigger)</f>
@@ -4931,7 +4931,7 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="150" t="str">
         <f>Swaps!K6</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00380#0001</v>
       </c>
       <c r="C62" s="14" t="str">
         <f>_xll.qlRateHelperQuoteName(B62)</f>
@@ -4956,17 +4956,17 @@
       </c>
       <c r="I62" s="11">
         <f>_xll.qlRateHelperEarliestDate($B62,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J62" s="10">
         <f>_xll.qlRateHelperLatestDate($B62,Trigger)</f>
-        <v>42290</v>
+        <v>42291</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="149" t="str">
         <f>Swaps!K7</f>
-        <v>obj_00369#0001</v>
+        <v>obj_0039e#0001</v>
       </c>
       <c r="C63" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B63)</f>
@@ -4991,11 +4991,11 @@
       </c>
       <c r="I63" s="4">
         <f>_xll.qlRateHelperEarliestDate($B63,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J63" s="3">
         <f>_xll.qlRateHelperLatestDate($B63,Trigger)</f>
-        <v>42382</v>
+        <v>42383</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="D64" s="6">
         <f>_xll.qlRateHelperQuoteValue($B64,Trigger)</f>
-        <v>9.6399999999999993E-3</v>
+        <v>8.8500000000000002E-3</v>
       </c>
       <c r="E64" s="6">
         <f>_xll.qlSwapRateHelperSpread($B64,Trigger)</f>
@@ -5026,17 +5026,17 @@
       </c>
       <c r="I64" s="4">
         <f>_xll.qlRateHelperEarliestDate($B64,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J64" s="3">
         <f>_xll.qlRateHelperLatestDate($B64,Trigger)</f>
-        <v>42473</v>
+        <v>42474</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="149" t="str">
         <f>Swaps!K9</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0037e#0001</v>
       </c>
       <c r="C65" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B65)</f>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="I65" s="4">
         <f>_xll.qlRateHelperEarliestDate($B65,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J65" s="3">
         <f>_xll.qlRateHelperLatestDate($B65,Trigger)</f>
-        <v>42564</v>
+        <v>42565</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="149" t="str">
         <f>Swaps!K10</f>
-        <v>obj_00397#0001</v>
+        <v>obj_00384#0001</v>
       </c>
       <c r="C66" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B66)</f>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="D66" s="6">
         <f>_xll.qlRateHelperQuoteValue($B66,Trigger)</f>
-        <v>1.111E-2</v>
+        <v>1.0049999999999998E-2</v>
       </c>
       <c r="E66" s="6">
         <f>_xll.qlSwapRateHelperSpread($B66,Trigger)</f>
@@ -5096,17 +5096,17 @@
       </c>
       <c r="I66" s="4">
         <f>_xll.qlRateHelperEarliestDate($B66,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J66" s="3">
         <f>_xll.qlRateHelperLatestDate($B66,Trigger)</f>
-        <v>42656</v>
+        <v>42657</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="149" t="str">
         <f>Swaps!K11</f>
-        <v>obj_00372#0001</v>
+        <v>obj_00381#0001</v>
       </c>
       <c r="C67" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B67)</f>
@@ -5114,7 +5114,7 @@
       </c>
       <c r="D67" s="6">
         <f>_xll.qlRateHelperQuoteValue($B67,Trigger)</f>
-        <v>1.376E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E67" s="6">
         <f>_xll.qlSwapRateHelperSpread($B67,Trigger)</f>
@@ -5131,17 +5131,17 @@
       </c>
       <c r="I67" s="4">
         <f>_xll.qlRateHelperEarliestDate($B67,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J67" s="3">
         <f>_xll.qlRateHelperLatestDate($B67,Trigger)</f>
-        <v>43021</v>
+        <v>43024</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="149" t="str">
         <f>Swaps!K12</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_0039b#0001</v>
       </c>
       <c r="C68" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B68)</f>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="D68" s="6">
         <f>_xll.qlRateHelperQuoteValue($B68,Trigger)</f>
-        <v>1.5819999999999997E-2</v>
+        <v>1.455E-2</v>
       </c>
       <c r="E68" s="6">
         <f>_xll.qlSwapRateHelperSpread($B68,Trigger)</f>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="I68" s="4">
         <f>_xll.qlRateHelperEarliestDate($B68,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J68" s="3">
         <f>_xll.qlRateHelperLatestDate($B68,Trigger)</f>
@@ -5176,7 +5176,7 @@
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="149" t="str">
         <f>Swaps!K13</f>
-        <v>obj_00396#0001</v>
+        <v>obj_00378#0001</v>
       </c>
       <c r="C69" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B69)</f>
@@ -5184,7 +5184,7 @@
       </c>
       <c r="D69" s="6">
         <f>_xll.qlRateHelperQuoteValue($B69,Trigger)</f>
-        <v>1.746E-2</v>
+        <v>1.6209999999999999E-2</v>
       </c>
       <c r="E69" s="6">
         <f>_xll.qlSwapRateHelperSpread($B69,Trigger)</f>
@@ -5201,7 +5201,7 @@
       </c>
       <c r="I69" s="4">
         <f>_xll.qlRateHelperEarliestDate($B69,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J69" s="3">
         <f>_xll.qlRateHelperLatestDate($B69,Trigger)</f>
@@ -5211,7 +5211,7 @@
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="149" t="str">
         <f>Swaps!K14</f>
-        <v>obj_00373#0001</v>
+        <v>obj_0038d#0001</v>
       </c>
       <c r="C70" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B70)</f>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="D70" s="6">
         <f>_xll.qlRateHelperQuoteValue($B70,Trigger)</f>
-        <v>1.8860000000000002E-2</v>
+        <v>1.7650000000000002E-2</v>
       </c>
       <c r="E70" s="6">
         <f>_xll.qlSwapRateHelperSpread($B70,Trigger)</f>
@@ -5236,17 +5236,17 @@
       </c>
       <c r="I70" s="4">
         <f>_xll.qlRateHelperEarliestDate($B70,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J70" s="3">
         <f>_xll.qlRateHelperLatestDate($B70,Trigger)</f>
-        <v>44117</v>
+        <v>44118</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="149" t="str">
         <f>Swaps!K15</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_0038f#0001</v>
       </c>
       <c r="C71" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B71)</f>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="D71" s="6">
         <f>_xll.qlRateHelperQuoteValue($B71,Trigger)</f>
-        <v>2.0049999999999998E-2</v>
+        <v>1.8919999999999999E-2</v>
       </c>
       <c r="E71" s="6">
         <f>_xll.qlSwapRateHelperSpread($B71,Trigger)</f>
@@ -5271,18 +5271,18 @@
       </c>
       <c r="I71" s="4">
         <f>_xll.qlRateHelperEarliestDate($B71,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J71" s="3">
         <f>_xll.qlRateHelperLatestDate($B71,Trigger)</f>
-        <v>44482</v>
+        <v>44483</v>
       </c>
       <c r="L71" s="9"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="149" t="str">
         <f>Swaps!K16</f>
-        <v>obj_003a7#0001</v>
+        <v>obj_0038c#0001</v>
       </c>
       <c r="C72" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B72)</f>
@@ -5290,7 +5290,7 @@
       </c>
       <c r="D72" s="6">
         <f>_xll.qlRateHelperQuoteValue($B72,Trigger)</f>
-        <v>2.1090000000000001E-2</v>
+        <v>2.0030000000000003E-2</v>
       </c>
       <c r="E72" s="6">
         <f>_xll.qlSwapRateHelperSpread($B72,Trigger)</f>
@@ -5307,18 +5307,18 @@
       </c>
       <c r="I72" s="4">
         <f>_xll.qlRateHelperEarliestDate($B72,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J72" s="3">
         <f>_xll.qlRateHelperLatestDate($B72,Trigger)</f>
-        <v>44847</v>
+        <v>44848</v>
       </c>
       <c r="L72" s="9"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="149" t="str">
         <f>Swaps!K17</f>
-        <v>obj_003ac#0001</v>
+        <v>obj_003a7#0001</v>
       </c>
       <c r="C73" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B73)</f>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="D73" s="6">
         <f>_xll.qlRateHelperQuoteValue($B73,Trigger)</f>
-        <v>2.2000000000000002E-2</v>
+        <v>2.1019999999999997E-2</v>
       </c>
       <c r="E73" s="6">
         <f>_xll.qlSwapRateHelperSpread($B73,Trigger)</f>
@@ -5343,18 +5343,18 @@
       </c>
       <c r="I73" s="4">
         <f>_xll.qlRateHelperEarliestDate($B73,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J73" s="3">
         <f>_xll.qlRateHelperLatestDate($B73,Trigger)</f>
-        <v>45212</v>
+        <v>45215</v>
       </c>
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B74" s="149" t="str">
         <f>Swaps!K18</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_003b0#0001</v>
       </c>
       <c r="C74" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B74)</f>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="D74" s="6">
         <f>_xll.qlRateHelperQuoteValue($B74,Trigger)</f>
-        <v>2.2800000000000001E-2</v>
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="E74" s="6">
         <f>_xll.qlSwapRateHelperSpread($B74,Trigger)</f>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="I74" s="4">
         <f>_xll.qlRateHelperEarliestDate($B74,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J74" s="3">
         <f>_xll.qlRateHelperLatestDate($B74,Trigger)</f>
@@ -5390,7 +5390,7 @@
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B75" s="149" t="str">
         <f>Swaps!K19</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_003a4#0001</v>
       </c>
       <c r="C75" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B75)</f>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="D75" s="6">
         <f>_xll.qlRateHelperQuoteValue($B75,Trigger)</f>
-        <v>2.3479999999999997E-2</v>
+        <v>2.2610000000000002E-2</v>
       </c>
       <c r="E75" s="6">
         <f>_xll.qlSwapRateHelperSpread($B75,Trigger)</f>
@@ -5415,18 +5415,18 @@
       </c>
       <c r="I75" s="4">
         <f>_xll.qlRateHelperEarliestDate($B75,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J75" s="3">
         <f>_xll.qlRateHelperLatestDate($B75,Trigger)</f>
-        <v>45943</v>
+        <v>45944</v>
       </c>
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B76" s="149" t="str">
         <f>Swaps!K20</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_003ab#0001</v>
       </c>
       <c r="C76" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B76)</f>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="D76" s="6">
         <f>_xll.qlRateHelperQuoteValue($B76,Trigger)</f>
-        <v>2.4080000000000004E-2</v>
+        <v>2.3220000000000001E-2</v>
       </c>
       <c r="E76" s="6">
         <f>_xll.qlSwapRateHelperSpread($B76,Trigger)</f>
@@ -5451,18 +5451,18 @@
       </c>
       <c r="I76" s="4">
         <f>_xll.qlRateHelperEarliestDate($B76,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J76" s="3">
         <f>_xll.qlRateHelperLatestDate($B76,Trigger)</f>
-        <v>46308</v>
+        <v>46309</v>
       </c>
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B77" s="149" t="str">
         <f>Swaps!K21</f>
-        <v>obj_00395#0001</v>
+        <v>obj_0039d#0001</v>
       </c>
       <c r="C77" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B77)</f>
@@ -5487,18 +5487,18 @@
       </c>
       <c r="I77" s="4">
         <f>_xll.qlRateHelperEarliestDate($B77,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J77" s="3">
         <f>_xll.qlRateHelperLatestDate($B77,Trigger)</f>
-        <v>46673</v>
+        <v>46674</v>
       </c>
       <c r="L77" s="9"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B78" s="149" t="str">
         <f>Swaps!K22</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_00392#0001</v>
       </c>
       <c r="C78" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B78)</f>
@@ -5523,18 +5523,18 @@
       </c>
       <c r="I78" s="4">
         <f>_xll.qlRateHelperEarliestDate($B78,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J78" s="3">
         <f>_xll.qlRateHelperLatestDate($B78,Trigger)</f>
-        <v>47039</v>
+        <v>47042</v>
       </c>
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="149" t="str">
         <f>Swaps!K23</f>
-        <v>obj_00366#0001</v>
+        <v>obj_0037d#0001</v>
       </c>
       <c r="C79" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B79)</f>
@@ -5542,7 +5542,7 @@
       </c>
       <c r="D79" s="6">
         <f>_xll.qlRateHelperQuoteValue($B79,Trigger)</f>
-        <v>2.5390000000000003E-2</v>
+        <v>2.4580000000000001E-2</v>
       </c>
       <c r="E79" s="6">
         <f>_xll.qlSwapRateHelperSpread($B79,Trigger)</f>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="I79" s="4">
         <f>_xll.qlRateHelperEarliestDate($B79,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J79" s="3">
         <f>_xll.qlRateHelperLatestDate($B79,Trigger)</f>
@@ -5570,7 +5570,7 @@
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B80" s="149" t="str">
         <f>Swaps!K24</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_00365#0001</v>
       </c>
       <c r="C80" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B80)</f>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="I80" s="4">
         <f>_xll.qlRateHelperEarliestDate($B80,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J80" s="3">
         <f>_xll.qlRateHelperLatestDate($B80,Trigger)</f>
@@ -5606,7 +5606,7 @@
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B81" s="149" t="str">
         <f>Swaps!K25</f>
-        <v>obj_00387#0001</v>
+        <v>obj_00370#0001</v>
       </c>
       <c r="C81" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B81)</f>
@@ -5631,18 +5631,18 @@
       </c>
       <c r="I81" s="4">
         <f>_xll.qlRateHelperEarliestDate($B81,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J81" s="3">
         <f>_xll.qlRateHelperLatestDate($B81,Trigger)</f>
-        <v>48134</v>
+        <v>48135</v>
       </c>
       <c r="L81" s="9"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="149" t="str">
         <f>Swaps!K26</f>
-        <v>obj_00371#0001</v>
+        <v>obj_0039f#0001</v>
       </c>
       <c r="C82" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B82)</f>
@@ -5667,18 +5667,18 @@
       </c>
       <c r="I82" s="4">
         <f>_xll.qlRateHelperEarliestDate($B82,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J82" s="3">
         <f>_xll.qlRateHelperLatestDate($B82,Trigger)</f>
-        <v>48500</v>
+        <v>48501</v>
       </c>
       <c r="L82" s="9"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="149" t="str">
         <f>Swaps!K27</f>
-        <v>obj_003af#0001</v>
+        <v>obj_0036e#0001</v>
       </c>
       <c r="C83" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B83)</f>
@@ -5703,18 +5703,18 @@
       </c>
       <c r="I83" s="4">
         <f>_xll.qlRateHelperEarliestDate($B83,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J83" s="3">
         <f>_xll.qlRateHelperLatestDate($B83,Trigger)</f>
-        <v>48865</v>
+        <v>48866</v>
       </c>
       <c r="L83" s="9"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="149" t="str">
         <f>Swaps!K28</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_0039a#0001</v>
       </c>
       <c r="C84" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B84)</f>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="D84" s="6">
         <f>_xll.qlRateHelperQuoteValue($B84,Trigger)</f>
-        <v>2.665E-2</v>
+        <v>2.589E-2</v>
       </c>
       <c r="E84" s="6">
         <f>_xll.qlSwapRateHelperSpread($B84,Trigger)</f>
@@ -5739,18 +5739,18 @@
       </c>
       <c r="I84" s="4">
         <f>_xll.qlRateHelperEarliestDate($B84,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J84" s="3">
         <f>_xll.qlRateHelperLatestDate($B84,Trigger)</f>
-        <v>49230</v>
+        <v>49233</v>
       </c>
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="149" t="str">
         <f>Swaps!K29</f>
-        <v>obj_00393#0001</v>
+        <v>obj_0039c#0001</v>
       </c>
       <c r="C85" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B85)</f>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="I85" s="4">
         <f>_xll.qlRateHelperEarliestDate($B85,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J85" s="3">
         <f>_xll.qlRateHelperLatestDate($B85,Trigger)</f>
@@ -5786,7 +5786,7 @@
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="149" t="str">
         <f>Swaps!K30</f>
-        <v>obj_003ad#0001</v>
+        <v>obj_00375#0001</v>
       </c>
       <c r="C86" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B86)</f>
@@ -5811,18 +5811,18 @@
       </c>
       <c r="I86" s="4">
         <f>_xll.qlRateHelperEarliestDate($B86,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J86" s="3">
         <f>_xll.qlRateHelperLatestDate($B86,Trigger)</f>
-        <v>49961</v>
+        <v>49962</v>
       </c>
       <c r="L86" s="9"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B87" s="149" t="str">
         <f>Swaps!K31</f>
-        <v>obj_00376#0001</v>
+        <v>obj_003ac#0001</v>
       </c>
       <c r="C87" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B87)</f>
@@ -5847,18 +5847,18 @@
       </c>
       <c r="I87" s="4">
         <f>_xll.qlRateHelperEarliestDate($B87,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J87" s="3">
         <f>_xll.qlRateHelperLatestDate($B87,Trigger)</f>
-        <v>50326</v>
+        <v>50327</v>
       </c>
       <c r="L87" s="9"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="149" t="str">
         <f>Swaps!K32</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_003aa#0001</v>
       </c>
       <c r="C88" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B88)</f>
@@ -5883,18 +5883,18 @@
       </c>
       <c r="I88" s="4">
         <f>_xll.qlRateHelperEarliestDate($B88,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J88" s="3">
         <f>_xll.qlRateHelperLatestDate($B88,Trigger)</f>
-        <v>50691</v>
+        <v>50692</v>
       </c>
       <c r="L88" s="9"/>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="149" t="str">
         <f>Swaps!K33</f>
-        <v>obj_003b1#0001</v>
+        <v>obj_00373#0001</v>
       </c>
       <c r="C89" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B89)</f>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="D89" s="6">
         <f>_xll.qlRateHelperQuoteValue($B89,Trigger)</f>
-        <v>2.7099999999999999E-2</v>
+        <v>2.6380000000000001E-2</v>
       </c>
       <c r="E89" s="6">
         <f>_xll.qlSwapRateHelperSpread($B89,Trigger)</f>
@@ -5919,18 +5919,18 @@
       </c>
       <c r="I89" s="4">
         <f>_xll.qlRateHelperEarliestDate($B89,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J89" s="3">
         <f>_xll.qlRateHelperLatestDate($B89,Trigger)</f>
-        <v>51056</v>
+        <v>51057</v>
       </c>
       <c r="L89" s="9"/>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="149" t="str">
         <f>Swaps!K34</f>
-        <v>obj_00378#0001</v>
+        <v>obj_003a3#0001</v>
       </c>
       <c r="C90" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B90)</f>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="I90" s="4">
         <f>_xll.qlRateHelperEarliestDate($B90,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J90" s="3">
         <f>_xll.qlRateHelperLatestDate($B90,Trigger)</f>
@@ -5966,7 +5966,7 @@
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="149" t="str">
         <f>Swaps!K35</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_00379#0001</v>
       </c>
       <c r="C91" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B91)</f>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="I91" s="4">
         <f>_xll.qlRateHelperEarliestDate($B91,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J91" s="3">
         <f>_xll.qlRateHelperLatestDate($B91,Trigger)</f>
@@ -6002,7 +6002,7 @@
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="149" t="str">
         <f>Swaps!K36</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_0037b#0001</v>
       </c>
       <c r="C92" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B92)</f>
@@ -6027,18 +6027,18 @@
       </c>
       <c r="I92" s="4">
         <f>_xll.qlRateHelperEarliestDate($B92,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J92" s="3">
         <f>_xll.qlRateHelperLatestDate($B92,Trigger)</f>
-        <v>52152</v>
+        <v>52153</v>
       </c>
       <c r="L92" s="9"/>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="149" t="str">
         <f>Swaps!K37</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00387#0001</v>
       </c>
       <c r="C93" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B93)</f>
@@ -6063,18 +6063,18 @@
       </c>
       <c r="I93" s="4">
         <f>_xll.qlRateHelperEarliestDate($B93,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J93" s="3">
         <f>_xll.qlRateHelperLatestDate($B93,Trigger)</f>
-        <v>52517</v>
+        <v>52518</v>
       </c>
       <c r="L93" s="9"/>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="149" t="str">
         <f>Swaps!K38</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_00366#0001</v>
       </c>
       <c r="C94" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B94)</f>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="D94" s="6">
         <f>_xll.qlRateHelperQuoteValue($B94,Trigger)</f>
-        <v>2.7309999999999997E-2</v>
+        <v>2.6619999999999998E-2</v>
       </c>
       <c r="E94" s="6">
         <f>_xll.qlSwapRateHelperSpread($B94,Trigger)</f>
@@ -6099,18 +6099,18 @@
       </c>
       <c r="I94" s="4">
         <f>_xll.qlRateHelperEarliestDate($B94,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J94" s="3">
         <f>_xll.qlRateHelperLatestDate($B94,Trigger)</f>
-        <v>52883</v>
+        <v>52884</v>
       </c>
       <c r="L94" s="9"/>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="149" t="str">
         <f>Swaps!K39</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_0037a#0001</v>
       </c>
       <c r="C95" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B95)</f>
@@ -6135,18 +6135,18 @@
       </c>
       <c r="I95" s="4">
         <f>_xll.qlRateHelperEarliestDate($B95,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J95" s="3">
         <f>_xll.qlRateHelperLatestDate($B95,Trigger)</f>
-        <v>54709</v>
+        <v>54710</v>
       </c>
       <c r="L95" s="9"/>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="149" t="str">
         <f>Swaps!K40</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_003b3#0001</v>
       </c>
       <c r="C96" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B96)</f>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="D96" s="6">
         <f>_xll.qlRateHelperQuoteValue($B96,Trigger)</f>
-        <v>2.7199999999999998E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
       <c r="E96" s="6">
         <f>_xll.qlSwapRateHelperSpread($B96,Trigger)</f>
@@ -6171,18 +6171,18 @@
       </c>
       <c r="I96" s="4">
         <f>_xll.qlRateHelperEarliestDate($B96,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J96" s="3">
         <f>_xll.qlRateHelperLatestDate($B96,Trigger)</f>
-        <v>56535</v>
+        <v>56536</v>
       </c>
       <c r="L96" s="9"/>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B97" s="149" t="str">
         <f>Swaps!K41</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00395#0001</v>
       </c>
       <c r="C97" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B97)</f>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D97" s="6">
         <f>_xll.qlRateHelperQuoteValue($B97,Trigger)</f>
-        <v>2.7199999999999998E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
       <c r="E97" s="6">
         <f>_xll.qlSwapRateHelperSpread($B97,Trigger)</f>
@@ -6207,18 +6207,18 @@
       </c>
       <c r="I97" s="4">
         <f>_xll.qlRateHelperEarliestDate($B97,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J97" s="3">
         <f>_xll.qlRateHelperLatestDate($B97,Trigger)</f>
-        <v>60188</v>
+        <v>60189</v>
       </c>
       <c r="L97" s="9"/>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B98" s="151" t="str">
         <f>Swaps!K42</f>
-        <v>obj_00394#0001</v>
+        <v>obj_00391#0001</v>
       </c>
       <c r="C98" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(B98)</f>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="D98" s="6">
         <f>_xll.qlRateHelperQuoteValue($B98,Trigger)</f>
-        <v>2.733E-2</v>
+        <v>2.665E-2</v>
       </c>
       <c r="E98" s="6">
         <f>_xll.qlSwapRateHelperSpread($B98,Trigger)</f>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="I98" s="4">
         <f>_xll.qlRateHelperEarliestDate($B98,Trigger)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="J98" s="3">
         <f>_xll.qlRateHelperLatestDate($B98,Trigger)</f>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="D2" s="25" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_0034a</v>
+        <v>obj_00351</v>
       </c>
       <c r="E2" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -6346,11 +6346,11 @@
       </c>
       <c r="H2" s="23">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I2" s="22">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="J2" s="24">
         <v>4.7437691733986558E-3</v>
@@ -6384,11 +6384,11 @@
       </c>
       <c r="H3" s="23">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41926</v>
+        <v>41927</v>
       </c>
       <c r="I3" s="22">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41927</v>
+        <v>41928</v>
       </c>
       <c r="J3" s="24">
         <v>4.7750187645798194E-3</v>
@@ -6406,7 +6406,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="25" t="str">
-        <v>obj_00358</v>
+        <v>obj_0034f</v>
       </c>
       <c r="E4" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -6422,11 +6422,11 @@
       </c>
       <c r="H4" s="23">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I4" s="22">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41932</v>
+        <v>41933</v>
       </c>
       <c r="J4" s="24">
         <v>4.8060785017727259E-3</v>
@@ -6444,7 +6444,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="25" t="str">
-        <v>obj_0035f</v>
+        <v>obj_00361</v>
       </c>
       <c r="E5" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="F5" s="24">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>4.8704038499999998E-3</v>
+        <v>4.8747040000000005E-3</v>
       </c>
       <c r="G5" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -6460,14 +6460,14 @@
       </c>
       <c r="H5" s="23">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I5" s="22">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41939</v>
+        <v>41940</v>
       </c>
       <c r="J5" s="24">
-        <v>4.8699489865515096E-3</v>
+        <v>4.8742483330410889E-3</v>
       </c>
       <c r="M5" s="73"/>
       <c r="N5" s="73"/>
@@ -6483,7 +6483,7 @@
         <v/>
       </c>
       <c r="D6" s="25" t="str">
-        <v>obj_0034b</v>
+        <v>obj_00352</v>
       </c>
       <c r="E6" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="F6" s="24">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>5.0444000000000001E-3</v>
+        <v>5.0505999999999997E-3</v>
       </c>
       <c r="G6" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -6499,14 +6499,14 @@
       </c>
       <c r="H6" s="23">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I6" s="22">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41956</v>
+        <v>41957</v>
       </c>
       <c r="J6" s="24">
-        <v>5.0433197262215205E-3</v>
+        <v>5.0495170694494799E-3</v>
       </c>
       <c r="M6" s="73"/>
       <c r="N6" s="73"/>
@@ -6516,14 +6516,14 @@
     <row r="7" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>GBP_YCSTDRH_RateHelpersSelected#0005</v>
+        <v>GBP_YCSTDRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
       <c r="D7" s="25" t="str">
-        <v>obj_00357</v>
+        <v>obj_0034a</v>
       </c>
       <c r="E7" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -6531,7 +6531,7 @@
       </c>
       <c r="F7" s="24">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>5.2963000000000003E-3</v>
+        <v>5.2900000000000004E-3</v>
       </c>
       <c r="G7" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -6539,14 +6539,14 @@
       </c>
       <c r="H7" s="23">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I7" s="22">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41988</v>
       </c>
       <c r="J7" s="24">
-        <v>5.2938806524068429E-3</v>
+        <v>5.2876246910424632E-3</v>
       </c>
       <c r="M7" s="73"/>
       <c r="N7" s="73"/>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="25" t="str">
-        <v>obj_00350</v>
+        <v>obj_00359</v>
       </c>
       <c r="E8" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="F8" s="24">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>5.5988000000000001E-3</v>
+        <v>5.5962999999999994E-3</v>
       </c>
       <c r="G8" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -6571,14 +6571,14 @@
       </c>
       <c r="H8" s="23">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I8" s="22">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42017</v>
+        <v>42018</v>
       </c>
       <c r="J8" s="24">
-        <v>5.5948531871852E-3</v>
+        <v>5.5923567094394991E-3</v>
       </c>
       <c r="M8" s="73"/>
       <c r="N8" s="73"/>
@@ -6587,7 +6587,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9" s="25" t="str">
-        <v>obj_0035d</v>
+        <v>obj_00362</v>
       </c>
       <c r="E9" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="F9" s="24">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>6.0985688900000003E-3</v>
+        <v>6.08258667E-3</v>
       </c>
       <c r="G9" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -6603,14 +6603,14 @@
       </c>
       <c r="H9" s="23">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I9" s="22">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42048</v>
+        <v>42051</v>
       </c>
       <c r="J9" s="24">
-        <v>6.0923107740422948E-3</v>
+        <v>6.0762602040534009E-3</v>
       </c>
       <c r="M9" s="73"/>
       <c r="N9" s="73"/>
@@ -6619,7 +6619,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D10" s="25" t="str">
-        <v>obj_0035e</v>
+        <v>obj_0035d</v>
       </c>
       <c r="E10" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="F10" s="24">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>6.5358666700000003E-3</v>
+        <v>6.52181333E-3</v>
       </c>
       <c r="G10" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -6635,14 +6635,14 @@
       </c>
       <c r="H10" s="23">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I10" s="22">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42076</v>
+        <v>42079</v>
       </c>
       <c r="J10" s="24">
-        <v>6.5270464689880184E-3</v>
+        <v>6.5129148734843576E-3</v>
       </c>
       <c r="M10" s="73"/>
       <c r="N10" s="73"/>
@@ -6651,7 +6651,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D11" s="25" t="str">
-        <v>obj_00359</v>
+        <v>obj_00357</v>
       </c>
       <c r="E11" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="F11" s="24">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>7.0043999999999992E-3</v>
+        <v>7.0081000000000006E-3</v>
       </c>
       <c r="G11" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -6667,14 +6667,14 @@
       </c>
       <c r="H11" s="23">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I11" s="22">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42107</v>
+        <v>42108</v>
       </c>
       <c r="J11" s="24">
-        <v>6.992196605178711E-3</v>
+        <v>6.9958837241277608E-3</v>
       </c>
       <c r="M11" s="73"/>
       <c r="N11" s="73"/>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" s="25" t="str">
-        <v>obj_00363</v>
+        <v>obj_0035b</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="F12" s="24">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>7.5338098399999999E-3</v>
+        <v>7.5726989099999999E-3</v>
       </c>
       <c r="G12" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -6699,14 +6699,14 @@
       </c>
       <c r="H12" s="23">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I12" s="22">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42137</v>
+        <v>42138</v>
       </c>
       <c r="J12" s="24">
-        <v>7.5173745380108757E-3</v>
+        <v>7.5560937431545109E-3</v>
       </c>
       <c r="M12" s="73"/>
       <c r="N12" s="73"/>
@@ -6715,7 +6715,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" s="25" t="str">
-        <v>obj_00361</v>
+        <v>obj_00363</v>
       </c>
       <c r="E13" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="F13" s="24">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>8.080866669999999E-3</v>
+        <v>8.0843666700000007E-3</v>
       </c>
       <c r="G13" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -6731,14 +6731,14 @@
       </c>
       <c r="H13" s="23">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I13" s="22">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
         <v>42170</v>
       </c>
       <c r="J13" s="24">
-        <v>8.059029709216162E-3</v>
+        <v>8.0625997106404633E-3</v>
       </c>
       <c r="M13" s="73"/>
       <c r="N13" s="73"/>
@@ -6755,7 +6755,7 @@
       </c>
       <c r="F14" s="24">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>8.1161606599999998E-3</v>
+        <v>8.10201038E-3</v>
       </c>
       <c r="G14" s="24" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -6763,14 +6763,14 @@
       </c>
       <c r="H14" s="23">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I14" s="22">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
         <v>42172</v>
       </c>
       <c r="J14" s="24">
-        <v>8.0939537157482984E-3</v>
+        <v>8.0799699310445984E-3</v>
       </c>
       <c r="M14" s="73"/>
       <c r="N14" s="73"/>
@@ -6779,15 +6779,15 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D15" s="25" t="str">
-        <v>obj_0038b</v>
+        <v>obj_0036c</v>
       </c>
       <c r="E15" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D15)</f>
-        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM5_Quote</v>
       </c>
       <c r="F15" s="24">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>9.0100000000000024E-3</v>
+        <v>7.7100000000000345E-3</v>
       </c>
       <c r="G15" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -6802,7 +6802,7 @@
         <v>42264</v>
       </c>
       <c r="J15" s="24">
-        <v>8.3397839118799222E-3</v>
+        <v>7.9772315646206814E-3</v>
       </c>
       <c r="M15" s="73"/>
       <c r="N15" s="73"/>
@@ -6811,15 +6811,15 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D16" s="25" t="str">
-        <v>obj_003ae</v>
+        <v>obj_00397</v>
       </c>
       <c r="E16" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D16)</f>
-        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU5_Quote</v>
       </c>
       <c r="F16" s="24">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.0634999999999931E-2</v>
+        <v>8.9850000000000017E-3</v>
       </c>
       <c r="G16" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -6834,7 +6834,7 @@
         <v>42354</v>
       </c>
       <c r="J16" s="24">
-        <v>8.8215572085989999E-3</v>
+        <v>8.1902428675789569E-3</v>
       </c>
       <c r="M16" s="182"/>
       <c r="N16" s="73"/>
@@ -6843,15 +6843,15 @@
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="25" t="str">
-        <v>obj_00375</v>
+        <v>obj_0037c</v>
       </c>
       <c r="E17" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D17)</f>
-        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MZ5_Quote</v>
       </c>
       <c r="F17" s="24">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.2253999999999972E-2</v>
+        <v>1.035400000000007E-2</v>
       </c>
       <c r="G17" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -6866,7 +6866,7 @@
         <v>42445</v>
       </c>
       <c r="J17" s="24">
-        <v>9.4189655916399728E-3</v>
+        <v>8.5672907836454818E-3</v>
       </c>
       <c r="M17" s="73"/>
       <c r="N17" s="73"/>
@@ -6875,15 +6875,15 @@
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="25" t="str">
-        <v>obj_00370</v>
+        <v>obj_003af</v>
       </c>
       <c r="E18" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D18)</f>
-        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MH6_Quote</v>
       </c>
       <c r="F18" s="24">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.3768000000000023E-2</v>
+        <v>1.1718000000000027E-2</v>
       </c>
       <c r="G18" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -6898,7 +6898,7 @@
         <v>42537</v>
       </c>
       <c r="J18" s="24">
-        <v>1.0069159063892717E-2</v>
+        <v>9.0391014456049738E-3</v>
       </c>
       <c r="M18" s="182"/>
       <c r="N18" s="73"/>
@@ -6907,15 +6907,15 @@
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D19" s="25" t="str">
-        <v>obj_0036d</v>
+        <v>obj_00372</v>
       </c>
       <c r="E19" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D19)</f>
-        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MM6_Quote</v>
       </c>
       <c r="F19" s="24">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.5276999999999964E-2</v>
+        <v>1.2976999999999995E-2</v>
       </c>
       <c r="G19" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -6930,7 +6930,7 @@
         <v>42628</v>
       </c>
       <c r="J19" s="24">
-        <v>1.0740715468917861E-2</v>
+        <v>9.5479476819382882E-3</v>
       </c>
       <c r="M19" s="182"/>
       <c r="N19" s="73"/>
@@ -6939,15 +6939,15 @@
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D20" s="25" t="str">
-        <v>obj_00391</v>
+        <v>obj_003a8</v>
       </c>
       <c r="E20" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D20)</f>
-        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
+        <v>GBPFUT3MU6_Quote</v>
       </c>
       <c r="F20" s="24">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.6677000000000025E-2</v>
+        <v>1.4427000000000053E-2</v>
       </c>
       <c r="G20" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -6962,7 +6962,7 @@
         <v>42725</v>
       </c>
       <c r="J20" s="24">
-        <v>1.1450970925656452E-2</v>
+        <v>1.0132739396864264E-2</v>
       </c>
       <c r="M20" s="182"/>
       <c r="N20" s="73"/>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D21" s="25" t="str">
-        <v>obj_00372</v>
+        <v>obj_00381</v>
       </c>
       <c r="E21" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D21)</f>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="F21" s="24">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.376E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="G21" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -6987,14 +6987,14 @@
       </c>
       <c r="H21" s="23">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I21" s="22">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43021</v>
+        <v>43024</v>
       </c>
       <c r="J21" s="24">
-        <v>1.3768142894347073E-2</v>
+        <v>1.2507034795452119E-2</v>
       </c>
       <c r="M21" s="182"/>
       <c r="N21" s="73"/>
@@ -7003,7 +7003,7 @@
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D22" s="25" t="str">
-        <v>obj_003a4</v>
+        <v>obj_0039b</v>
       </c>
       <c r="E22" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D22)</f>
@@ -7011,7 +7011,7 @@
       </c>
       <c r="F22" s="24">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.5819999999999997E-2</v>
+        <v>1.455E-2</v>
       </c>
       <c r="G22" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -7019,14 +7019,14 @@
       </c>
       <c r="H22" s="23">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I22" s="22">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
         <v>43388</v>
       </c>
       <c r="J22" s="24">
-        <v>1.585598711548427E-2</v>
+        <v>1.4584012900354996E-2</v>
       </c>
       <c r="M22" s="73"/>
       <c r="N22" s="73"/>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D23" s="25" t="str">
-        <v>obj_00396</v>
+        <v>obj_00378</v>
       </c>
       <c r="E23" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D23)</f>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="F23" s="24">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.746E-2</v>
+        <v>1.6209999999999999E-2</v>
       </c>
       <c r="G23" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -7051,14 +7051,14 @@
       </c>
       <c r="H23" s="23">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I23" s="22">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
         <v>43752</v>
       </c>
       <c r="J23" s="24">
-        <v>1.7530765286243154E-2</v>
+        <v>1.6277992114738023E-2</v>
       </c>
       <c r="M23" s="182"/>
       <c r="N23" s="73"/>
@@ -7067,7 +7067,7 @@
     </row>
     <row r="24" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D24" s="25" t="str">
-        <v>obj_00373</v>
+        <v>obj_0038d</v>
       </c>
       <c r="E24" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D24)</f>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="F24" s="24">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.8860000000000002E-2</v>
+        <v>1.7650000000000002E-2</v>
       </c>
       <c r="G24" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -7083,14 +7083,14 @@
       </c>
       <c r="H24" s="23">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I24" s="22">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44117</v>
+        <v>44118</v>
       </c>
       <c r="J24" s="24">
-        <v>1.8972807795900316E-2</v>
+        <v>1.7759974966811431E-2</v>
       </c>
       <c r="M24" s="73"/>
       <c r="N24" s="73"/>
@@ -7099,7 +7099,7 @@
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D25" s="25" t="str">
-        <v>obj_003a0</v>
+        <v>obj_0038f</v>
       </c>
       <c r="E25" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D25)</f>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="F25" s="24">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.0049999999999998E-2</v>
+        <v>1.8919999999999999E-2</v>
       </c>
       <c r="G25" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -7115,14 +7115,14 @@
       </c>
       <c r="H25" s="23">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I25" s="22">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44482</v>
+        <v>44483</v>
       </c>
       <c r="J25" s="24">
-        <v>2.0209359354211084E-2</v>
+        <v>1.9079547173377193E-2</v>
       </c>
       <c r="M25" s="73"/>
       <c r="N25" s="73"/>
@@ -7131,7 +7131,7 @@
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D26" s="25" t="str">
-        <v>obj_003a7</v>
+        <v>obj_0038c</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D26)</f>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="F26" s="24">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.1090000000000001E-2</v>
+        <v>2.0030000000000003E-2</v>
       </c>
       <c r="G26" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -7147,14 +7147,14 @@
       </c>
       <c r="H26" s="23">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I26" s="22">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>44847</v>
+        <v>44848</v>
       </c>
       <c r="J26" s="24">
-        <v>2.1300469833425605E-2</v>
+        <v>2.0243881544333851E-2</v>
       </c>
       <c r="M26" s="73"/>
       <c r="N26" s="73"/>
@@ -7163,7 +7163,7 @@
     </row>
     <row r="27" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D27" s="25" t="str">
-        <v>obj_003ac</v>
+        <v>obj_003a7</v>
       </c>
       <c r="E27" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D27)</f>
@@ -7171,7 +7171,7 @@
       </c>
       <c r="F27" s="24">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.2000000000000002E-2</v>
+        <v>2.1019999999999997E-2</v>
       </c>
       <c r="G27" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -7179,14 +7179,14 @@
       </c>
       <c r="H27" s="23">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I27" s="22">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>45212</v>
+        <v>45215</v>
       </c>
       <c r="J27" s="24">
-        <v>2.2264414797843718E-2</v>
+        <v>2.1292817302007144E-2</v>
       </c>
       <c r="M27" s="73"/>
       <c r="N27" s="73"/>
@@ -7195,7 +7195,7 @@
     </row>
     <row r="28" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D28" s="25" t="str">
-        <v>obj_0037b</v>
+        <v>obj_003b0</v>
       </c>
       <c r="E28" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D28)</f>
@@ -7203,7 +7203,7 @@
       </c>
       <c r="F28" s="24">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.2800000000000001E-2</v>
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="G28" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -7211,14 +7211,14 @@
       </c>
       <c r="H28" s="23">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I28" s="22">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
         <v>45579</v>
       </c>
       <c r="J28" s="24">
-        <v>2.3119771037523034E-2</v>
+        <v>2.2235287192528264E-2</v>
       </c>
       <c r="M28" s="73"/>
       <c r="N28" s="73"/>
@@ -7227,7 +7227,7 @@
     </row>
     <row r="29" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D29" s="25" t="str">
-        <v>obj_0037d</v>
+        <v>obj_003ab</v>
       </c>
       <c r="E29" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D29)</f>
@@ -7235,7 +7235,7 @@
       </c>
       <c r="F29" s="24">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.4080000000000004E-2</v>
+        <v>2.3220000000000001E-2</v>
       </c>
       <c r="G29" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -7243,14 +7243,14 @@
       </c>
       <c r="H29" s="23">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I29" s="22">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>46308</v>
+        <v>46309</v>
       </c>
       <c r="J29" s="24">
-        <v>2.4506030132746694E-2</v>
+        <v>2.3661276417649386E-2</v>
       </c>
       <c r="M29" s="73"/>
       <c r="N29" s="73"/>
@@ -7259,7 +7259,7 @@
     </row>
     <row r="30" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D30" s="25" t="str">
-        <v>obj_00366</v>
+        <v>obj_0037d</v>
       </c>
       <c r="E30" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D30)</f>
@@ -7267,7 +7267,7 @@
       </c>
       <c r="F30" s="24">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.5390000000000003E-2</v>
+        <v>2.4580000000000001E-2</v>
       </c>
       <c r="G30" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -7275,14 +7275,14 @@
       </c>
       <c r="H30" s="23">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I30" s="22">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
         <v>47406</v>
       </c>
       <c r="J30" s="24">
-        <v>2.5945965184275315E-2</v>
+        <v>2.515331714543596E-2</v>
       </c>
       <c r="M30" s="73"/>
       <c r="N30" s="73"/>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="31" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D31" s="25" t="str">
-        <v>obj_0036c</v>
+        <v>obj_0039a</v>
       </c>
       <c r="E31" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D31)</f>
@@ -7299,7 +7299,7 @@
       </c>
       <c r="F31" s="24">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.665E-2</v>
+        <v>2.589E-2</v>
       </c>
       <c r="G31" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -7307,14 +7307,14 @@
       </c>
       <c r="H31" s="23">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I31" s="22">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>49230</v>
+        <v>49233</v>
       </c>
       <c r="J31" s="24">
-        <v>2.7354101537435081E-2</v>
+        <v>2.6613989110438743E-2</v>
       </c>
       <c r="M31" s="73"/>
       <c r="N31" s="73"/>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="32" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D32" s="25" t="str">
-        <v>obj_003b1</v>
+        <v>obj_00373</v>
       </c>
       <c r="E32" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D32)</f>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="F32" s="24">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.7099999999999999E-2</v>
+        <v>2.6380000000000001E-2</v>
       </c>
       <c r="G32" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -7339,14 +7339,14 @@
       </c>
       <c r="H32" s="23">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I32" s="22">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>51056</v>
+        <v>51057</v>
       </c>
       <c r="J32" s="24">
-        <v>2.7794512069043518E-2</v>
+        <v>2.7103164054534262E-2</v>
       </c>
       <c r="M32" s="73"/>
       <c r="N32" s="73"/>
@@ -7355,7 +7355,7 @@
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D33" s="25" t="str">
-        <v>obj_0036f</v>
+        <v>obj_00366</v>
       </c>
       <c r="E33" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D33)</f>
@@ -7363,7 +7363,7 @@
       </c>
       <c r="F33" s="24">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.7309999999999997E-2</v>
+        <v>2.6619999999999998E-2</v>
       </c>
       <c r="G33" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -7371,14 +7371,14 @@
       </c>
       <c r="H33" s="23">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I33" s="22">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>52883</v>
+        <v>52884</v>
       </c>
       <c r="J33" s="24">
-        <v>2.795998665109669E-2</v>
+        <v>2.730723634639955E-2</v>
       </c>
       <c r="M33" s="73"/>
       <c r="N33" s="73"/>
@@ -7387,7 +7387,7 @@
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D34" s="25" t="str">
-        <v>obj_0039b</v>
+        <v>obj_003b3</v>
       </c>
       <c r="E34" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D34)</f>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="F34" s="24">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.7199999999999998E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
       <c r="G34" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -7403,14 +7403,14 @@
       </c>
       <c r="H34" s="23">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I34" s="22">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>56535</v>
+        <v>56536</v>
       </c>
       <c r="J34" s="24">
-        <v>2.7570241720796279E-2</v>
+        <v>2.6928367906774012E-2</v>
       </c>
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
@@ -7419,7 +7419,7 @@
     </row>
     <row r="35" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D35" s="25" t="str">
-        <v>obj_00382</v>
+        <v>obj_00395</v>
       </c>
       <c r="E35" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D35)</f>
@@ -7427,7 +7427,7 @@
       </c>
       <c r="F35" s="24">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.7199999999999998E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
       <c r="G35" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -7435,14 +7435,14 @@
       </c>
       <c r="H35" s="23">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I35" s="22">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>60188</v>
+        <v>60189</v>
       </c>
       <c r="J35" s="24">
-        <v>2.7458485495838431E-2</v>
+        <v>2.6810763694943215E-2</v>
       </c>
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="36" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D36" s="25" t="str">
-        <v>obj_00394</v>
+        <v>obj_00391</v>
       </c>
       <c r="E36" s="25" t="str">
         <f>_xll.qlRateHelperQuoteName(D36)</f>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="F36" s="24">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.733E-2</v>
+        <v>2.665E-2</v>
       </c>
       <c r="G36" s="24">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -7467,14 +7467,14 @@
       </c>
       <c r="H36" s="23">
         <f>_xll.qlRateHelperEarliestDate($D36)</f>
-        <v>41925</v>
+        <v>41926</v>
       </c>
       <c r="I36" s="22">
         <f>_xll.qlRateHelperLatestDate($D36)</f>
         <v>63842</v>
       </c>
       <c r="J36" s="24">
-        <v>2.7676292114762923E-2</v>
+        <v>2.7018896546611763E-2</v>
       </c>
       <c r="M36" s="73"/>
       <c r="N36" s="73"/>
@@ -10143,7 +10143,7 @@
       </c>
       <c r="J3" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I3,H3,Permanent,Trigger)</f>
-        <v>obj_0034a#0001</v>
+        <v>obj_00351#0001</v>
       </c>
       <c r="K3" s="83" t="str">
         <f>_xll.ohRangeRetrieveError(J3)</f>
@@ -10174,7 +10174,7 @@
       </c>
       <c r="H4" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00349#0001</v>
+        <v>obj_0034c#0001</v>
       </c>
       <c r="I4" s="80" t="str">
         <f>Currency&amp;$B4&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10222,7 +10222,7 @@
       </c>
       <c r="J5" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I5,H5,Permanent,Trigger)</f>
-        <v>obj_00358#0001</v>
+        <v>obj_0034f#0001</v>
       </c>
       <c r="K5" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J5)</f>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="H6" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00355#0001</v>
+        <v>obj_00350#0001</v>
       </c>
       <c r="I6" s="80" t="str">
         <f>Currency&amp;$B6&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10262,7 +10262,7 @@
       </c>
       <c r="J6" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I6,B6,C6,D6,E6,F6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035f#0001</v>
+        <v>obj_00361#0001</v>
       </c>
       <c r="K6" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J6)</f>
@@ -10302,7 +10302,7 @@
       </c>
       <c r="J7" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I7,B7,C7,D7,E7,F7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00362#0001</v>
+        <v>obj_0035f#0001</v>
       </c>
       <c r="K7" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J7)</f>
@@ -10342,7 +10342,7 @@
       </c>
       <c r="J8" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I8,H8,Permanent,Trigger)</f>
-        <v>obj_0034b#0001</v>
+        <v>obj_00352#0001</v>
       </c>
       <c r="K8" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J8)</f>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="J9" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I9,H9,Permanent,Trigger)</f>
-        <v>obj_00357#0001</v>
+        <v>obj_0034a#0001</v>
       </c>
       <c r="K9" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J9)</f>
@@ -10422,7 +10422,7 @@
       </c>
       <c r="J10" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I10,H10,Permanent,Trigger)</f>
-        <v>obj_00350#0001</v>
+        <v>obj_00359#0001</v>
       </c>
       <c r="K10" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J10)</f>
@@ -10454,7 +10454,7 @@
       </c>
       <c r="H11" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034d#0001</v>
+        <v>obj_0034b#0001</v>
       </c>
       <c r="I11" s="80" t="str">
         <f>Currency&amp;$B11&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10462,7 +10462,7 @@
       </c>
       <c r="J11" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I11,B11,C11,D11,E11,F11,G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035d#0001</v>
+        <v>obj_00362#0001</v>
       </c>
       <c r="K11" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J11)</f>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="H12" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034f#0001</v>
+        <v>obj_00353#0001</v>
       </c>
       <c r="I12" s="80" t="str">
         <f>Currency&amp;$B12&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="J12" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I12,B12,C12,D12,E12,F12,G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035e#0001</v>
+        <v>obj_0035d#0001</v>
       </c>
       <c r="K12" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J12)</f>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="J13" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I13,H13,Permanent,Trigger)</f>
-        <v>obj_00359#0001</v>
+        <v>obj_00357#0001</v>
       </c>
       <c r="K13" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J13)</f>
@@ -10574,7 +10574,7 @@
       </c>
       <c r="H14" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0034c#0001</v>
+        <v>obj_00358#0001</v>
       </c>
       <c r="I14" s="80" t="str">
         <f>Currency&amp;$B14&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10582,7 +10582,7 @@
       </c>
       <c r="J14" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I14,B14,C14,D14,E14,F14,G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00363#0001</v>
+        <v>obj_0035b#0001</v>
       </c>
       <c r="K14" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J14)</f>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="H15" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00352#0001</v>
+        <v>obj_00354#0001</v>
       </c>
       <c r="I15" s="80" t="str">
         <f>Currency&amp;$B15&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10622,7 +10622,7 @@
       </c>
       <c r="J15" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I15,B15,C15,D15,E15,F15,G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00361#0001</v>
+        <v>obj_00363#0001</v>
       </c>
       <c r="K15" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J15)</f>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="H17" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00351#0001</v>
+        <v>obj_0034d#0001</v>
       </c>
       <c r="I17" s="80" t="str">
         <f>Currency&amp;$B17&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="J17" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I17,B17,C17,D17,E17,F17,G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035b#0001</v>
+        <v>obj_0035c#0001</v>
       </c>
       <c r="K17" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J17)</f>
@@ -10734,7 +10734,7 @@
       </c>
       <c r="H18" s="84" t="str">
         <f>_xll.qlLibor(,Currency,B18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00354#0001</v>
+        <v>obj_00349#0001</v>
       </c>
       <c r="I18" s="80" t="str">
         <f>Currency&amp;$B18&amp;"D"&amp;"_Mx"&amp;QuoteSuffix</f>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="J18" s="79" t="str">
         <f>_xll.qlDepositRateHelper2(,I18,B18,C18,D18,E18,F18,G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0035c#0001</v>
+        <v>obj_0035e#0001</v>
       </c>
       <c r="K18" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J18)</f>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="J19" s="181" t="str">
         <f>_xll.qlDepositRateHelper(,I19,H19,Permanent,Trigger)</f>
-        <v>obj_00353#0001</v>
+        <v>obj_00355#0001</v>
       </c>
       <c r="K19" s="78" t="str">
         <f>_xll.ohRangeRetrieveError(J19)</f>
@@ -10795,7 +10795,7 @@
       <c r="A20" s="82"/>
       <c r="B20" s="81">
         <f>_xll.qlCalendarBusinessDaysBetween(Calendar,_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),C20&amp;"D",,,Trigger),D24,Trigger)-1</f>
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="84">
         <v>0</v>
@@ -10892,7 +10892,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10901,7 +10903,7 @@
     <col min="3" max="3" width="6" style="72" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="72" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="72" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.7109375" style="72" customWidth="1"/>
@@ -10984,8 +10986,8 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F3" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MV4_HST_CLOSE_Quote</v>
+        <f t="shared" ref="F3:F44" si="1">Currency&amp;"FUT"&amp;$E$1&amp;$D3&amp;QuoteSuffix</f>
+        <v>GBPFUT3MV4_Quote</v>
       </c>
       <c r="G3" s="193">
         <f>IFERROR(INDEX($N$3:$N$8,MATCH(D3,$M$3:$M$8,0))/100,0)</f>
@@ -10993,7 +10995,7 @@
       </c>
       <c r="H3" s="135" t="str">
         <f>_xll.qlFuturesRateHelper(,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00367#0002</v>
+        <v>obj_00382#0001</v>
       </c>
       <c r="I3" s="136" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -11030,16 +11032,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F4" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D4&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MX4_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MX4_Quote</v>
       </c>
       <c r="G4" s="193">
-        <f t="shared" ref="G4:G44" si="1">IFERROR(INDEX($N$3:$N$8,MATCH(D4,$M$3:$M$8,0))/100,0)</f>
+        <f t="shared" ref="G4:G44" si="2">IFERROR(INDEX($N$3:$N$8,MATCH(D4,$M$3:$M$8,0))/100,0)</f>
         <v>0</v>
       </c>
       <c r="H4" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a3#0004</v>
+        <v>obj_00386#0001</v>
       </c>
       <c r="I4" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -11076,16 +11078,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F5" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D5&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ4_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ4_Quote</v>
       </c>
       <c r="G5" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H5" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039e#0004</v>
+        <v>obj_0037f#0001</v>
       </c>
       <c r="I5" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -11118,16 +11120,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F6" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D6&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MF5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MF5_Quote</v>
       </c>
       <c r="G6" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H6" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00390#0004</v>
+        <v>obj_00389#0001</v>
       </c>
       <c r="I6" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -11160,16 +11162,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F7" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D7&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MG5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MG5_Quote</v>
       </c>
       <c r="G7" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a2#0004</v>
+        <v>obj_003a6#0001</v>
       </c>
       <c r="I7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -11202,16 +11204,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F8" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D8&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH5_Quote</v>
       </c>
       <c r="G8" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H8" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00392#0004</v>
+        <v>obj_003b1#0001</v>
       </c>
       <c r="I8" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -11244,16 +11246,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F9" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D9&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MJ5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MJ5_Quote</v>
       </c>
       <c r="G9" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H9" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00398#0004</v>
+        <v>obj_003a0#0001</v>
       </c>
       <c r="I9" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -11278,16 +11280,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F10" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D10&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MK5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MK5_Quote</v>
       </c>
       <c r="G10" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a8#0004</v>
+        <v>obj_0038a#0001</v>
       </c>
       <c r="I10" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -11312,16 +11314,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F11" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D11&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM5_Quote</v>
       </c>
       <c r="G11" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="H11" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038b#0004</v>
+        <v>obj_0036c#0001</v>
       </c>
       <c r="I11" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -11346,16 +11348,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F12" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D12&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MN5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MN5_Quote</v>
       </c>
       <c r="G12" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a5#0004</v>
+        <v>obj_00371#0001</v>
       </c>
       <c r="I12" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -11380,16 +11382,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F13" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D13&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MQ5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MQ5_Quote</v>
       </c>
       <c r="G13" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00386#0004</v>
+        <v>obj_00388#0001</v>
       </c>
       <c r="I13" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -11414,16 +11416,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F14" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D14&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU5_Quote</v>
       </c>
       <c r="G14" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="H14" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003ae#0004</v>
+        <v>obj_00397#0001</v>
       </c>
       <c r="I14" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H14)</f>
@@ -11448,16 +11450,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F15" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D15&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ5_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ5_Quote</v>
       </c>
       <c r="G15" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5999999999999989E-5</v>
       </c>
       <c r="H15" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00375#0004</v>
+        <v>obj_0037c#0001</v>
       </c>
       <c r="I15" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H15)</f>
@@ -11482,16 +11484,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F16" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D16&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH6_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH6_Quote</v>
       </c>
       <c r="G16" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3200000000000001E-4</v>
       </c>
       <c r="H16" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00370#0004</v>
+        <v>obj_003af#0001</v>
       </c>
       <c r="I16" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H16)</f>
@@ -11516,16 +11518,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F17" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D17&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM6_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM6_Quote</v>
       </c>
       <c r="G17" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.73E-4</v>
       </c>
       <c r="H17" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036d#0004</v>
+        <v>obj_00372#0001</v>
       </c>
       <c r="I17" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H17)</f>
@@ -11550,16 +11552,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F18" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D18&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU6_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU6_Quote</v>
       </c>
       <c r="G18" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.23E-4</v>
       </c>
       <c r="H18" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00391#0004</v>
+        <v>obj_003a8#0001</v>
       </c>
       <c r="I18" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H18)</f>
@@ -11584,16 +11586,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F19" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D19&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ6_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ6_Quote</v>
       </c>
       <c r="G19" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H19" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00365#0004</v>
+        <v>obj_00368#0001</v>
       </c>
       <c r="I19" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H19)</f>
@@ -11618,16 +11620,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F20" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D20&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH7_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH7_Quote</v>
       </c>
       <c r="G20" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H20" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b0#0004</v>
+        <v>obj_003a5#0001</v>
       </c>
       <c r="I20" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H20)</f>
@@ -11652,16 +11654,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F21" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D21&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM7_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM7_Quote</v>
       </c>
       <c r="G21" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H21" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b3#0004</v>
+        <v>obj_003a9#0001</v>
       </c>
       <c r="I21" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H21)</f>
@@ -11686,16 +11688,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F22" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D22&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU7_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU7_Quote</v>
       </c>
       <c r="G22" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H22" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037f#0004</v>
+        <v>obj_003a1#0001</v>
       </c>
       <c r="I22" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H22)</f>
@@ -11720,16 +11722,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F23" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D23&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ7_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ7_Quote</v>
       </c>
       <c r="G23" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H23" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0037e#0004</v>
+        <v>obj_003a2#0001</v>
       </c>
       <c r="I23" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H23)</f>
@@ -11754,16 +11756,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F24" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D24&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH8_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH8_Quote</v>
       </c>
       <c r="G24" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H24" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00388#0004</v>
+        <v>obj_00367#0001</v>
       </c>
       <c r="I24" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H24)</f>
@@ -11788,16 +11790,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F25" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D25&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM8_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM8_Quote</v>
       </c>
       <c r="G25" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00380#0004</v>
+        <v>obj_00398#0001</v>
       </c>
       <c r="I25" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H25)</f>
@@ -11822,16 +11824,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F26" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D26&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU8_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU8_Quote</v>
       </c>
       <c r="G26" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H26" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039f#0004</v>
+        <v>obj_003ae#0001</v>
       </c>
       <c r="I26" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H26)</f>
@@ -11856,16 +11858,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F27" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D27&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ8_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ8_Quote</v>
       </c>
       <c r="G27" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00374#0004</v>
+        <v>obj_0038e#0001</v>
       </c>
       <c r="I27" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H27)</f>
@@ -11890,16 +11892,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F28" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D28&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH9_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH9_Quote</v>
       </c>
       <c r="G28" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H28" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003aa#0004</v>
+        <v>obj_00376#0001</v>
       </c>
       <c r="I28" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H28)</f>
@@ -11924,16 +11926,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F29" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D29&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM9_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM9_Quote</v>
       </c>
       <c r="G29" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H29" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a1#0004</v>
+        <v>obj_00396#0001</v>
       </c>
       <c r="I29" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H29)</f>
@@ -11958,16 +11960,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F30" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D30&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU9_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU9_Quote</v>
       </c>
       <c r="G30" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H30" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00383#0004</v>
+        <v>obj_0038b#0001</v>
       </c>
       <c r="I30" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H30)</f>
@@ -11992,16 +11994,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F31" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D31&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ9_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ9_Quote</v>
       </c>
       <c r="G31" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H31" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00384#0004</v>
+        <v>obj_0036f#0001</v>
       </c>
       <c r="I31" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H31)</f>
@@ -12026,16 +12028,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F32" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D32&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH0_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH0_Quote</v>
       </c>
       <c r="G32" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H32" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00377#0004</v>
+        <v>obj_00374#0001</v>
       </c>
       <c r="I32" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H32)</f>
@@ -12060,16 +12062,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F33" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D33&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM0_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM0_Quote</v>
       </c>
       <c r="G33" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H33" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00368#0004</v>
+        <v>obj_00394#0001</v>
       </c>
       <c r="I33" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H33)</f>
@@ -12094,16 +12096,16 @@
         <v>GbpLibor3M</v>
       </c>
       <c r="F34" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D34&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU0_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU0_Quote</v>
       </c>
       <c r="G34" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H34" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0039a#0004</v>
+        <v>obj_003b2#0001</v>
       </c>
       <c r="I34" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H34)</f>
@@ -12124,20 +12126,20 @@
         <v>Z0</v>
       </c>
       <c r="E35" s="132" t="str">
-        <f t="shared" ref="E35:E44" si="2">PROPER(Currency)&amp;FamilyName&amp;$E$1</f>
+        <f t="shared" ref="E35:E44" si="3">PROPER(Currency)&amp;FamilyName&amp;$E$1</f>
         <v>GbpLibor3M</v>
       </c>
       <c r="F35" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D35&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ0_HST_CLOSE_Quote</v>
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ0_Quote</v>
       </c>
       <c r="G35" s="193">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H35" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036e#0004</v>
+        <v>obj_00390#0001</v>
       </c>
       <c r="I35" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H35)</f>
@@ -12158,20 +12160,20 @@
         <v>H1</v>
       </c>
       <c r="E36" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F36" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH1_Quote</v>
+      </c>
+      <c r="G36" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F36" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D36&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH1_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G36" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H36" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00379#0004</v>
+        <v>obj_0036d#0001</v>
       </c>
       <c r="I36" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H36)</f>
@@ -12192,20 +12194,20 @@
         <v>M1</v>
       </c>
       <c r="E37" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F37" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM1_Quote</v>
+      </c>
+      <c r="G37" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F37" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D37&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM1_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G37" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H37" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a9#0004</v>
+        <v>obj_00369#0001</v>
       </c>
       <c r="I37" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H37)</f>
@@ -12226,20 +12228,20 @@
         <v>U1</v>
       </c>
       <c r="E38" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F38" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU1_Quote</v>
+      </c>
+      <c r="G38" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F38" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D38&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU1_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G38" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H38" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0038e#0004</v>
+        <v>obj_0036b#0001</v>
       </c>
       <c r="I38" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H38)</f>
@@ -12260,20 +12262,20 @@
         <v>Z1</v>
       </c>
       <c r="E39" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F39" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ1_Quote</v>
+      </c>
+      <c r="G39" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F39" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D39&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ1_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G39" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H39" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0036b#0004</v>
+        <v>obj_00393#0001</v>
       </c>
       <c r="I39" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H39)</f>
@@ -12294,20 +12296,20 @@
         <v>H2</v>
       </c>
       <c r="E40" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F40" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH2_Quote</v>
+      </c>
+      <c r="G40" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F40" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D40&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH2_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G40" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003a6#0004</v>
+        <v>obj_00399#0001</v>
       </c>
       <c r="I40" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H40)</f>
@@ -12328,20 +12330,20 @@
         <v>M2</v>
       </c>
       <c r="E41" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F41" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MM2_Quote</v>
+      </c>
+      <c r="G41" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F41" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D41&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MM2_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G41" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00381#0004</v>
+        <v>obj_00377#0001</v>
       </c>
       <c r="I41" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H41)</f>
@@ -12363,20 +12365,20 @@
         <v>U2</v>
       </c>
       <c r="E42" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F42" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MU2_Quote</v>
+      </c>
+      <c r="G42" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F42" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D42&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MU2_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G42" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003ab#0004</v>
+        <v>obj_003ad#0001</v>
       </c>
       <c r="I42" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H42)</f>
@@ -12397,20 +12399,20 @@
         <v>Z2</v>
       </c>
       <c r="E43" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F43" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MZ2_Quote</v>
+      </c>
+      <c r="G43" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F43" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D43&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MZ2_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G43" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00399#0004</v>
+        <v>obj_00383#0001</v>
       </c>
       <c r="I43" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H43)</f>
@@ -12431,20 +12433,20 @@
         <v>H3</v>
       </c>
       <c r="E44" s="132" t="str">
+        <f t="shared" si="3"/>
+        <v>GbpLibor3M</v>
+      </c>
+      <c r="F44" s="134" t="str">
+        <f t="shared" si="1"/>
+        <v>GBPFUT3MH3_Quote</v>
+      </c>
+      <c r="G44" s="193">
         <f t="shared" si="2"/>
-        <v>GbpLibor3M</v>
-      </c>
-      <c r="F44" s="134" t="str">
-        <f>Currency&amp;"FUT"&amp;$E$1&amp;$D44&amp;"_HST_CLOSE"&amp;QuoteSuffix</f>
-        <v>GBPFUT3MH3_HST_CLOSE_Quote</v>
-      </c>
-      <c r="G44" s="193">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44" s="140" t="str">
         <f>_xll.qlFuturesRateHelper(,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_003b2#0004</v>
+        <v>obj_0036a#0001</v>
       </c>
       <c r="I44" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H44)</f>
@@ -12643,7 +12645,7 @@
       </c>
       <c r="K6" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$4,$I6,B6,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038c#0001</v>
+        <v>obj_00380#0001</v>
       </c>
       <c r="L6" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -12690,7 +12692,7 @@
       </c>
       <c r="K7" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$4,$I7,B7,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00369#0001</v>
+        <v>obj_0039e#0001</v>
       </c>
       <c r="L7" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -12792,7 +12794,7 @@
       </c>
       <c r="K9" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$4,$I9,B9,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00389#0001</v>
+        <v>obj_0037e#0001</v>
       </c>
       <c r="L9" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -12839,7 +12841,7 @@
       </c>
       <c r="K10" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$4,$I10,B10,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00397#0001</v>
+        <v>obj_00384#0001</v>
       </c>
       <c r="L10" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -12890,7 +12892,7 @@
       </c>
       <c r="K11" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$4,$I11,B11,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00372#0001</v>
+        <v>obj_00381#0001</v>
       </c>
       <c r="L11" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -12932,7 +12934,7 @@
       </c>
       <c r="K12" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$4,$I12,B12,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a4#0001</v>
+        <v>obj_0039b#0001</v>
       </c>
       <c r="L12" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -12974,7 +12976,7 @@
       </c>
       <c r="K13" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$4,$I13,B13,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00396#0001</v>
+        <v>obj_00378#0001</v>
       </c>
       <c r="L13" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -13016,7 +13018,7 @@
       </c>
       <c r="K14" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$4,$I14,B14,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00373#0001</v>
+        <v>obj_0038d#0001</v>
       </c>
       <c r="L14" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -13058,7 +13060,7 @@
       </c>
       <c r="K15" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$4,$I15,B15,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a0#0001</v>
+        <v>obj_0038f#0001</v>
       </c>
       <c r="L15" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K15)</f>
@@ -13100,7 +13102,7 @@
       </c>
       <c r="K16" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$4,$I16,B16,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003a7#0001</v>
+        <v>obj_0038c#0001</v>
       </c>
       <c r="L16" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K16)</f>
@@ -13142,7 +13144,7 @@
       </c>
       <c r="K17" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$4,$I17,B17,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ac#0001</v>
+        <v>obj_003a7#0001</v>
       </c>
       <c r="L17" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K17)</f>
@@ -13184,7 +13186,7 @@
       </c>
       <c r="K18" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$4,$I18,B18,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037b#0001</v>
+        <v>obj_003b0#0001</v>
       </c>
       <c r="L18" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K18)</f>
@@ -13226,7 +13228,7 @@
       </c>
       <c r="K19" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$4,$I19,B19,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039d#0001</v>
+        <v>obj_003a4#0001</v>
       </c>
       <c r="L19" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K19)</f>
@@ -13268,7 +13270,7 @@
       </c>
       <c r="K20" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$4,$I20,B20,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037d#0001</v>
+        <v>obj_003ab#0001</v>
       </c>
       <c r="L20" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K20)</f>
@@ -13310,7 +13312,7 @@
       </c>
       <c r="K21" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$4,$I21,B21,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00395#0001</v>
+        <v>obj_0039d#0001</v>
       </c>
       <c r="L21" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K21)</f>
@@ -13352,7 +13354,7 @@
       </c>
       <c r="K22" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$4,$I22,B22,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037a#0001</v>
+        <v>obj_00392#0001</v>
       </c>
       <c r="L22" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K22)</f>
@@ -13394,7 +13396,7 @@
       </c>
       <c r="K23" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$4,$I23,B23,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00366#0001</v>
+        <v>obj_0037d#0001</v>
       </c>
       <c r="L23" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K23)</f>
@@ -13436,7 +13438,7 @@
       </c>
       <c r="K24" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$4,$I24,B24,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0037c#0001</v>
+        <v>obj_00365#0001</v>
       </c>
       <c r="L24" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K24)</f>
@@ -13478,7 +13480,7 @@
       </c>
       <c r="K25" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$4,$I25,B25,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00387#0001</v>
+        <v>obj_00370#0001</v>
       </c>
       <c r="L25" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K25)</f>
@@ -13520,7 +13522,7 @@
       </c>
       <c r="K26" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$4,$I26,B26,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00371#0001</v>
+        <v>obj_0039f#0001</v>
       </c>
       <c r="L26" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K26)</f>
@@ -13562,7 +13564,7 @@
       </c>
       <c r="K27" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$4,$I27,B27,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003af#0001</v>
+        <v>obj_0036e#0001</v>
       </c>
       <c r="L27" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K27)</f>
@@ -13604,7 +13606,7 @@
       </c>
       <c r="K28" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$4,$I28,B28,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036c#0001</v>
+        <v>obj_0039a#0001</v>
       </c>
       <c r="L28" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K28)</f>
@@ -13646,7 +13648,7 @@
       </c>
       <c r="K29" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J29,$C29,Calendar,$F29,$G29,$H29,$K$4,$I29,B29,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00393#0001</v>
+        <v>obj_0039c#0001</v>
       </c>
       <c r="L29" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K29)</f>
@@ -13688,7 +13690,7 @@
       </c>
       <c r="K30" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J30,$C30,Calendar,$F30,$G30,$H30,$K$4,$I30,B30,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003ad#0001</v>
+        <v>obj_00375#0001</v>
       </c>
       <c r="L30" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K30)</f>
@@ -13730,7 +13732,7 @@
       </c>
       <c r="K31" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J31,$C31,Calendar,$F31,$G31,$H31,$K$4,$I31,B31,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00376#0001</v>
+        <v>obj_003ac#0001</v>
       </c>
       <c r="L31" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K31)</f>
@@ -13772,7 +13774,7 @@
       </c>
       <c r="K32" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J32,$C32,Calendar,$F32,$G32,$H32,$K$4,$I32,B32,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038f#0001</v>
+        <v>obj_003aa#0001</v>
       </c>
       <c r="L32" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K32)</f>
@@ -13814,7 +13816,7 @@
       </c>
       <c r="K33" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J33,$C33,Calendar,$F33,$G33,$H33,$K$4,$I33,B33,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_003b1#0001</v>
+        <v>obj_00373#0001</v>
       </c>
       <c r="L33" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K33)</f>
@@ -13856,7 +13858,7 @@
       </c>
       <c r="K34" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J34,$C34,Calendar,$F34,$G34,$H34,$K$4,$I34,B34,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00378#0001</v>
+        <v>obj_003a3#0001</v>
       </c>
       <c r="L34" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K34)</f>
@@ -13898,7 +13900,7 @@
       </c>
       <c r="K35" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J35,$C35,Calendar,$F35,$G35,$H35,$K$4,$I35,B35,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038a#0001</v>
+        <v>obj_00379#0001</v>
       </c>
       <c r="L35" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K35)</f>
@@ -13940,7 +13942,7 @@
       </c>
       <c r="K36" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J36,$C36,Calendar,$F36,$G36,$H36,$K$4,$I36,B36,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036a#0001</v>
+        <v>obj_0037b#0001</v>
       </c>
       <c r="L36" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K36)</f>
@@ -13982,7 +13984,7 @@
       </c>
       <c r="K37" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J37,$C37,Calendar,$F37,$G37,$H37,$K$4,$I37,B37,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0038d#0001</v>
+        <v>obj_00387#0001</v>
       </c>
       <c r="L37" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K37)</f>
@@ -14024,7 +14026,7 @@
       </c>
       <c r="K38" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J38,$C38,Calendar,$F38,$G38,$H38,$K$4,$I38,B38,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0036f#0001</v>
+        <v>obj_00366#0001</v>
       </c>
       <c r="L38" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K38)</f>
@@ -14066,7 +14068,7 @@
       </c>
       <c r="K39" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J39,$C39,Calendar,$F39,$G39,$H39,$K$4,$I39,B39,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039c#0001</v>
+        <v>obj_0037a#0001</v>
       </c>
       <c r="L39" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K39)</f>
@@ -14108,7 +14110,7 @@
       </c>
       <c r="K40" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J40,$C40,Calendar,$F40,$G40,$H40,$K$4,$I40,B40,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0039b#0001</v>
+        <v>obj_003b3#0001</v>
       </c>
       <c r="L40" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K40)</f>
@@ -14150,7 +14152,7 @@
       </c>
       <c r="K41" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J41,$C41,Calendar,$F41,$G41,$H41,$K$4,$I41,B41,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00382#0001</v>
+        <v>obj_00395#0001</v>
       </c>
       <c r="L41" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K41)</f>
@@ -14192,7 +14194,7 @@
       </c>
       <c r="K42" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(,$J42,$C42,Calendar,$F42,$G42,$H42,$K$4,$I42,B42,,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00394#0001</v>
+        <v>obj_00391#0001</v>
       </c>
       <c r="L42" s="157" t="str">
         <f>_xll.ohRangeRetrieveError(K42)</f>

</xml_diff>